<commit_message>
Rule: Mead Exclusive Flood Control Space - edit
This rule was being used to set Mead outflow in conditions where Mead was almost empty. Edited execution constraints to look if Flood Control Flag is equal to 1, not NaN.
</commit_message>
<xml_diff>
--- a/Input Data/DevTesting/DevTesting_InflowsTEST.xlsx
+++ b/Input Data/DevTesting/DevTesting_InflowsTEST.xlsx
@@ -383,7 +383,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B2" sqref="B2:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -416,7 +416,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>11.829420000000001</v>
+        <v>19.441980000000001</v>
       </c>
       <c r="C2">
         <v>29.924630000000001</v>
@@ -439,7 +439,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>10.65719</v>
+        <v>13.76132</v>
       </c>
       <c r="C3">
         <v>17.456529999999997</v>
@@ -462,7 +462,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>11.68661</v>
+        <v>13.449920000000001</v>
       </c>
       <c r="C4">
         <v>15.51074</v>
@@ -485,7 +485,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>10.962639999999999</v>
+        <v>12.900499999999999</v>
       </c>
       <c r="C5">
         <v>13.77521</v>
@@ -508,7 +508,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>8.5745450000000005</v>
+        <v>13.215870000000001</v>
       </c>
       <c r="C6">
         <v>13.44595</v>
@@ -531,7 +531,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>8.4952070000000006</v>
+        <v>36.56926</v>
       </c>
       <c r="C7">
         <v>21.274709999999999</v>
@@ -554,7 +554,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>19.130580000000002</v>
+        <v>76.125619999999998</v>
       </c>
       <c r="C8">
         <v>38.318680000000001</v>
@@ -577,7 +577,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>33.441319999999997</v>
+        <v>104.5686</v>
       </c>
       <c r="C9">
         <v>142.84960000000001</v>
@@ -600,7 +600,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>21.27074</v>
+        <v>75.929259999999999</v>
       </c>
       <c r="C10">
         <v>241.46779999999998</v>
@@ -623,7 +623,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>9.4730580000000018</v>
+        <v>34.538179999999997</v>
       </c>
       <c r="C11">
         <v>139.16029999999998</v>
@@ -646,7 +646,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>8.2254550000000002</v>
+        <v>30.251900000000003</v>
       </c>
       <c r="C12">
         <v>56.11835</v>
@@ -669,7 +669,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>18.839009999999998</v>
+        <v>13.16033</v>
       </c>
       <c r="C13">
         <v>22.746449999999999</v>
@@ -692,7 +692,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>11.829420000000001</v>
+        <v>15.98479</v>
       </c>
       <c r="C14">
         <v>27.465119999999999</v>
@@ -715,7 +715,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>10.65719</v>
+        <v>10.61157</v>
       </c>
       <c r="C15">
         <v>15.675370000000001</v>
@@ -738,7 +738,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>11.68661</v>
+        <v>7.9517359999999995</v>
       </c>
       <c r="C16">
         <v>17.018180000000001</v>
@@ -761,7 +761,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>10.962639999999999</v>
+        <v>7.5173549999999993</v>
       </c>
       <c r="C17">
         <v>15.21917</v>
@@ -784,7 +784,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>8.5745450000000005</v>
+        <v>7.4836360000000006</v>
       </c>
       <c r="C18">
         <v>15.18942</v>
@@ -807,7 +807,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>8.4952070000000006</v>
+        <v>8.2076029999999989</v>
       </c>
       <c r="C19">
         <v>22.08</v>
@@ -830,7 +830,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>19.130580000000002</v>
+        <v>21.365950000000002</v>
       </c>
       <c r="C20">
         <v>46.151400000000002</v>
@@ -853,7 +853,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>33.441319999999997</v>
+        <v>93.10611999999999</v>
       </c>
       <c r="C21">
         <v>229.4281</v>
@@ -876,7 +876,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>21.27074</v>
+        <v>130.05019999999999</v>
       </c>
       <c r="C22">
         <v>176.8066</v>
@@ -899,7 +899,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>9.4730580000000018</v>
+        <v>44.526940000000003</v>
       </c>
       <c r="C23">
         <v>103.69589999999999</v>
@@ -922,7 +922,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>8.2254550000000002</v>
+        <v>24.902480000000001</v>
       </c>
       <c r="C24">
         <v>62.717359999999999</v>
@@ -945,7 +945,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>18.839009999999998</v>
+        <v>25.378509999999999</v>
       </c>
       <c r="C25">
         <v>35.688600000000001</v>
@@ -968,7 +968,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>11.829420000000001</v>
+        <v>39.286910000000006</v>
       </c>
       <c r="C26">
         <v>36.099170000000001</v>
@@ -991,7 +991,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>10.65719</v>
+        <v>21.189060000000001</v>
       </c>
       <c r="C27">
         <v>21.459169999999997</v>
@@ -1014,7 +1014,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>11.68661</v>
+        <v>22.05152</v>
       </c>
       <c r="C28">
         <v>16.532229999999998</v>
@@ -1037,7 +1037,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>10.962639999999999</v>
+        <v>16.454060000000002</v>
       </c>
       <c r="C29">
         <v>15.30843</v>
@@ -1060,7 +1060,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>8.5745450000000005</v>
+        <v>12.43914</v>
       </c>
       <c r="C30">
         <v>12.440329999999999</v>
@@ -1083,7 +1083,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>8.4952070000000006</v>
+        <v>15.50592</v>
       </c>
       <c r="C31">
         <v>27.498840000000001</v>
@@ -1106,7 +1106,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>19.130580000000002</v>
+        <v>48.120040000000003</v>
       </c>
       <c r="C32">
         <v>108.2043</v>
@@ -1129,7 +1129,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>33.441319999999997</v>
+        <v>126.32539999999999</v>
       </c>
       <c r="C33">
         <v>195.5504</v>
@@ -1152,7 +1152,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>21.27074</v>
+        <v>125.53530000000001</v>
       </c>
       <c r="C34">
         <v>253.01160000000002</v>
@@ -1175,7 +1175,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>9.4730580000000018</v>
+        <v>44.607870000000005</v>
       </c>
       <c r="C35">
         <v>99.431399999999996</v>
@@ -1198,7 +1198,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>8.2254550000000002</v>
+        <v>24.032049999999998</v>
       </c>
       <c r="C36">
         <v>37.176199999999994</v>
@@ -1221,7 +1221,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>18.839009999999998</v>
+        <v>46.412550000000003</v>
       </c>
       <c r="C37">
         <v>42.928260000000002</v>
@@ -1249,7 +1249,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B2" sqref="B2:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1282,7 +1282,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>4.1928396689999996</v>
+        <v>4.5902854780700002</v>
       </c>
       <c r="C2">
         <v>8.2923371899999996</v>
@@ -1305,7 +1305,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>3.5082644630000002</v>
+        <v>5.8111237864799996</v>
       </c>
       <c r="C3">
         <v>6.2157421489999996</v>
@@ -1328,7 +1328,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>3.152330579</v>
+        <v>2.1699001854500004</v>
       </c>
       <c r="C4">
         <v>5.1372892559999999</v>
@@ -1351,7 +1351,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>2.6214148759999998</v>
+        <v>2.76610243994</v>
       </c>
       <c r="C5">
         <v>4.5278082639999999</v>
@@ -1374,7 +1374,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>4.4010842979999998</v>
+        <v>3.3411156255500001</v>
       </c>
       <c r="C6">
         <v>3.9161057850000001</v>
@@ -1397,7 +1397,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>9.232343801999999</v>
+        <v>4.1484537600699998</v>
       </c>
       <c r="C7">
         <v>5.0694743799999999</v>
@@ -1420,7 +1420,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>13.278069421</v>
+        <v>12.5513977934</v>
       </c>
       <c r="C8">
         <v>4.7846876030000001</v>
@@ -1443,7 +1443,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>8.1911008259999996</v>
+        <v>25.636687612000003</v>
       </c>
       <c r="C9">
         <v>17.916158677999999</v>
@@ -1466,7 +1466,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>3.8432528929999998</v>
+        <v>12.923275837499999</v>
       </c>
       <c r="C10">
         <v>54.605494215</v>
@@ -1489,7 +1489,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>2.619768595</v>
+        <v>8.9502678131899991</v>
       </c>
       <c r="C11">
         <v>33.199219835000001</v>
@@ -1512,7 +1512,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>2.899160331</v>
+        <v>5.2194004279500001</v>
       </c>
       <c r="C12">
         <v>15.906981818</v>
@@ -1535,7 +1535,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>3.7647471070000003</v>
+        <v>4.4504380646000001</v>
       </c>
       <c r="C13">
         <v>7.6451504130000005</v>
@@ -1558,7 +1558,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>4.1928396689999996</v>
+        <v>3.9161435394000002</v>
       </c>
       <c r="C14">
         <v>7.6850578509999998</v>
@@ -1581,7 +1581,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>3.5082644630000002</v>
+        <v>3.1131471405000002</v>
       </c>
       <c r="C15">
         <v>6.6010512399999994</v>
@@ -1604,7 +1604,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>3.152330579</v>
+        <v>3.6258501891999999</v>
       </c>
       <c r="C16">
         <v>7.0984462810000002</v>
@@ -1627,7 +1627,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>2.6214148759999998</v>
+        <v>3.1648001709</v>
       </c>
       <c r="C17">
         <v>5.4367338840000006</v>
@@ -1650,7 +1650,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>4.4010842979999998</v>
+        <v>3.1958501891999997</v>
       </c>
       <c r="C18">
         <v>3.631775207</v>
@@ -1673,7 +1673,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>9.232343801999999</v>
+        <v>7.4521337433000001</v>
       </c>
       <c r="C19">
         <v>3.352264463</v>
@@ -1696,7 +1696,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>13.278069421</v>
+        <v>15.8195762024</v>
       </c>
       <c r="C20">
         <v>5.7545057850000001</v>
@@ -1719,7 +1719,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>8.1911008259999996</v>
+        <v>38.8314094849</v>
       </c>
       <c r="C21">
         <v>47.944383471000002</v>
@@ -1742,7 +1742,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>3.8432528929999998</v>
+        <v>12.5039044495</v>
       </c>
       <c r="C22">
         <v>71.879087603000002</v>
@@ -1765,7 +1765,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>2.619768595</v>
+        <v>5.5609594727000005</v>
       </c>
       <c r="C23">
         <v>42.633282645000001</v>
@@ -1788,7 +1788,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>2.899160331</v>
+        <v>4.3801983469999994</v>
       </c>
       <c r="C24">
         <v>20.371557024999998</v>
@@ -1811,7 +1811,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>3.7647471070000003</v>
+        <v>6.3203186188</v>
       </c>
       <c r="C25">
         <v>11.676952066</v>
@@ -1834,7 +1834,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>4.1928396689999996</v>
+        <v>5.0160610961999996</v>
       </c>
       <c r="C26">
         <v>10.936978512</v>
@@ -1857,7 +1857,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>3.5082644630000002</v>
+        <v>3.8878501891999999</v>
       </c>
       <c r="C27">
         <v>7.32</v>
@@ -1880,7 +1880,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>3.152330579</v>
+        <v>3.9968501891999999</v>
       </c>
       <c r="C28">
         <v>6.1669289259999998</v>
@@ -1903,7 +1903,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>2.6214148759999998</v>
+        <v>3.2408001709000001</v>
       </c>
       <c r="C29">
         <v>5.4657322309999996</v>
@@ -1926,7 +1926,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>4.4010842979999998</v>
+        <v>3.8808501891999998</v>
       </c>
       <c r="C30">
         <v>4.7108826449999999</v>
@@ -1949,7 +1949,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>9.232343801999999</v>
+        <v>7.3539051970999996</v>
       </c>
       <c r="C31">
         <v>6.0535933880000004</v>
@@ -1972,7 +1972,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>13.278069421</v>
+        <v>25.400750488300002</v>
       </c>
       <c r="C32">
         <v>10.271464463000001</v>
@@ -1995,7 +1995,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>8.1911008259999996</v>
+        <v>41.525772460900001</v>
       </c>
       <c r="C33">
         <v>40.584198346999997</v>
@@ -2018,7 +2018,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>3.8432528929999998</v>
+        <v>16.1900247803</v>
       </c>
       <c r="C34">
         <v>58.168085949999998</v>
@@ -2041,7 +2041,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>2.619768595</v>
+        <v>7.7384530944999996</v>
       </c>
       <c r="C35">
         <v>23.878968595</v>
@@ -2064,7 +2064,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>2.899160331</v>
+        <v>5.9147315062999999</v>
       </c>
       <c r="C36">
         <v>10.269421488000001</v>
@@ -2087,7 +2087,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>3.7647471070000003</v>
+        <v>3.9043111115000002</v>
       </c>
       <c r="C37">
         <v>9.2335735540000012</v>
@@ -2115,7 +2115,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B2" sqref="B2:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2148,7 +2148,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>5.7843169999999997</v>
+        <v>11.8096</v>
       </c>
       <c r="C2">
         <v>19.320040000000002</v>
@@ -2171,7 +2171,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>4.9138710000000003</v>
+        <v>6.0536440000000002</v>
       </c>
       <c r="C3">
         <v>10.24516</v>
@@ -2194,7 +2194,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>4.7501549999999995</v>
+        <v>5.8738339999999996</v>
       </c>
       <c r="C4">
         <v>8.6558600000000006</v>
@@ -2217,7 +2217,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>3.7661750000000001</v>
+        <v>5.290241</v>
       </c>
       <c r="C5">
         <v>0.37124020000000002</v>
@@ -2240,7 +2240,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>2.5588359999999999</v>
+        <v>5.292859</v>
       </c>
       <c r="C6">
         <v>5.1253289999999998</v>
@@ -2263,7 +2263,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>3.0275700000000003</v>
+        <v>13.29707</v>
       </c>
       <c r="C7">
         <v>8.0487269999999995</v>
@@ -2286,7 +2286,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>9.7743269999999995</v>
+        <v>41.68826</v>
       </c>
       <c r="C8">
         <v>11.393450000000001</v>
@@ -2309,7 +2309,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>15.625389999999999</v>
+        <v>58.142389999999999</v>
       </c>
       <c r="C9">
         <v>58.473639999999996</v>
@@ -2332,7 +2332,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>7.344436</v>
+        <v>34.141260000000003</v>
       </c>
       <c r="C10">
         <v>112.2482</v>
@@ -2355,7 +2355,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>3.6237020000000002</v>
+        <v>14.47199</v>
       </c>
       <c r="C11">
         <v>47.462800000000001</v>
@@ -2378,7 +2378,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>3.3712460000000002</v>
+        <v>13.93252</v>
       </c>
       <c r="C12">
         <v>23.439990000000002</v>
@@ -2401,7 +2401,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>9.9227310000000006</v>
+        <v>6.2529489999999992</v>
       </c>
       <c r="C13">
         <v>11.152419999999999</v>
@@ -2424,7 +2424,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>5.7843169999999997</v>
+        <v>8.9992859999999997</v>
       </c>
       <c r="C14">
         <v>18.693860000000001</v>
@@ -2447,7 +2447,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>4.9138710000000003</v>
+        <v>3.9251499999999999</v>
       </c>
       <c r="C15">
         <v>7.3858509999999997</v>
@@ -2470,7 +2470,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>4.7501549999999995</v>
+        <v>2.6607270000000001</v>
       </c>
       <c r="C16">
         <v>7.3714120000000003</v>
@@ -2493,7 +2493,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>3.7661750000000001</v>
+        <v>2.772456</v>
       </c>
       <c r="C17">
         <v>6.1968399999999999</v>
@@ -2516,7 +2516,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>2.5588359999999999</v>
+        <v>2.4570250000000002</v>
       </c>
       <c r="C18">
         <v>5.32925</v>
@@ -2539,7 +2539,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>3.0275700000000003</v>
+        <v>4.1965290000000008</v>
       </c>
       <c r="C19">
         <v>7.4334150000000001</v>
@@ -2562,7 +2562,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>9.7743269999999995</v>
+        <v>15.09423</v>
       </c>
       <c r="C20">
         <v>18.190549999999998</v>
@@ -2585,7 +2585,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>15.625389999999999</v>
+        <v>53.299800000000005</v>
       </c>
       <c r="C21">
         <v>100.81010000000001</v>
@@ -2608,7 +2608,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>7.344436</v>
+        <v>73.172169999999994</v>
       </c>
       <c r="C22">
         <v>71.207369999999997</v>
@@ -2631,7 +2631,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>3.6237020000000002</v>
+        <v>23.922999999999998</v>
       </c>
       <c r="C23">
         <v>35.676180000000002</v>
@@ -2654,7 +2654,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>3.3712460000000002</v>
+        <v>13.41836</v>
       </c>
       <c r="C24">
         <v>24.032250000000001</v>
@@ -2677,7 +2677,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>9.9227310000000006</v>
+        <v>17.082129999999999</v>
       </c>
       <c r="C25">
         <v>19.543779999999998</v>
@@ -2700,7 +2700,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>5.7843169999999997</v>
+        <v>21.42878</v>
       </c>
       <c r="C26">
         <v>23.183759999999999</v>
@@ -2723,7 +2723,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>4.9138710000000003</v>
+        <v>12.464549999999999</v>
       </c>
       <c r="C27">
         <v>11.256540000000001</v>
@@ -2746,7 +2746,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>4.7501549999999995</v>
+        <v>7.168927</v>
       </c>
       <c r="C28">
         <v>9.0916960000000007</v>
@@ -2769,7 +2769,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>3.7661750000000001</v>
+        <v>5.6124170000000007</v>
       </c>
       <c r="C29">
         <v>6.0569649999999999</v>
@@ -2792,7 +2792,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>2.5588359999999999</v>
+        <v>3.9631619999999996</v>
       </c>
       <c r="C30">
         <v>5.3950610000000001</v>
@@ -2815,7 +2815,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>3.0275700000000003</v>
+        <v>6.0090050000000002</v>
       </c>
       <c r="C31">
         <v>8.6311929999999997</v>
@@ -2838,7 +2838,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>9.7743269999999995</v>
+        <v>22.758610000000001</v>
       </c>
       <c r="C32">
         <v>40.939120000000003</v>
@@ -2861,7 +2861,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>15.625389999999999</v>
+        <v>65.197479999999999</v>
       </c>
       <c r="C33">
         <v>96.956450000000004</v>
@@ -2884,7 +2884,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>7.344436</v>
+        <v>50.733220000000003</v>
       </c>
       <c r="C34">
         <v>127.67960000000001</v>
@@ -2907,7 +2907,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>3.6237020000000002</v>
+        <v>14.986120000000001</v>
       </c>
       <c r="C35">
         <v>44.021080000000005</v>
@@ -2930,7 +2930,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>3.3712460000000002</v>
+        <v>10.19256</v>
       </c>
       <c r="C36">
         <v>17.965790000000002</v>
@@ -2953,7 +2953,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>9.9227310000000006</v>
+        <v>31.6144</v>
       </c>
       <c r="C37">
         <v>25.509799999999998</v>
@@ -2981,7 +2981,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B2" sqref="B2:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3014,7 +3014,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>13.610580000000001</v>
+        <v>17.2234767594</v>
       </c>
       <c r="C2">
         <v>56.132227000000007</v>
@@ -3037,7 +3037,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>22.792069999999999</v>
+        <v>17.963411431800001</v>
       </c>
       <c r="C3">
         <v>45.659489999999998</v>
@@ -3060,7 +3060,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>19.989419999999999</v>
+        <v>22.847759661000005</v>
       </c>
       <c r="C4">
         <v>31.687921000000003</v>
@@ -3083,7 +3083,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>18.973880000000001</v>
+        <v>15.4679653765</v>
       </c>
       <c r="C5">
         <v>28.363636000000003</v>
@@ -3106,7 +3106,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>17.018180000000001</v>
+        <v>13.5012335226</v>
       </c>
       <c r="C6">
         <v>37.527279999999998</v>
@@ -3129,7 +3129,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>34.591740000000001</v>
+        <v>81.137289331899993</v>
       </c>
       <c r="C7">
         <v>113.553713</v>
@@ -3152,7 +3152,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>125.71239999999999</v>
+        <v>198.439085318</v>
       </c>
       <c r="C8">
         <v>157.41221999999999</v>
@@ -3175,7 +3175,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>150.12889999999999</v>
+        <v>275.11685217600001</v>
       </c>
       <c r="C9">
         <v>584.80663000000004</v>
@@ -3198,7 +3198,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>82.018509999999992</v>
+        <v>181.04769779900002</v>
       </c>
       <c r="C10">
         <v>916.16519999999991</v>
@@ -3221,7 +3221,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>2.1147770000000001</v>
+        <v>24.453508829100002</v>
       </c>
       <c r="C11">
         <v>362.142</v>
@@ -3244,7 +3244,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>1.3283309999999999</v>
+        <v>13.537740430400001</v>
       </c>
       <c r="C12">
         <v>85.918019000000001</v>
@@ -3267,7 +3267,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>2.7110079999999996</v>
+        <v>6.7797935554900004</v>
       </c>
       <c r="C13">
         <v>26.419836</v>
@@ -3290,7 +3290,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>13.610580000000001</v>
+        <v>8.1857855999999991</v>
       </c>
       <c r="C14">
         <v>54.017840999999997</v>
@@ -3313,7 +3313,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>22.792069999999999</v>
+        <v>11.26215</v>
       </c>
       <c r="C15">
         <v>45.000989999999994</v>
@@ -3336,7 +3336,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>19.989419999999999</v>
+        <v>14.5388419</v>
       </c>
       <c r="C16">
         <v>40.938848</v>
@@ -3359,7 +3359,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>18.973880000000001</v>
+        <v>14.915702700000001</v>
       </c>
       <c r="C17">
         <v>40.214873999999995</v>
@@ -3382,7 +3382,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>17.018180000000001</v>
+        <v>18.690249200000004</v>
       </c>
       <c r="C18">
         <v>35.900840000000002</v>
@@ -3405,7 +3405,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>34.591740000000001</v>
+        <v>78.291584999999998</v>
       </c>
       <c r="C19">
         <v>55.735551000000001</v>
@@ -3428,7 +3428,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>125.71239999999999</v>
+        <v>158.10248999999999</v>
       </c>
       <c r="C20">
         <v>284.82645000000002</v>
@@ -3451,7 +3451,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>150.12889999999999</v>
+        <v>191.84133000000003</v>
       </c>
       <c r="C21">
         <v>1127.1271400000001</v>
@@ -3474,7 +3474,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>82.018509999999992</v>
+        <v>299.64297000000005</v>
       </c>
       <c r="C22">
         <v>959.00819999999999</v>
@@ -3497,7 +3497,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>2.1147770000000001</v>
+        <v>43.709752000000002</v>
       </c>
       <c r="C23">
         <v>318.68433999999996</v>
@@ -3520,7 +3520,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>1.3283309999999999</v>
+        <v>7.7057847000000006</v>
       </c>
       <c r="C24">
         <v>94.476685000000018</v>
@@ -3543,7 +3543,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>2.7110079999999996</v>
+        <v>7.5272730000000001</v>
       </c>
       <c r="C25">
         <v>55.207920000000001</v>
@@ -3566,7 +3566,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>13.610580000000001</v>
+        <v>20.052892499999999</v>
       </c>
       <c r="C26">
         <v>66.23602600000001</v>
@@ -3589,7 +3589,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>22.792069999999999</v>
+        <v>21.506778000000001</v>
       </c>
       <c r="C27">
         <v>63.250920000000001</v>
@@ -3612,7 +3612,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>19.989419999999999</v>
+        <v>14.852230199999999</v>
       </c>
       <c r="C28">
         <v>51.153719999999993</v>
@@ -3635,7 +3635,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>18.973880000000001</v>
+        <v>14.899833799999998</v>
       </c>
       <c r="C29">
         <v>39.966936000000004</v>
@@ -3658,7 +3658,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>17.018180000000001</v>
+        <v>15.104132400000001</v>
       </c>
       <c r="C30">
         <v>38.142160000000004</v>
@@ -3681,7 +3681,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>34.591740000000001</v>
+        <v>52.595716000000003</v>
       </c>
       <c r="C31">
         <v>121.64629400000001</v>
@@ -3704,7 +3704,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>125.71239999999999</v>
+        <v>120.31737000000001</v>
       </c>
       <c r="C32">
         <v>488.58840000000004</v>
@@ -3727,7 +3727,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>150.12889999999999</v>
+        <v>365.13722000000001</v>
       </c>
       <c r="C33">
         <v>810.6447300000001</v>
@@ -3750,7 +3750,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>82.018509999999992</v>
+        <v>341.7321</v>
       </c>
       <c r="C34">
         <v>446.57850000000002</v>
@@ -3773,7 +3773,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>2.1147770000000001</v>
+        <v>52.573892000000001</v>
       </c>
       <c r="C35">
         <v>103.52924299999999</v>
@@ -3796,7 +3796,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>1.3283309999999999</v>
+        <v>25.7434726</v>
       </c>
       <c r="C36">
         <v>40.764287000000003</v>
@@ -3819,7 +3819,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>2.7110079999999996</v>
+        <v>19.317024</v>
       </c>
       <c r="C37">
         <v>21.352065</v>
@@ -3847,7 +3847,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B2" sqref="B2:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3880,7 +3880,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>26.933299999999999</v>
+        <v>25.65063</v>
       </c>
       <c r="C2">
         <v>52.643529999999998</v>
@@ -3903,7 +3903,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>27.565709999999999</v>
+        <v>25.848500000000001</v>
       </c>
       <c r="C3">
         <v>36.661449999999995</v>
@@ -3926,7 +3926,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>23.133759999999999</v>
+        <v>19.727689999999999</v>
       </c>
       <c r="C4">
         <v>27.399540000000002</v>
@@ -3949,7 +3949,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>21.598710000000001</v>
+        <v>23.681330000000003</v>
       </c>
       <c r="C5">
         <v>27.065459999999998</v>
@@ -3972,7 +3972,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>16.705490000000001</v>
+        <v>21.779769999999999</v>
       </c>
       <c r="C6">
         <v>23.79964</v>
@@ -3995,7 +3995,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>29.637840000000001</v>
+        <v>42.286139999999996</v>
       </c>
       <c r="C7">
         <v>31.192679999999999</v>
@@ -4018,7 +4018,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>53.477849999999997</v>
+        <v>97.546199999999999</v>
       </c>
       <c r="C8">
         <v>42.44979</v>
@@ -4041,7 +4041,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>53.1265</v>
+        <v>139.4675</v>
       </c>
       <c r="C9">
         <v>167.9264</v>
@@ -4064,7 +4064,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>36.121370000000006</v>
+        <v>145.73420000000002</v>
       </c>
       <c r="C10">
         <v>442.96320000000003</v>
@@ -4087,7 +4087,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>13.82577</v>
+        <v>59.89226</v>
       </c>
       <c r="C11">
         <v>238.18529999999998</v>
@@ -4110,7 +4110,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>9.5871069999999996</v>
+        <v>50.195550000000004</v>
       </c>
       <c r="C12">
         <v>113.9067</v>
@@ -4133,7 +4133,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>12.736979999999999</v>
+        <v>18.242060000000002</v>
       </c>
       <c r="C13">
         <v>41.228720000000003</v>
@@ -4156,7 +4156,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>26.933299999999999</v>
+        <v>25.446180000000002</v>
       </c>
       <c r="C14">
         <v>34.384010000000004</v>
@@ -4179,7 +4179,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>27.565709999999999</v>
+        <v>20.843250000000001</v>
       </c>
       <c r="C15">
         <v>31.637630000000001</v>
@@ -4202,7 +4202,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>23.133759999999999</v>
+        <v>17.206790000000002</v>
       </c>
       <c r="C16">
         <v>34.850529999999999</v>
@@ -4225,7 +4225,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>21.598710000000001</v>
+        <v>18.372479999999999</v>
       </c>
       <c r="C17">
         <v>29.029330000000002</v>
@@ -4248,7 +4248,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>16.705490000000001</v>
+        <v>15.768120000000001</v>
       </c>
       <c r="C18">
         <v>21.8188</v>
@@ -4271,7 +4271,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>29.637840000000001</v>
+        <v>24.624470000000002</v>
       </c>
       <c r="C19">
         <v>23.558810000000001</v>
@@ -4294,7 +4294,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>53.477849999999997</v>
+        <v>38.664230000000003</v>
       </c>
       <c r="C20">
         <v>74.140799999999999</v>
@@ -4317,7 +4317,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>53.1265</v>
+        <v>94.119309999999999</v>
       </c>
       <c r="C21">
         <v>569.19709999999998</v>
@@ -4340,7 +4340,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>36.121370000000006</v>
+        <v>181.04429999999999</v>
       </c>
       <c r="C22">
         <v>527.41669999999999</v>
@@ -4363,7 +4363,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>13.82577</v>
+        <v>68.314869999999999</v>
       </c>
       <c r="C23">
         <v>262.25380000000001</v>
@@ -4386,7 +4386,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>9.5871069999999996</v>
+        <v>38.767489999999995</v>
       </c>
       <c r="C24">
         <v>130.6918</v>
@@ -4409,7 +4409,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>12.736979999999999</v>
+        <v>25.374939999999999</v>
       </c>
       <c r="C25">
         <v>64.263419999999996</v>
@@ -4432,7 +4432,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>26.933299999999999</v>
+        <v>40.062609999999999</v>
       </c>
       <c r="C26">
         <v>57.819780000000002</v>
@@ -4455,7 +4455,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>27.565709999999999</v>
+        <v>36.532849999999996</v>
       </c>
       <c r="C27">
         <v>41.806339999999999</v>
@@ -4478,7 +4478,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>23.133759999999999</v>
+        <v>23.919130000000003</v>
       </c>
       <c r="C28">
         <v>34.39472</v>
@@ -4501,7 +4501,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>21.598710000000001</v>
+        <v>21.607330000000001</v>
       </c>
       <c r="C29">
         <v>29.158279999999998</v>
@@ -4524,7 +4524,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>16.705490000000001</v>
+        <v>19.958110000000001</v>
       </c>
       <c r="C30">
         <v>24.265139999999999</v>
@@ -4547,7 +4547,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>29.637840000000001</v>
+        <v>33.065460000000002</v>
       </c>
       <c r="C31">
         <v>39.716800000000006</v>
@@ -4570,7 +4570,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>53.477849999999997</v>
+        <v>71.596429999999998</v>
       </c>
       <c r="C32">
         <v>137.2192</v>
@@ -4593,7 +4593,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>53.1265</v>
+        <v>198.84229999999999</v>
       </c>
       <c r="C33">
         <v>351.79079999999999</v>
@@ -4616,7 +4616,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>36.121370000000006</v>
+        <v>233.51589999999999</v>
       </c>
       <c r="C34">
         <v>402.8288</v>
@@ -4639,7 +4639,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>13.82577</v>
+        <v>96.341719999999995</v>
       </c>
       <c r="C35">
         <v>148.87560000000002</v>
@@ -4662,7 +4662,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>9.5871069999999996</v>
+        <v>49.2697</v>
       </c>
       <c r="C36">
         <v>64.618809999999996</v>
@@ -4685,7 +4685,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>12.736979999999999</v>
+        <v>29.47878</v>
       </c>
       <c r="C37">
         <v>47.620190000000001</v>
@@ -4713,7 +4713,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B2" sqref="B2:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4746,7 +4746,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>32.110115700000001</v>
+        <v>39.394533629999998</v>
       </c>
       <c r="C2">
         <v>68.716436279999996</v>
@@ -4769,7 +4769,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>32.813494220000003</v>
+        <v>33.881778259999997</v>
       </c>
       <c r="C3">
         <v>43.518480710000006</v>
@@ -4792,7 +4792,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>29.418505789999998</v>
+        <v>27.669721450000001</v>
       </c>
       <c r="C4">
         <v>35.09828589</v>
@@ -4815,7 +4815,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>27.87798347</v>
+        <v>27.27724585</v>
       </c>
       <c r="C5">
         <v>34.04163672</v>
@@ -4838,7 +4838,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>23.495424790000001</v>
+        <v>25.65475696</v>
       </c>
       <c r="C6">
         <v>30.235136539999999</v>
@@ -4861,7 +4861,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>35.21547769</v>
+        <v>52.467886480000004</v>
       </c>
       <c r="C7">
         <v>41.592700440000002</v>
@@ -4884,7 +4884,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>71.951563639999989</v>
+        <v>123.1677864</v>
       </c>
       <c r="C8">
         <v>60.059090450000006</v>
@@ -4907,7 +4907,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>64.690413219999996</v>
+        <v>166.23262990000001</v>
       </c>
       <c r="C9">
         <v>249.09494649999999</v>
@@ -4930,7 +4930,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>43.138492559999996</v>
+        <v>162.82172750000001</v>
       </c>
       <c r="C10">
         <v>576.80068549999999</v>
@@ -4953,7 +4953,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>21.23258182</v>
+        <v>66.551131959999992</v>
       </c>
       <c r="C11">
         <v>297.2250659</v>
@@ -4976,7 +4976,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>13.801923970000001</v>
+        <v>58.545583860000001</v>
       </c>
       <c r="C12">
         <v>144.12701709999999</v>
@@ -4999,7 +4999,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>18.97560992</v>
+        <v>25.914385379999999</v>
       </c>
       <c r="C13">
         <v>52.694858399999994</v>
@@ -5022,7 +5022,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>32.110115700000001</v>
+        <v>36.869770629999998</v>
       </c>
       <c r="C14">
         <v>43.019139889999998</v>
@@ -5045,7 +5045,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>32.813494220000003</v>
+        <v>26.493841980000003</v>
       </c>
       <c r="C15">
         <v>42.015881960000002</v>
@@ -5068,7 +5068,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>29.418505789999998</v>
+        <v>22.3585213</v>
       </c>
       <c r="C16">
         <v>45.296903440000001</v>
@@ -5091,7 +5091,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>27.87798347</v>
+        <v>23.030349919999999</v>
       </c>
       <c r="C17">
         <v>39.872492800000003</v>
@@ -5114,7 +5114,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>23.495424790000001</v>
+        <v>20.91384274</v>
       </c>
       <c r="C18">
         <v>30.78035083</v>
@@ -5137,7 +5137,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>35.21547769</v>
+        <v>31.03302747</v>
       </c>
       <c r="C19">
         <v>42.671297120000006</v>
@@ -5160,7 +5160,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>71.951563639999989</v>
+        <v>50.721259519999997</v>
       </c>
       <c r="C20">
         <v>106.621708</v>
@@ -5183,7 +5183,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>64.690413219999996</v>
+        <v>113.5885339</v>
       </c>
       <c r="C21">
         <v>769.72709569999995</v>
@@ -5206,7 +5206,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>43.138492559999996</v>
+        <v>210.88209959999998</v>
       </c>
       <c r="C22">
         <v>662.80359279999993</v>
@@ -5229,7 +5229,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>21.23258182</v>
+        <v>80.177667360000001</v>
       </c>
       <c r="C23">
         <v>325.4162202</v>
@@ -5252,7 +5252,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>13.801923970000001</v>
+        <v>48.30885327</v>
       </c>
       <c r="C24">
         <v>157.17131099999997</v>
@@ -5275,7 +5275,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>18.97560992</v>
+        <v>35.13480878</v>
       </c>
       <c r="C25">
         <v>76.50550195000001</v>
@@ -5298,7 +5298,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>32.110115700000001</v>
+        <v>50.739999759999996</v>
       </c>
       <c r="C26">
         <v>72.042445189999995</v>
@@ -5321,7 +5321,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>32.813494220000003</v>
+        <v>40.74616657</v>
       </c>
       <c r="C27">
         <v>48.517599370000006</v>
@@ -5344,7 +5344,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>29.418505789999998</v>
+        <v>29.260138309999999</v>
       </c>
       <c r="C28">
         <v>42.934383909999994</v>
@@ -5367,7 +5367,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>27.87798347</v>
+        <v>27.96941739</v>
       </c>
       <c r="C29">
         <v>48.678900759999998</v>
@@ -5390,7 +5390,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>23.495424790000001</v>
+        <v>25.635685850000002</v>
       </c>
       <c r="C30">
         <v>41.501980959999997</v>
@@ -5413,7 +5413,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>35.21547769</v>
+        <v>41.571222470000002</v>
       </c>
       <c r="C31">
         <v>63.788940189999998</v>
@@ -5436,7 +5436,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>71.951563639999989</v>
+        <v>86.141379270000002</v>
       </c>
       <c r="C32">
         <v>189.85580300000001</v>
@@ -5459,7 +5459,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>64.690413219999996</v>
+        <v>273.29278149999999</v>
       </c>
       <c r="C33">
         <v>462.03587599999997</v>
@@ -5482,7 +5482,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>43.138492559999996</v>
+        <v>307.63734909999999</v>
       </c>
       <c r="C34">
         <v>514.38671190000002</v>
@@ -5505,7 +5505,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>21.23258182</v>
+        <v>120.152479</v>
       </c>
       <c r="C35">
         <v>175.12004639999998</v>
@@ -5528,7 +5528,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>13.801923970000001</v>
+        <v>68.633078740000002</v>
       </c>
       <c r="C36">
         <v>77.042593139999994</v>
@@ -5551,7 +5551,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>18.97560992</v>
+        <v>48.996869079999996</v>
       </c>
       <c r="C37">
         <v>59.260924070000002</v>
@@ -5579,7 +5579,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B2" sqref="B2:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5612,7 +5612,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>14.970879999999999</v>
+        <v>20.33756</v>
       </c>
       <c r="C2">
         <v>169.04750000000001</v>
@@ -5635,7 +5635,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>26.954619999999998</v>
+        <v>18.924009999999999</v>
       </c>
       <c r="C3">
         <v>85.647600000000011</v>
@@ -5658,7 +5658,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>18.25827</v>
+        <v>22.01257</v>
       </c>
       <c r="C4">
         <v>59.939</v>
@@ -5681,7 +5681,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>21.393889999999999</v>
+        <v>25.471310000000003</v>
       </c>
       <c r="C5">
         <v>61.521560000000001</v>
@@ -5704,7 +5704,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>20.954930000000001</v>
+        <v>28.280740000000002</v>
       </c>
       <c r="C6">
         <v>52.56156</v>
@@ -5727,7 +5727,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>47.637879999999996</v>
+        <v>104.3515</v>
       </c>
       <c r="C7">
         <v>136.8801</v>
@@ -5750,7 +5750,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>70.065830000000005</v>
+        <v>95.365289999999987</v>
       </c>
       <c r="C8">
         <v>232.77549999999999</v>
@@ -5773,7 +5773,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>46.065599999999996</v>
+        <v>122.5091</v>
       </c>
       <c r="C9">
         <v>452.05059999999997</v>
@@ -5796,7 +5796,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>157.2115</v>
+        <v>239.87779999999998</v>
       </c>
       <c r="C10">
         <v>975.82140000000004</v>
@@ -5819,7 +5819,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>63.639069999999997</v>
+        <v>153.726</v>
       </c>
       <c r="C11">
         <v>512.54129999999998</v>
@@ -5842,7 +5842,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>13.298</v>
+        <v>68.679179999999988</v>
       </c>
       <c r="C12">
         <v>247.72749999999999</v>
@@ -5865,7 +5865,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>28.954229999999999</v>
+        <v>53.122419999999998</v>
       </c>
       <c r="C13">
         <v>164.14679999999998</v>
@@ -5888,7 +5888,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>14.970879999999999</v>
+        <v>36.973910000000004</v>
       </c>
       <c r="C14">
         <v>140.1962</v>
@@ -5911,7 +5911,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>26.954619999999998</v>
+        <v>47.918039999999998</v>
       </c>
       <c r="C15">
         <v>112.52189999999999</v>
@@ -5934,7 +5934,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>18.25827</v>
+        <v>28.404400000000003</v>
       </c>
       <c r="C16">
         <v>90.910570000000007</v>
@@ -5957,7 +5957,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>21.393889999999999</v>
+        <v>30.70806</v>
       </c>
       <c r="C17">
         <v>84.902289999999994</v>
@@ -5980,7 +5980,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>20.954930000000001</v>
+        <v>35.77704</v>
       </c>
       <c r="C18">
         <v>75.771539999999987</v>
@@ -6003,7 +6003,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>47.637879999999996</v>
+        <v>76.180050000000008</v>
       </c>
       <c r="C19">
         <v>140.35050000000001</v>
@@ -6026,7 +6026,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>70.065830000000005</v>
+        <v>106.428</v>
       </c>
       <c r="C20">
         <v>235.99610000000001</v>
@@ -6049,7 +6049,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>46.065599999999996</v>
+        <v>92.201530000000005</v>
       </c>
       <c r="C21">
         <v>543.29669999999999</v>
@@ -6072,7 +6072,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>157.2115</v>
+        <v>261.35309999999998</v>
       </c>
       <c r="C22">
         <v>530.226</v>
@@ -6095,7 +6095,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>63.639069999999997</v>
+        <v>162.10599999999999</v>
       </c>
       <c r="C23">
         <v>370.27909999999997</v>
@@ -6118,7 +6118,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>13.298</v>
+        <v>59.494690000000006</v>
       </c>
       <c r="C24">
         <v>203.21079999999998</v>
@@ -6141,7 +6141,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>28.954229999999999</v>
+        <v>48.890449999999994</v>
       </c>
       <c r="C25">
         <v>118.09389999999999</v>
@@ -6164,7 +6164,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>14.970879999999999</v>
+        <v>35.780739999999994</v>
       </c>
       <c r="C26">
         <v>118.96599999999999</v>
@@ -6187,7 +6187,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>26.954619999999998</v>
+        <v>47.075410000000005</v>
       </c>
       <c r="C27">
         <v>85.920659999999998</v>
@@ -6210,7 +6210,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>18.25827</v>
+        <v>22.76275</v>
       </c>
       <c r="C28">
         <v>52.190190000000001</v>
@@ -6233,7 +6233,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>21.393889999999999</v>
+        <v>38.115029999999997</v>
       </c>
       <c r="C29">
         <v>61.143730000000005</v>
@@ -6256,7 +6256,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>20.954930000000001</v>
+        <v>39.982610000000001</v>
       </c>
       <c r="C30">
         <v>51.260640000000002</v>
@@ -6279,7 +6279,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>47.637879999999996</v>
+        <v>67.268679999999989</v>
       </c>
       <c r="C31">
         <v>109.876</v>
@@ -6302,7 +6302,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>70.065830000000005</v>
+        <v>95.591649999999987</v>
       </c>
       <c r="C32">
         <v>286.45740000000001</v>
@@ -6325,7 +6325,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>46.065599999999996</v>
+        <v>195.31210000000002</v>
       </c>
       <c r="C33">
         <v>312.86859999999996</v>
@@ -6348,7 +6348,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>157.2115</v>
+        <v>506.25880000000001</v>
       </c>
       <c r="C34">
         <v>209.73729999999998</v>
@@ -6371,7 +6371,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>63.639069999999997</v>
+        <v>142.50779999999997</v>
       </c>
       <c r="C35">
         <v>127.7692</v>
@@ -6394,7 +6394,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>13.298</v>
+        <v>97.705389999999994</v>
       </c>
       <c r="C36">
         <v>48.783610000000003</v>
@@ -6417,7 +6417,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>28.954229999999999</v>
+        <v>67.803789999999992</v>
       </c>
       <c r="C37">
         <v>35.540120000000002</v>
@@ -6445,7 +6445,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B2" sqref="B2:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6478,7 +6478,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>21.273599999999998</v>
+        <v>22.420480000000001</v>
       </c>
       <c r="C2">
         <v>129.3175</v>
@@ -6501,7 +6501,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>26.996009999999998</v>
+        <v>27.626840000000001</v>
       </c>
       <c r="C3">
         <v>61.481319999999997</v>
@@ -6524,7 +6524,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>23.327310000000001</v>
+        <v>21.969429999999999</v>
       </c>
       <c r="C4">
         <v>46.940440000000002</v>
@@ -6547,7 +6547,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>22.07075</v>
+        <v>22.889669999999999</v>
       </c>
       <c r="C5">
         <v>42.761890000000001</v>
@@ -6570,7 +6570,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>18.617339999999999</v>
+        <v>21.369439999999997</v>
       </c>
       <c r="C6">
         <v>35.075029999999998</v>
@@ -6593,7 +6593,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>29.762450000000001</v>
+        <v>49.170929999999998</v>
       </c>
       <c r="C7">
         <v>63.06006</v>
@@ -6616,7 +6616,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>54.981629999999996</v>
+        <v>67.760249999999999</v>
       </c>
       <c r="C8">
         <v>115.89439999999999</v>
@@ -6639,7 +6639,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>45.791830000000004</v>
+        <v>95.74973</v>
       </c>
       <c r="C9">
         <v>236.249</v>
@@ -6662,7 +6662,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>160.1464</v>
+        <v>214.14400000000001</v>
       </c>
       <c r="C10">
         <v>522.69079999999997</v>
@@ -6685,7 +6685,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>69.484700000000004</v>
+        <v>140.72620000000001</v>
       </c>
       <c r="C11">
         <v>359.62729999999999</v>
@@ -6708,7 +6708,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>28.712499999999999</v>
+        <v>65.066850000000002</v>
       </c>
       <c r="C12">
         <v>160.2843</v>
@@ -6731,7 +6731,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>28.611720000000002</v>
+        <v>40.527670000000001</v>
       </c>
       <c r="C13">
         <v>103.8493</v>
@@ -6754,7 +6754,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>21.273599999999998</v>
+        <v>35.61412</v>
       </c>
       <c r="C14">
         <v>100.85239999999999</v>
@@ -6777,7 +6777,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>26.996009999999998</v>
+        <v>37.797260000000001</v>
       </c>
       <c r="C15">
         <v>70.01764</v>
@@ -6800,7 +6800,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>23.327310000000001</v>
+        <v>29.38804</v>
       </c>
       <c r="C16">
         <v>53.479800000000004</v>
@@ -6823,7 +6823,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>22.07075</v>
+        <v>26.242159999999998</v>
       </c>
       <c r="C17">
         <v>49.335059999999999</v>
@@ -6846,7 +6846,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>18.617339999999999</v>
+        <v>24.344339999999999</v>
       </c>
       <c r="C18">
         <v>39.879429999999999</v>
@@ -6869,7 +6869,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>29.762450000000001</v>
+        <v>46.252989999999997</v>
       </c>
       <c r="C19">
         <v>50.260649999999998</v>
@@ -6892,7 +6892,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>54.981629999999996</v>
+        <v>82.989750000000001</v>
       </c>
       <c r="C20">
         <v>109.2385</v>
@@ -6915,7 +6915,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>45.791830000000004</v>
+        <v>69.752279999999999</v>
       </c>
       <c r="C21">
         <v>243.55610000000001</v>
@@ -6938,7 +6938,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>160.1464</v>
+        <v>222.3032</v>
       </c>
       <c r="C22">
         <v>366.88909999999998</v>
@@ -6961,7 +6961,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>69.484700000000004</v>
+        <v>149.42760000000001</v>
       </c>
       <c r="C23">
         <v>290.44009999999997</v>
@@ -6984,7 +6984,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>28.712499999999999</v>
+        <v>61.891800000000003</v>
       </c>
       <c r="C24">
         <v>138.85929999999999</v>
@@ -7007,7 +7007,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>28.611720000000002</v>
+        <v>43.094379999999994</v>
       </c>
       <c r="C25">
         <v>82.289500000000004</v>
@@ -7030,7 +7030,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>21.273599999999998</v>
+        <v>40.161819999999999</v>
       </c>
       <c r="C26">
         <v>92.795410000000004</v>
@@ -7053,7 +7053,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>26.996009999999998</v>
+        <v>42.30594</v>
       </c>
       <c r="C27">
         <v>63.582650000000001</v>
@@ -7076,7 +7076,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>23.327310000000001</v>
+        <v>28.482970000000002</v>
       </c>
       <c r="C28">
         <v>36.659469999999999</v>
@@ -7099,7 +7099,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>22.07075</v>
+        <v>25.85201</v>
       </c>
       <c r="C29">
         <v>39.5837</v>
@@ -7122,7 +7122,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>18.617339999999999</v>
+        <v>22.516759999999998</v>
       </c>
       <c r="C30">
         <v>32.730879999999999</v>
@@ -7145,7 +7145,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>29.762450000000001</v>
+        <v>41.581009999999999</v>
       </c>
       <c r="C31">
         <v>47.732399999999998</v>
@@ -7168,7 +7168,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>54.981629999999996</v>
+        <v>69.753950000000003</v>
       </c>
       <c r="C32">
         <v>160.1337</v>
@@ -7191,7 +7191,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>45.791830000000004</v>
+        <v>146.82640000000001</v>
       </c>
       <c r="C33">
         <v>231.12309999999999</v>
@@ -7214,7 +7214,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>160.1464</v>
+        <v>357.33640000000003</v>
       </c>
       <c r="C34">
         <v>174.53149999999999</v>
@@ -7237,7 +7237,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>69.484700000000004</v>
+        <v>120.5804</v>
       </c>
       <c r="C35">
         <v>110.0626</v>
@@ -7260,7 +7260,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>28.712499999999999</v>
+        <v>70.49624</v>
       </c>
       <c r="C36">
         <v>57.69323</v>
@@ -7283,7 +7283,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>28.611720000000002</v>
+        <v>56.838370000000005</v>
       </c>
       <c r="C37">
         <v>45.54701</v>
@@ -7311,7 +7311,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B2" sqref="B2:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7344,7 +7344,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>28.5381</v>
+        <v>29.911240000000003</v>
       </c>
       <c r="C2">
         <v>57.626129999999996</v>
@@ -7367,7 +7367,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>29.192509999999999</v>
+        <v>28.338819999999998</v>
       </c>
       <c r="C3">
         <v>38.787129999999998</v>
@@ -7390,7 +7390,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>25.082039999999999</v>
+        <v>22.189720000000001</v>
       </c>
       <c r="C4">
         <v>29.786150000000003</v>
@@ -7413,7 +7413,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>23.545290000000001</v>
+        <v>24.796060000000001</v>
       </c>
       <c r="C5">
         <v>29.228069999999999</v>
@@ -7436,7 +7436,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>19.421470000000003</v>
+        <v>23.329759999999997</v>
       </c>
       <c r="C6">
         <v>26.373840000000001</v>
@@ -7459,7 +7459,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>31.86889</v>
+        <v>46.358839999999994</v>
       </c>
       <c r="C7">
         <v>35.352690000000003</v>
@@ -7482,7 +7482,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>62.345300000000002</v>
+        <v>109.8446</v>
       </c>
       <c r="C8">
         <v>50.902250000000002</v>
@@ -7505,7 +7505,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>58.214660000000002</v>
+        <v>151.24420000000001</v>
       </c>
       <c r="C9">
         <v>203.64060000000001</v>
@@ -7528,7 +7528,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>38.787849999999999</v>
+        <v>152.22749999999999</v>
       </c>
       <c r="C10">
         <v>493.82140000000004</v>
@@ -7551,7 +7551,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>16.12191</v>
+        <v>61.956510000000002</v>
       </c>
       <c r="C11">
         <v>256.48759999999999</v>
@@ -7574,7 +7574,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>10.89368</v>
+        <v>52.784059999999997</v>
       </c>
       <c r="C12">
         <v>123.27500000000001</v>
@@ -7597,7 +7597,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>14.6709</v>
+        <v>20.620480000000001</v>
       </c>
       <c r="C13">
         <v>44.78322</v>
@@ -7620,7 +7620,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>28.5381</v>
+        <v>28.987490000000001</v>
       </c>
       <c r="C14">
         <v>37.060900000000004</v>
@@ -7643,7 +7643,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>29.192509999999999</v>
+        <v>22.594930000000002</v>
       </c>
       <c r="C15">
         <v>34.854889999999997</v>
@@ -7666,7 +7666,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>25.082039999999999</v>
+        <v>18.803830000000001</v>
       </c>
       <c r="C16">
         <v>38.088900000000002</v>
@@ -7689,7 +7689,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>23.545290000000001</v>
+        <v>19.816419999999997</v>
       </c>
       <c r="C17">
         <v>32.390709999999999</v>
@@ -7712,7 +7712,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>19.421470000000003</v>
+        <v>17.826409999999999</v>
       </c>
       <c r="C18">
         <v>25.403419999999997</v>
@@ -7735,7 +7735,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>31.86889</v>
+        <v>27.187889999999999</v>
       </c>
       <c r="C19">
         <v>31.203799999999998</v>
@@ -7758,7 +7758,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>62.345300000000002</v>
+        <v>44.451610000000002</v>
       </c>
       <c r="C20">
         <v>89.73163000000001</v>
@@ -7781,7 +7781,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>58.214660000000002</v>
+        <v>102.6858</v>
       </c>
       <c r="C21">
         <v>657.4303000000001</v>
@@ -7804,7 +7804,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>38.787849999999999</v>
+        <v>192.3827</v>
       </c>
       <c r="C22">
         <v>578.86369999999999</v>
@@ -7827,7 +7827,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>16.12191</v>
+        <v>71.992339999999999</v>
       </c>
       <c r="C23">
         <v>281.83409999999998</v>
@@ -7850,7 +7850,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>10.89368</v>
+        <v>41.72531</v>
       </c>
       <c r="C24">
         <v>138.90049999999999</v>
@@ -7873,7 +7873,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>14.6709</v>
+        <v>28.400500000000001</v>
       </c>
       <c r="C25">
         <v>68.058460000000011</v>
@@ -7896,7 +7896,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>28.5381</v>
+        <v>43.372599999999998</v>
       </c>
       <c r="C26">
         <v>62.2288</v>
@@ -7919,7 +7919,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>29.192509999999999</v>
+        <v>37.838980000000006</v>
       </c>
       <c r="C27">
         <v>43.886830000000003</v>
@@ -7942,7 +7942,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>25.082039999999999</v>
+        <v>25.574840000000002</v>
       </c>
       <c r="C28">
         <v>37.042010000000005</v>
@@ -7965,7 +7965,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>23.545290000000001</v>
+        <v>23.57958</v>
       </c>
       <c r="C29">
         <v>35.209669999999996</v>
@@ -7988,7 +7988,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>19.421470000000003</v>
+        <v>22.229140000000001</v>
       </c>
       <c r="C30">
         <v>31.159880000000001</v>
@@ -8011,7 +8011,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>31.86889</v>
+        <v>36.467760000000006</v>
       </c>
       <c r="C31">
         <v>49.345660000000002</v>
@@ -8034,7 +8034,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>62.345300000000002</v>
+        <v>78.578009999999992</v>
       </c>
       <c r="C32">
         <v>162.48479999999998</v>
@@ -8057,7 +8057,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>58.214660000000002</v>
+        <v>231.60050000000001</v>
       </c>
       <c r="C33">
         <v>400.29859999999996</v>
@@ -8080,7 +8080,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>38.787849999999999</v>
+        <v>261.68209999999999</v>
       </c>
       <c r="C34">
         <v>445.2208</v>
@@ -8103,7 +8103,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>16.12191</v>
+        <v>103.7231</v>
       </c>
       <c r="C35">
         <v>157.01139999999998</v>
@@ -8126,7 +8126,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>10.89368</v>
+        <v>55.27234</v>
       </c>
       <c r="C36">
         <v>68.470179999999999</v>
@@ -8149,7 +8149,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>14.6709</v>
+        <v>35.529389999999999</v>
       </c>
       <c r="C37">
         <v>51.228819999999999</v>
@@ -8177,7 +8177,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B2" sqref="B2:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8210,7 +8210,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>10.021450000000002</v>
+        <v>17.748669999999997</v>
       </c>
       <c r="C2">
         <v>75.344719999999995</v>
@@ -8233,7 +8233,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>12.19148</v>
+        <v>17.533480000000001</v>
       </c>
       <c r="C3">
         <v>46.063499999999998</v>
@@ -8256,7 +8256,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>13.011670000000001</v>
+        <v>15.71598</v>
       </c>
       <c r="C4">
         <v>43.659769999999995</v>
@@ -8279,7 +8279,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>11.895149999999999</v>
+        <v>17.264040000000001</v>
       </c>
       <c r="C5">
         <v>1.0055529999999999</v>
@@ -8302,7 +8302,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>10.178520000000001</v>
+        <v>27.449660000000002</v>
       </c>
       <c r="C6">
         <v>43.26229</v>
@@ -8325,7 +8325,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>15.90635</v>
+        <v>137.28829999999999</v>
       </c>
       <c r="C7">
         <v>110.98339999999999</v>
@@ -8348,7 +8348,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>35.733160000000005</v>
+        <v>191.40810000000002</v>
       </c>
       <c r="C8">
         <v>179.8477</v>
@@ -8371,7 +8371,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>7.5885420000000003</v>
+        <v>169.8776</v>
       </c>
       <c r="C9">
         <v>314.64299999999997</v>
@@ -8394,7 +8394,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>-10.4526</v>
+        <v>93.102050000000006</v>
       </c>
       <c r="C10">
         <v>414.76890000000003</v>
@@ -8417,7 +8417,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>3.8717159999999997</v>
+        <v>15.737129999999999</v>
       </c>
       <c r="C11">
         <v>168.04429999999999</v>
@@ -8440,7 +8440,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>-3.19814</v>
+        <v>21.246419999999997</v>
       </c>
       <c r="C12">
         <v>60.047730000000001</v>
@@ -8463,7 +8463,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>10.64512</v>
+        <v>9.9849359999999994</v>
       </c>
       <c r="C13">
         <v>13.002139999999999</v>
@@ -8486,7 +8486,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>10.021450000000002</v>
+        <v>29.356729999999999</v>
       </c>
       <c r="C14">
         <v>64.497839999999997</v>
@@ -8509,7 +8509,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>12.19148</v>
+        <v>9.9630299999999998</v>
       </c>
       <c r="C15">
         <v>25.684750000000001</v>
@@ -8532,7 +8532,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>13.011670000000001</v>
+        <v>6.9595209999999996</v>
       </c>
       <c r="C16">
         <v>30.688310000000001</v>
@@ -8555,7 +8555,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>11.895149999999999</v>
+        <v>8.9373619999999985</v>
       </c>
       <c r="C17">
         <v>29.408150000000003</v>
@@ -8578,7 +8578,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>10.178520000000001</v>
+        <v>10.98348</v>
       </c>
       <c r="C18">
         <v>35.651129999999995</v>
@@ -8601,7 +8601,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>15.90635</v>
+        <v>28.956169999999997</v>
       </c>
       <c r="C19">
         <v>101.2761</v>
@@ -8624,7 +8624,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>35.733160000000005</v>
+        <v>90.381559999999993</v>
       </c>
       <c r="C20">
         <v>154.72929999999999</v>
@@ -8647,7 +8647,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>7.5885420000000003</v>
+        <v>198.63129999999998</v>
       </c>
       <c r="C21">
         <v>426.0181</v>
@@ -8670,7 +8670,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>-10.4526</v>
+        <v>196.8229</v>
       </c>
       <c r="C22">
         <v>228.25910000000002</v>
@@ -8693,7 +8693,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>3.8717159999999997</v>
+        <v>66.634539999999987</v>
       </c>
       <c r="C23">
         <v>56.936970000000002</v>
@@ -8716,7 +8716,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>-3.19814</v>
+        <v>35.160690000000002</v>
       </c>
       <c r="C24">
         <v>63.035440000000001</v>
@@ -8739,7 +8739,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>10.64512</v>
+        <v>40.31814</v>
       </c>
       <c r="C25">
         <v>43.810389999999998</v>
@@ -8762,7 +8762,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>10.021450000000002</v>
+        <v>64.725560000000002</v>
       </c>
       <c r="C26">
         <v>87.143320000000003</v>
@@ -8785,7 +8785,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>12.19148</v>
+        <v>42.68385</v>
       </c>
       <c r="C27">
         <v>49.978550000000006</v>
@@ -8808,7 +8808,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>13.011670000000001</v>
+        <v>24.70768</v>
       </c>
       <c r="C28">
         <v>51.539760000000001</v>
@@ -8831,7 +8831,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>11.895149999999999</v>
+        <v>23.775389999999998</v>
       </c>
       <c r="C29">
         <v>33.395650000000003</v>
@@ -8854,7 +8854,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>10.178520000000001</v>
+        <v>29.48254</v>
       </c>
       <c r="C30">
         <v>39.099059999999994</v>
@@ -8877,7 +8877,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>15.90635</v>
+        <v>63.039199999999994</v>
       </c>
       <c r="C31">
         <v>189.46770000000001</v>
@@ -8900,7 +8900,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>35.733160000000005</v>
+        <v>198.83429999999998</v>
       </c>
       <c r="C32">
         <v>391.90949999999998</v>
@@ -8923,7 +8923,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>7.5885420000000003</v>
+        <v>259.34410000000003</v>
       </c>
       <c r="C33">
         <v>462.69309999999996</v>
@@ -8946,7 +8946,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>-10.4526</v>
+        <v>187.26570000000001</v>
       </c>
       <c r="C34">
         <v>443.85129999999998</v>
@@ -8969,7 +8969,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>3.8717159999999997</v>
+        <v>34.649099999999997</v>
       </c>
       <c r="C35">
         <v>117.72839999999999</v>
@@ -8992,7 +8992,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>-3.19814</v>
+        <v>38.17568</v>
       </c>
       <c r="C36">
         <v>42.762740000000001</v>
@@ -9015,7 +9015,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>10.64512</v>
+        <v>83.770649999999989</v>
       </c>
       <c r="C37">
         <v>83.437619999999995</v>
@@ -9043,7 +9043,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B2" sqref="B2:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9076,7 +9076,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>60.37</v>
+        <v>48.204999999999998</v>
       </c>
       <c r="C2">
         <v>85.269000000000005</v>
@@ -9099,7 +9099,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>48.1</v>
+        <v>34.927</v>
       </c>
       <c r="C3">
         <v>51.2</v>
@@ -9122,7 +9122,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>38.956000000000003</v>
+        <v>29.489000000000001</v>
       </c>
       <c r="C4">
         <v>49.487000000000002</v>
@@ -9145,7 +9145,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>32.081000000000003</v>
+        <v>33.975999999999999</v>
       </c>
       <c r="C5">
         <v>34.761000000000003</v>
@@ -9168,7 +9168,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>21.065000000000001</v>
+        <v>37.262999999999998</v>
       </c>
       <c r="C6">
         <v>35.189</v>
@@ -9191,7 +9191,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>33.061</v>
+        <v>61.067</v>
       </c>
       <c r="C7">
         <v>51.15</v>
@@ -9214,7 +9214,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>55.658000000000001</v>
+        <v>134.399</v>
       </c>
       <c r="C8">
         <v>104.712</v>
@@ -9237,7 +9237,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>34.543999999999997</v>
+        <v>111.255</v>
       </c>
       <c r="C9">
         <v>428.37900000000002</v>
@@ -9260,7 +9260,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>14.784000000000001</v>
+        <v>67.995000000000005</v>
       </c>
       <c r="C10">
         <v>573.36599999999999</v>
@@ -9283,7 +9283,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>2.5459999999999998</v>
+        <v>23.109000000000002</v>
       </c>
       <c r="C11">
         <v>250.25200000000001</v>
@@ -9306,7 +9306,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>19.314</v>
+        <v>28.164000000000001</v>
       </c>
       <c r="C12">
         <v>86.494</v>
@@ -9329,7 +9329,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>48.661000000000001</v>
+        <v>41.506</v>
       </c>
       <c r="C13">
         <v>49.707000000000001</v>
@@ -9352,7 +9352,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>60.37</v>
+        <v>57.545000000000002</v>
       </c>
       <c r="C14">
         <v>74.402000000000001</v>
@@ -9375,7 +9375,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>48.1</v>
+        <v>39.061999999999998</v>
       </c>
       <c r="C15">
         <v>51.75</v>
@@ -9398,7 +9398,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>38.956000000000003</v>
+        <v>37.182000000000002</v>
       </c>
       <c r="C16">
         <v>55.29</v>
@@ -9421,7 +9421,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>32.081000000000003</v>
+        <v>28.965</v>
       </c>
       <c r="C17">
         <v>37.475999999999999</v>
@@ -9444,7 +9444,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>21.065000000000001</v>
+        <v>20.663</v>
       </c>
       <c r="C18">
         <v>39.938000000000002</v>
@@ -9467,7 +9467,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>33.061</v>
+        <v>29.103999999999999</v>
       </c>
       <c r="C19">
         <v>42.962000000000003</v>
@@ -9490,7 +9490,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>55.658000000000001</v>
+        <v>52.813000000000002</v>
       </c>
       <c r="C20">
         <v>124.867</v>
@@ -9513,7 +9513,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>34.543999999999997</v>
+        <v>87.227000000000004</v>
       </c>
       <c r="C21">
         <v>600.93600000000004</v>
@@ -9536,7 +9536,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>14.784000000000001</v>
+        <v>71.593999999999994</v>
       </c>
       <c r="C22">
         <v>437.95299999999997</v>
@@ -9559,7 +9559,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>2.5459999999999998</v>
+        <v>25.241</v>
       </c>
       <c r="C23">
         <v>132.39500000000001</v>
@@ -9582,7 +9582,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>19.314</v>
+        <v>14.561999999999999</v>
       </c>
       <c r="C24">
         <v>77.998000000000005</v>
@@ -9605,7 +9605,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>48.661000000000001</v>
+        <v>50.073999999999998</v>
       </c>
       <c r="C25">
         <v>84.79</v>
@@ -9628,7 +9628,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>60.37</v>
+        <v>70.822000000000003</v>
       </c>
       <c r="C26">
         <v>103.297</v>
@@ -9651,7 +9651,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>48.1</v>
+        <v>38.637999999999998</v>
       </c>
       <c r="C27">
         <v>64.864000000000004</v>
@@ -9674,7 +9674,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>38.956000000000003</v>
+        <v>28.521999999999998</v>
       </c>
       <c r="C28">
         <v>58.972999999999999</v>
@@ -9697,7 +9697,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>32.081000000000003</v>
+        <v>23.189</v>
       </c>
       <c r="C29">
         <v>30.925000000000001</v>
@@ -9720,7 +9720,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>21.065000000000001</v>
+        <v>24.265999999999998</v>
       </c>
       <c r="C30">
         <v>31.488</v>
@@ -9743,7 +9743,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>33.061</v>
+        <v>31.861999999999998</v>
       </c>
       <c r="C31">
         <v>62.232999999999997</v>
@@ -9766,7 +9766,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>55.658000000000001</v>
+        <v>54.905000000000001</v>
       </c>
       <c r="C32">
         <v>291.58699999999999</v>
@@ -9789,7 +9789,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>34.543999999999997</v>
+        <v>190.47900000000001</v>
       </c>
       <c r="C33">
         <v>494.05599999999998</v>
@@ -9812,7 +9812,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>14.784000000000001</v>
+        <v>142.92699999999999</v>
       </c>
       <c r="C34">
         <v>228.32499999999999</v>
@@ -9835,7 +9835,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>2.5459999999999998</v>
+        <v>43.594000000000001</v>
       </c>
       <c r="C35">
         <v>81.888000000000005</v>
@@ -9858,7 +9858,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>19.314</v>
+        <v>23.756</v>
       </c>
       <c r="C36">
         <v>27.384</v>
@@ -9881,7 +9881,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>48.661000000000001</v>
+        <v>45.13</v>
       </c>
       <c r="C37">
         <v>70.25</v>
@@ -9909,7 +9909,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B2" sqref="B2:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9942,7 +9942,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>158.81595000000002</v>
+        <v>260.28469000000001</v>
       </c>
       <c r="C2">
         <v>846.84659999999997</v>
@@ -9965,7 +9965,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>287.96489000000003</v>
+        <v>272.4674</v>
       </c>
       <c r="C3">
         <v>667.49953000000005</v>
@@ -9988,7 +9988,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>226.2824</v>
+        <v>246.49001000000001</v>
       </c>
       <c r="C4">
         <v>543.58793000000003</v>
@@ -10011,7 +10011,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>233.20201999999998</v>
+        <v>205.31920000000002</v>
       </c>
       <c r="C5">
         <v>449.51796999999999</v>
@@ -10034,7 +10034,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>215.52601999999999</v>
+        <v>330.68854999999996</v>
       </c>
       <c r="C6">
         <v>469.14665000000002</v>
@@ -10057,7 +10057,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>296.53591999999998</v>
+        <v>747.62995999999998</v>
       </c>
       <c r="C7">
         <v>1001.97183</v>
@@ -10080,7 +10080,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>386.59916999999996</v>
+        <v>965.29324999999994</v>
       </c>
       <c r="C8">
         <v>1130.7236</v>
@@ -10103,7 +10103,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>311.30665000000005</v>
+        <v>1068.1749499999999</v>
       </c>
       <c r="C9">
         <v>3205.0938500000002</v>
@@ -10126,7 +10126,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>284.45735999999999</v>
+        <v>1043.7099699999999</v>
       </c>
       <c r="C10">
         <v>6659.4755599999999</v>
@@ -10149,7 +10149,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>-18.405060000000002</v>
+        <v>335.76249999999999</v>
       </c>
       <c r="C11">
         <v>3547.5024199999998</v>
@@ -10172,7 +10172,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>-49.893699999999995</v>
+        <v>339.38526999999999</v>
       </c>
       <c r="C12">
         <v>1287.8981999999999</v>
@@ -10195,7 +10195,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>310.33545000000004</v>
+        <v>124.22367999999999</v>
       </c>
       <c r="C13">
         <v>561.35106999999994</v>
@@ -10218,7 +10218,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>158.81595000000002</v>
+        <v>237.74179999999998</v>
       </c>
       <c r="C14">
         <v>716.36901</v>
@@ -10241,7 +10241,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>287.96489000000003</v>
+        <v>288.48759999999999</v>
       </c>
       <c r="C15">
         <v>595.52926000000002</v>
@@ -10264,7 +10264,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>226.2824</v>
+        <v>247.55924999999999</v>
       </c>
       <c r="C16">
         <v>541.21950000000004</v>
@@ -10287,7 +10287,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>233.20201999999998</v>
+        <v>271.04752000000002</v>
       </c>
       <c r="C17">
         <v>397.41045000000003</v>
@@ -10310,7 +10310,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>215.52601999999999</v>
+        <v>204.91283999999999</v>
       </c>
       <c r="C18">
         <v>479.55982</v>
@@ -10333,7 +10333,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>296.53591999999998</v>
+        <v>377.20555000000002</v>
       </c>
       <c r="C19">
         <v>760.60487999999998</v>
@@ -10356,7 +10356,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>386.59916999999996</v>
+        <v>455.58172999999999</v>
       </c>
       <c r="C20">
         <v>1522.8559</v>
@@ -10379,7 +10379,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>311.30665000000005</v>
+        <v>708.49370999999996</v>
       </c>
       <c r="C21">
         <v>5429.2664100000002</v>
@@ -10402,7 +10402,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>284.45735999999999</v>
+        <v>1438.6799099999998</v>
       </c>
       <c r="C22">
         <v>5687.9918899999993</v>
@@ -10425,7 +10425,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>-18.405060000000002</v>
+        <v>581.30113000000006</v>
       </c>
       <c r="C23">
         <v>2676.0059900000001</v>
@@ -10448,7 +10448,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>-49.893699999999995</v>
+        <v>197.25624999999999</v>
       </c>
       <c r="C24">
         <v>1376.8901899999998</v>
@@ -10471,7 +10471,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>310.33545000000004</v>
+        <v>302.60960999999998</v>
       </c>
       <c r="C25">
         <v>661.97355000000005</v>
@@ -10494,7 +10494,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>158.81595000000002</v>
+        <v>454.74218999999999</v>
       </c>
       <c r="C26">
         <v>881.92110000000002</v>
@@ -10517,7 +10517,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>287.96489000000003</v>
+        <v>386.21096</v>
       </c>
       <c r="C27">
         <v>691.69087000000002</v>
@@ -10540,7 +10540,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>226.2824</v>
+        <v>276.30721999999997</v>
       </c>
       <c r="C28">
         <v>540.37846000000002</v>
@@ -10563,7 +10563,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>233.20201999999998</v>
+        <v>504.20076</v>
       </c>
       <c r="C29">
         <v>539.64705000000004</v>
@@ -10586,7 +10586,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>215.52601999999999</v>
+        <v>493.39231000000001</v>
       </c>
       <c r="C30">
         <v>455.70453000000003</v>
@@ -10609,7 +10609,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>296.53591999999998</v>
+        <v>500.71429999999998</v>
       </c>
       <c r="C31">
         <v>1141.30573</v>
@@ -10632,7 +10632,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>386.59916999999996</v>
+        <v>749.45023000000003</v>
       </c>
       <c r="C32">
         <v>2707.6015400000001</v>
@@ -10655,7 +10655,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>311.30665000000005</v>
+        <v>1550.6840199999999</v>
       </c>
       <c r="C33">
         <v>4366.7583399999994</v>
@@ -10678,7 +10678,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>284.45735999999999</v>
+        <v>2358.6873900000001</v>
       </c>
       <c r="C34">
         <v>3799.56016</v>
@@ -10701,7 +10701,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>-18.405060000000002</v>
+        <v>629.63194999999996</v>
       </c>
       <c r="C35">
         <v>1331.4722199999999</v>
@@ -10724,7 +10724,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>-49.893699999999995</v>
+        <v>398.57389000000001</v>
       </c>
       <c r="C36">
         <v>553.74089000000004</v>
@@ -10747,7 +10747,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>310.33545000000004</v>
+        <v>498.08321999999998</v>
       </c>
       <c r="C37">
         <v>506.79510999999997</v>

</xml_diff>

<commit_message>
Rule edit - Mead Exclusive Flood Control Space
Edited execution constraint to check if FC slot was greater than 0 (not just Not NaN). This rule was setting Mead outflow during very low scenarios in which flood control rules should not be executing.
</commit_message>
<xml_diff>
--- a/Input Data/DevTesting/DevTesting_InflowsTEST.xlsx
+++ b/Input Data/DevTesting/DevTesting_InflowsTEST.xlsx
@@ -416,7 +416,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>15.79041</v>
+        <v>19.441980000000001</v>
       </c>
       <c r="C2">
         <v>29.924630000000001</v>
@@ -439,7 +439,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>12.844959999999999</v>
+        <v>13.76132</v>
       </c>
       <c r="C3">
         <v>17.456529999999997</v>
@@ -462,7 +462,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>11.424790000000002</v>
+        <v>13.449920000000001</v>
       </c>
       <c r="C4">
         <v>15.51074</v>
@@ -485,7 +485,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>11.26017</v>
+        <v>12.900499999999999</v>
       </c>
       <c r="C5">
         <v>13.77521</v>
@@ -508,7 +508,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>11.56165</v>
+        <v>13.215870000000001</v>
       </c>
       <c r="C6">
         <v>13.44595</v>
@@ -531,7 +531,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>21.15372</v>
+        <v>36.56926</v>
       </c>
       <c r="C7">
         <v>21.274709999999999</v>
@@ -554,7 +554,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>49.432070000000003</v>
+        <v>76.125619999999998</v>
       </c>
       <c r="C8">
         <v>38.318680000000001</v>
@@ -577,7 +577,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>209.61320000000001</v>
+        <v>104.5686</v>
       </c>
       <c r="C9">
         <v>142.84960000000001</v>
@@ -600,7 +600,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>103.21980000000001</v>
+        <v>75.929259999999999</v>
       </c>
       <c r="C10">
         <v>241.46779999999998</v>
@@ -623,7 +623,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>45.758679999999998</v>
+        <v>34.538179999999997</v>
       </c>
       <c r="C11">
         <v>139.16029999999998</v>
@@ -646,7 +646,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>14.51702</v>
+        <v>30.251900000000003</v>
       </c>
       <c r="C12">
         <v>56.11835</v>
@@ -669,7 +669,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>12.69421</v>
+        <v>13.16033</v>
       </c>
       <c r="C13">
         <v>22.746449999999999</v>
@@ -692,7 +692,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>12.46017</v>
+        <v>15.98479</v>
       </c>
       <c r="C14">
         <v>27.465119999999999</v>
@@ -715,7 +715,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>10.10182</v>
+        <v>10.61157</v>
       </c>
       <c r="C15">
         <v>15.675370000000001</v>
@@ -738,7 +738,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>8.8879339999999996</v>
+        <v>7.9517359999999995</v>
       </c>
       <c r="C16">
         <v>17.018180000000001</v>
@@ -761,7 +761,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>9.778512000000001</v>
+        <v>7.5173549999999993</v>
       </c>
       <c r="C17">
         <v>15.21917</v>
@@ -784,7 +784,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>9.1398349999999997</v>
+        <v>7.4836360000000006</v>
       </c>
       <c r="C18">
         <v>15.18942</v>
@@ -807,7 +807,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>12.311399999999999</v>
+        <v>8.2076029999999989</v>
       </c>
       <c r="C19">
         <v>22.08</v>
@@ -830,7 +830,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>51.094209999999997</v>
+        <v>21.365950000000002</v>
       </c>
       <c r="C20">
         <v>46.151400000000002</v>
@@ -853,7 +853,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>131.1848</v>
+        <v>93.10611999999999</v>
       </c>
       <c r="C21">
         <v>229.4281</v>
@@ -876,7 +876,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>114.3888</v>
+        <v>130.05019999999999</v>
       </c>
       <c r="C22">
         <v>176.8066</v>
@@ -899,7 +899,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>27.149750000000001</v>
+        <v>44.526940000000003</v>
       </c>
       <c r="C23">
         <v>103.69589999999999</v>
@@ -922,7 +922,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>35.162980000000005</v>
+        <v>24.902480000000001</v>
       </c>
       <c r="C24">
         <v>62.717359999999999</v>
@@ -945,7 +945,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>17.960330000000003</v>
+        <v>25.378509999999999</v>
       </c>
       <c r="C25">
         <v>35.688600000000001</v>
@@ -968,7 +968,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>16.989419999999999</v>
+        <v>39.286910000000006</v>
       </c>
       <c r="C26">
         <v>36.099170000000001</v>
@@ -991,7 +991,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>14.1243</v>
+        <v>21.189060000000001</v>
       </c>
       <c r="C27">
         <v>21.459169999999997</v>
@@ -1014,7 +1014,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>13.76727</v>
+        <v>22.05152</v>
       </c>
       <c r="C28">
         <v>16.532229999999998</v>
@@ -1037,7 +1037,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>11.406940000000001</v>
+        <v>16.454060000000002</v>
       </c>
       <c r="C29">
         <v>15.30843</v>
@@ -1060,7 +1060,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>9.9629750000000001</v>
+        <v>12.43914</v>
       </c>
       <c r="C30">
         <v>12.440329999999999</v>
@@ -1083,7 +1083,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>15.859830000000001</v>
+        <v>15.50592</v>
       </c>
       <c r="C31">
         <v>27.498840000000001</v>
@@ -1106,7 +1106,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>40.68694</v>
+        <v>48.120040000000003</v>
       </c>
       <c r="C32">
         <v>108.2043</v>
@@ -1129,7 +1129,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>90.614879999999999</v>
+        <v>126.32539999999999</v>
       </c>
       <c r="C33">
         <v>195.5504</v>
@@ -1152,7 +1152,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>217.3289</v>
+        <v>125.53530000000001</v>
       </c>
       <c r="C34">
         <v>253.01160000000002</v>
@@ -1175,7 +1175,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>83.498179999999991</v>
+        <v>44.607870000000005</v>
       </c>
       <c r="C35">
         <v>99.431399999999996</v>
@@ -1198,7 +1198,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>25.03537</v>
+        <v>24.032049999999998</v>
       </c>
       <c r="C36">
         <v>37.176199999999994</v>
@@ -1221,7 +1221,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>16.367599999999999</v>
+        <v>46.412550000000003</v>
       </c>
       <c r="C37">
         <v>42.928260000000002</v>
@@ -1282,7 +1282,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>4.8311157300000005</v>
+        <v>4.5902854780700002</v>
       </c>
       <c r="C2">
         <v>8.2923371899999996</v>
@@ -1305,7 +1305,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>5.2234959600000002</v>
+        <v>5.8111237864799996</v>
       </c>
       <c r="C3">
         <v>6.2157421489999996</v>
@@ -1328,7 +1328,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>4.7704959599999999</v>
+        <v>2.1699001854500004</v>
       </c>
       <c r="C4">
         <v>5.1372892559999999</v>
@@ -1351,7 +1351,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>4.1261157599999994</v>
+        <v>2.76610243994</v>
       </c>
       <c r="C5">
         <v>4.5278082639999999</v>
@@ -1374,7 +1374,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>4.4671569299999998</v>
+        <v>3.3411156255500001</v>
       </c>
       <c r="C6">
         <v>3.9161057850000001</v>
@@ -1397,7 +1397,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>11.15485939</v>
+        <v>4.1484537600699998</v>
       </c>
       <c r="C7">
         <v>5.0694743799999999</v>
@@ -1420,7 +1420,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>45.991305799999999</v>
+        <v>12.5513977934</v>
       </c>
       <c r="C8">
         <v>4.7846876030000001</v>
@@ -1443,7 +1443,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>36.95099999</v>
+        <v>25.636687612000003</v>
       </c>
       <c r="C9">
         <v>17.916158677999999</v>
@@ -1466,7 +1466,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>15.646999970000001</v>
+        <v>12.923275837499999</v>
       </c>
       <c r="C10">
         <v>54.605494215</v>
@@ -1489,7 +1489,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>7.08704964</v>
+        <v>8.9502678131899991</v>
       </c>
       <c r="C11">
         <v>33.199219835000001</v>
@@ -1512,7 +1512,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>6.2172149699999997</v>
+        <v>5.2194004279500001</v>
       </c>
       <c r="C12">
         <v>15.906981818</v>
@@ -1535,7 +1535,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>6.72847931</v>
+        <v>4.4504380646000001</v>
       </c>
       <c r="C13">
         <v>7.6451504130000005</v>
@@ -1558,7 +1558,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>4.7024296999999997</v>
+        <v>3.9161435394000002</v>
       </c>
       <c r="C14">
         <v>7.6850578509999998</v>
@@ -1581,7 +1581,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>3.8798182000000003</v>
+        <v>3.1131471405000002</v>
       </c>
       <c r="C15">
         <v>6.6010512399999994</v>
@@ -1604,7 +1604,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>4.2182479800000001</v>
+        <v>3.6258501891999999</v>
       </c>
       <c r="C16">
         <v>7.0984462810000002</v>
@@ -1627,7 +1627,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>3.55025624</v>
+        <v>3.1648001709</v>
       </c>
       <c r="C17">
         <v>5.4367338840000006</v>
@@ -1650,7 +1650,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>4.3552479799999997</v>
+        <v>3.1958501891999997</v>
       </c>
       <c r="C18">
         <v>3.631775207</v>
@@ -1673,7 +1673,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>10.6979174</v>
+        <v>7.4521337433000001</v>
       </c>
       <c r="C19">
         <v>3.352264463</v>
@@ -1696,7 +1696,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>21.822223139999998</v>
+        <v>15.8195762024</v>
       </c>
       <c r="C20">
         <v>5.7545057850000001</v>
@@ -1719,7 +1719,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>35.094429720000001</v>
+        <v>38.8314094849</v>
       </c>
       <c r="C21">
         <v>47.944383471000002</v>
@@ -1742,7 +1742,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>9.6564710500000004</v>
+        <v>12.5039044495</v>
       </c>
       <c r="C22">
         <v>71.879087603000002</v>
@@ -1765,7 +1765,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>9.5899256000000008</v>
+        <v>5.5609594727000005</v>
       </c>
       <c r="C23">
         <v>42.633282645000001</v>
@@ -1788,7 +1788,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>6.3007272400000005</v>
+        <v>4.3801983469999994</v>
       </c>
       <c r="C24">
         <v>20.371557024999998</v>
@@ -1811,7 +1811,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>6.7167438499999994</v>
+        <v>6.3203186188</v>
       </c>
       <c r="C25">
         <v>11.676952066</v>
@@ -1834,7 +1834,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>4.7056032100000005</v>
+        <v>5.0160610961999996</v>
       </c>
       <c r="C26">
         <v>10.936978512</v>
@@ -1857,7 +1857,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>5.4317767899999998</v>
+        <v>3.8878501891999999</v>
       </c>
       <c r="C27">
         <v>7.32</v>
@@ -1880,7 +1880,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>4.6540743300000003</v>
+        <v>3.9968501891999999</v>
       </c>
       <c r="C28">
         <v>6.1669289259999998</v>
@@ -1903,7 +1903,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>3.9633635599999999</v>
+        <v>3.2408001709000001</v>
       </c>
       <c r="C29">
         <v>5.4657322309999996</v>
@@ -1926,7 +1926,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>4.6378759399999998</v>
+        <v>3.8808501891999998</v>
       </c>
       <c r="C30">
         <v>4.7108826449999999</v>
@@ -1949,7 +1949,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>7.4825371699999996</v>
+        <v>7.3539051970999996</v>
       </c>
       <c r="C31">
         <v>6.0535933880000004</v>
@@ -1972,7 +1972,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>21.78670249</v>
+        <v>25.400750488300002</v>
       </c>
       <c r="C32">
         <v>10.271464463000001</v>
@@ -1995,7 +1995,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>64.997586779999992</v>
+        <v>41.525772460900001</v>
       </c>
       <c r="C33">
         <v>40.584198346999997</v>
@@ -2018,7 +2018,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>36.56282642</v>
+        <v>16.1900247803</v>
       </c>
       <c r="C34">
         <v>58.168085949999998</v>
@@ -2041,7 +2041,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>11.36762813</v>
+        <v>7.7384530944999996</v>
       </c>
       <c r="C35">
         <v>23.878968595</v>
@@ -2064,7 +2064,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>7.1627272599999996</v>
+        <v>5.9147315062999999</v>
       </c>
       <c r="C36">
         <v>10.269421488000001</v>
@@ -2087,7 +2087,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>7.2987851799999994</v>
+        <v>3.9043111115000002</v>
       </c>
       <c r="C37">
         <v>9.2335735540000012</v>
@@ -2148,7 +2148,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>9.3044419999999999</v>
+        <v>11.8096</v>
       </c>
       <c r="C2">
         <v>19.320040000000002</v>
@@ -2171,7 +2171,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>5.281784</v>
+        <v>6.0536440000000002</v>
       </c>
       <c r="C3">
         <v>10.24516</v>
@@ -2194,7 +2194,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>4.825469</v>
+        <v>5.8738339999999996</v>
       </c>
       <c r="C4">
         <v>8.6558600000000006</v>
@@ -2217,7 +2217,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>5.4648789999999998</v>
+        <v>5.290241</v>
       </c>
       <c r="C5">
         <v>0.37124020000000002</v>
@@ -2240,7 +2240,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>5.2060529999999998</v>
+        <v>5.292859</v>
       </c>
       <c r="C6">
         <v>5.1253289999999998</v>
@@ -2263,7 +2263,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>8.5143039999999992</v>
+        <v>13.29707</v>
       </c>
       <c r="C7">
         <v>8.0487269999999995</v>
@@ -2286,7 +2286,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>21.721540000000001</v>
+        <v>41.68826</v>
       </c>
       <c r="C8">
         <v>11.393450000000001</v>
@@ -2309,7 +2309,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>98.217590000000001</v>
+        <v>58.142389999999999</v>
       </c>
       <c r="C9">
         <v>58.473639999999996</v>
@@ -2332,7 +2332,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>43.64761</v>
+        <v>34.141260000000003</v>
       </c>
       <c r="C10">
         <v>112.2482</v>
@@ -2355,7 +2355,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>19.205770000000001</v>
+        <v>14.47199</v>
       </c>
       <c r="C11">
         <v>47.462800000000001</v>
@@ -2378,7 +2378,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>7.8293670000000004</v>
+        <v>13.93252</v>
       </c>
       <c r="C12">
         <v>23.439990000000002</v>
@@ -2401,7 +2401,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>7.6047780000000005</v>
+        <v>6.2529489999999992</v>
       </c>
       <c r="C13">
         <v>11.152419999999999</v>
@@ -2424,7 +2424,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>8.1999610000000001</v>
+        <v>8.9992859999999997</v>
       </c>
       <c r="C14">
         <v>18.693860000000001</v>
@@ -2447,7 +2447,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>4.3675119999999996</v>
+        <v>3.9251499999999999</v>
       </c>
       <c r="C15">
         <v>7.3858509999999997</v>
@@ -2470,7 +2470,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>3.656628</v>
+        <v>2.6607270000000001</v>
       </c>
       <c r="C16">
         <v>7.3714120000000003</v>
@@ -2493,7 +2493,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>3.972585</v>
+        <v>2.772456</v>
       </c>
       <c r="C17">
         <v>6.1968399999999999</v>
@@ -2516,7 +2516,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>3.214861</v>
+        <v>2.4570250000000002</v>
       </c>
       <c r="C18">
         <v>5.32925</v>
@@ -2539,7 +2539,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>3.434898</v>
+        <v>4.1965290000000008</v>
       </c>
       <c r="C19">
         <v>7.4334150000000001</v>
@@ -2562,7 +2562,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>26.953779999999998</v>
+        <v>15.09423</v>
       </c>
       <c r="C20">
         <v>18.190549999999998</v>
@@ -2585,7 +2585,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>69.031059999999997</v>
+        <v>53.299800000000005</v>
       </c>
       <c r="C21">
         <v>100.81010000000001</v>
@@ -2608,7 +2608,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>45.965249999999997</v>
+        <v>73.172169999999994</v>
       </c>
       <c r="C22">
         <v>71.207369999999997</v>
@@ -2631,7 +2631,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>11.759360000000001</v>
+        <v>23.922999999999998</v>
       </c>
       <c r="C23">
         <v>35.676180000000002</v>
@@ -2654,7 +2654,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>18.859029999999997</v>
+        <v>13.41836</v>
       </c>
       <c r="C24">
         <v>24.032250000000001</v>
@@ -2677,7 +2677,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>10.256930000000001</v>
+        <v>17.082129999999999</v>
       </c>
       <c r="C25">
         <v>19.543779999999998</v>
@@ -2700,7 +2700,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>11.73377</v>
+        <v>21.42878</v>
       </c>
       <c r="C26">
         <v>23.183759999999999</v>
@@ -2723,7 +2723,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>6.5544650000000004</v>
+        <v>12.464549999999999</v>
       </c>
       <c r="C27">
         <v>11.256540000000001</v>
@@ -2746,7 +2746,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>6.1817020000000005</v>
+        <v>7.168927</v>
       </c>
       <c r="C28">
         <v>9.0916960000000007</v>
@@ -2769,7 +2769,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>4.8122990000000003</v>
+        <v>5.6124170000000007</v>
       </c>
       <c r="C29">
         <v>6.0569649999999999</v>
@@ -2792,7 +2792,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>4.1712449999999999</v>
+        <v>3.9631619999999996</v>
       </c>
       <c r="C30">
         <v>5.3950610000000001</v>
@@ -2815,7 +2815,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>7.3053590000000002</v>
+        <v>6.0090050000000002</v>
       </c>
       <c r="C31">
         <v>8.6311929999999997</v>
@@ -2838,7 +2838,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>21.617039999999999</v>
+        <v>22.758610000000001</v>
       </c>
       <c r="C32">
         <v>40.939120000000003</v>
@@ -2861,7 +2861,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>44.17848</v>
+        <v>65.197479999999999</v>
       </c>
       <c r="C33">
         <v>96.956450000000004</v>
@@ -2884,7 +2884,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>78.654049999999998</v>
+        <v>50.733220000000003</v>
       </c>
       <c r="C34">
         <v>127.67960000000001</v>
@@ -2907,7 +2907,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>23.105610000000002</v>
+        <v>14.986120000000001</v>
       </c>
       <c r="C35">
         <v>44.021080000000005</v>
@@ -2930,7 +2930,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>9.3066380000000013</v>
+        <v>10.19256</v>
       </c>
       <c r="C36">
         <v>17.965790000000002</v>
@@ -2953,7 +2953,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>7.5785809999999998</v>
+        <v>31.6144</v>
       </c>
       <c r="C37">
         <v>25.509799999999998</v>
@@ -3014,7 +3014,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>21.98479</v>
+        <v>17.2234767594</v>
       </c>
       <c r="C2">
         <v>56.132227000000007</v>
@@ -3037,7 +3037,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>26.602310000000003</v>
+        <v>17.963411431800001</v>
       </c>
       <c r="C3">
         <v>45.659489999999998</v>
@@ -3060,7 +3060,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>20.951400000000003</v>
+        <v>22.847759661000005</v>
       </c>
       <c r="C4">
         <v>31.687921000000003</v>
@@ -3083,7 +3083,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>26.901820000000001</v>
+        <v>15.4679653765</v>
       </c>
       <c r="C5">
         <v>28.363636000000003</v>
@@ -3106,7 +3106,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>35.928599999999996</v>
+        <v>13.5012335226</v>
       </c>
       <c r="C6">
         <v>37.527279999999998</v>
@@ -3129,7 +3129,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>76.345789999999994</v>
+        <v>81.137289331899993</v>
       </c>
       <c r="C7">
         <v>113.553713</v>
@@ -3152,7 +3152,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>259.79500000000002</v>
+        <v>198.439085318</v>
       </c>
       <c r="C8">
         <v>157.41221999999999</v>
@@ -3175,7 +3175,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>714.64459999999997</v>
+        <v>275.11685217600001</v>
       </c>
       <c r="C9">
         <v>584.80663000000004</v>
@@ -3198,7 +3198,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>517.05119999999999</v>
+        <v>181.04769779900002</v>
       </c>
       <c r="C10">
         <v>916.16519999999991</v>
@@ -3221,7 +3221,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>112.43899999999999</v>
+        <v>24.453508829100002</v>
       </c>
       <c r="C11">
         <v>362.142</v>
@@ -3244,7 +3244,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>20.45355</v>
+        <v>13.537740430400001</v>
       </c>
       <c r="C12">
         <v>85.918019000000001</v>
@@ -3267,7 +3267,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>13.908100000000001</v>
+        <v>6.7797935554900004</v>
       </c>
       <c r="C13">
         <v>26.419836</v>
@@ -3290,7 +3290,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>30.779499999999999</v>
+        <v>8.1857855999999991</v>
       </c>
       <c r="C14">
         <v>54.017840999999997</v>
@@ -3313,7 +3313,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>28.163310000000003</v>
+        <v>11.26215</v>
       </c>
       <c r="C15">
         <v>45.000989999999994</v>
@@ -3336,7 +3336,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>17.67868</v>
+        <v>14.5388419</v>
       </c>
       <c r="C16">
         <v>40.938848</v>
@@ -3359,7 +3359,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>15.675370000000001</v>
+        <v>14.915702700000001</v>
       </c>
       <c r="C17">
         <v>40.214873999999995</v>
@@ -3382,7 +3382,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>14.34446</v>
+        <v>18.690249200000004</v>
       </c>
       <c r="C18">
         <v>35.900840000000002</v>
@@ -3405,7 +3405,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>31.973549999999999</v>
+        <v>78.291584999999998</v>
       </c>
       <c r="C19">
         <v>55.735551000000001</v>
@@ -3428,7 +3428,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>198.47399999999999</v>
+        <v>158.10248999999999</v>
       </c>
       <c r="C20">
         <v>284.82645000000002</v>
@@ -3451,7 +3451,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>473.8116</v>
+        <v>191.84133000000003</v>
       </c>
       <c r="C21">
         <v>1127.1271400000001</v>
@@ -3474,7 +3474,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>612.25790000000006</v>
+        <v>299.64297000000005</v>
       </c>
       <c r="C22">
         <v>959.00819999999999</v>
@@ -3497,7 +3497,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>80.219499999999996</v>
+        <v>43.709752000000002</v>
       </c>
       <c r="C23">
         <v>318.68433999999996</v>
@@ -3520,7 +3520,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>25.72364</v>
+        <v>7.7057847000000006</v>
       </c>
       <c r="C24">
         <v>94.476685000000018</v>
@@ -3543,7 +3543,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>13.80298</v>
+        <v>7.5272730000000001</v>
       </c>
       <c r="C25">
         <v>55.207920000000001</v>
@@ -3566,7 +3566,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>26.753060000000001</v>
+        <v>20.052892499999999</v>
       </c>
       <c r="C26">
         <v>66.23602600000001</v>
@@ -3589,7 +3589,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>33.334209999999999</v>
+        <v>21.506778000000001</v>
       </c>
       <c r="C27">
         <v>63.250920000000001</v>
@@ -3612,7 +3612,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>28.65917</v>
+        <v>14.852230199999999</v>
       </c>
       <c r="C28">
         <v>51.153719999999993</v>
@@ -3635,7 +3635,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>29.95438</v>
+        <v>14.899833799999998</v>
       </c>
       <c r="C29">
         <v>39.966936000000004</v>
@@ -3658,7 +3658,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>27.459169999999997</v>
+        <v>15.104132400000001</v>
       </c>
       <c r="C30">
         <v>38.142160000000004</v>
@@ -3681,7 +3681,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>97.541160000000005</v>
+        <v>52.595716000000003</v>
       </c>
       <c r="C31">
         <v>121.64629400000001</v>
@@ -3704,7 +3704,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>326.26120000000003</v>
+        <v>120.31737000000001</v>
       </c>
       <c r="C32">
         <v>488.58840000000004</v>
@@ -3727,7 +3727,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>831.8678000000001</v>
+        <v>365.13722000000001</v>
       </c>
       <c r="C33">
         <v>810.6447300000001</v>
@@ -3750,7 +3750,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>1168.6610000000001</v>
+        <v>341.7321</v>
       </c>
       <c r="C34">
         <v>446.57850000000002</v>
@@ -3773,7 +3773,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>535.14049999999997</v>
+        <v>52.573892000000001</v>
       </c>
       <c r="C35">
         <v>103.52924299999999</v>
@@ -3796,7 +3796,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>67.438020000000009</v>
+        <v>25.7434726</v>
       </c>
       <c r="C36">
         <v>40.764287000000003</v>
@@ -3819,7 +3819,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>34.901160000000004</v>
+        <v>19.317024</v>
       </c>
       <c r="C37">
         <v>21.352065</v>
@@ -3880,7 +3880,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>33.035129999999995</v>
+        <v>25.65063</v>
       </c>
       <c r="C2">
         <v>52.643529999999998</v>
@@ -3903,7 +3903,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>27.419119999999999</v>
+        <v>25.848500000000001</v>
       </c>
       <c r="C3">
         <v>36.661449999999995</v>
@@ -3926,7 +3926,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>27.544640000000001</v>
+        <v>19.727689999999999</v>
       </c>
       <c r="C4">
         <v>27.399540000000002</v>
@@ -3949,7 +3949,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>26.41872</v>
+        <v>23.681330000000003</v>
       </c>
       <c r="C5">
         <v>27.065459999999998</v>
@@ -3972,7 +3972,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>23.512830000000001</v>
+        <v>21.779769999999999</v>
       </c>
       <c r="C6">
         <v>23.79964</v>
@@ -3995,7 +3995,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>39.590180000000004</v>
+        <v>42.286139999999996</v>
       </c>
       <c r="C7">
         <v>31.192679999999999</v>
@@ -4018,7 +4018,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>104.3032</v>
+        <v>97.546199999999999</v>
       </c>
       <c r="C8">
         <v>42.44979</v>
@@ -4041,7 +4041,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>343.60040000000004</v>
+        <v>139.4675</v>
       </c>
       <c r="C9">
         <v>167.9264</v>
@@ -4064,7 +4064,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>229.21860000000001</v>
+        <v>145.73420000000002</v>
       </c>
       <c r="C10">
         <v>442.96320000000003</v>
@@ -4087,7 +4087,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>95.147869999999998</v>
+        <v>59.89226</v>
       </c>
       <c r="C11">
         <v>238.18529999999998</v>
@@ -4110,7 +4110,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>41.65493</v>
+        <v>50.195550000000004</v>
       </c>
       <c r="C12">
         <v>113.9067</v>
@@ -4133,7 +4133,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>26.129630000000002</v>
+        <v>18.242060000000002</v>
       </c>
       <c r="C13">
         <v>41.228720000000003</v>
@@ -4156,7 +4156,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>32.706380000000003</v>
+        <v>25.446180000000002</v>
       </c>
       <c r="C14">
         <v>34.384010000000004</v>
@@ -4179,7 +4179,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>27.054479999999998</v>
+        <v>20.843250000000001</v>
       </c>
       <c r="C15">
         <v>31.637630000000001</v>
@@ -4202,7 +4202,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>20.68282</v>
+        <v>17.206790000000002</v>
       </c>
       <c r="C16">
         <v>34.850529999999999</v>
@@ -4225,7 +4225,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>22.10623</v>
+        <v>18.372479999999999</v>
       </c>
       <c r="C17">
         <v>29.029330000000002</v>
@@ -4248,7 +4248,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>21.535550000000001</v>
+        <v>15.768120000000001</v>
       </c>
       <c r="C18">
         <v>21.8188</v>
@@ -4271,7 +4271,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>28.69293</v>
+        <v>24.624470000000002</v>
       </c>
       <c r="C19">
         <v>23.558810000000001</v>
@@ -4294,7 +4294,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>96.121080000000006</v>
+        <v>38.664230000000003</v>
       </c>
       <c r="C20">
         <v>74.140799999999999</v>
@@ -4317,7 +4317,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>142.97889999999998</v>
+        <v>94.119309999999999</v>
       </c>
       <c r="C21">
         <v>569.19709999999998</v>
@@ -4340,7 +4340,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>204.64929999999998</v>
+        <v>181.04429999999999</v>
       </c>
       <c r="C22">
         <v>527.41669999999999</v>
@@ -4363,7 +4363,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>49.841059999999999</v>
+        <v>68.314869999999999</v>
       </c>
       <c r="C23">
         <v>262.25380000000001</v>
@@ -4386,7 +4386,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>55.565730000000002</v>
+        <v>38.767489999999995</v>
       </c>
       <c r="C24">
         <v>130.6918</v>
@@ -4409,7 +4409,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>23.139009999999999</v>
+        <v>25.374939999999999</v>
       </c>
       <c r="C25">
         <v>64.263419999999996</v>
@@ -4432,7 +4432,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>29.27262</v>
+        <v>40.062609999999999</v>
       </c>
       <c r="C26">
         <v>57.819780000000002</v>
@@ -4455,7 +4455,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>27.175540000000002</v>
+        <v>36.532849999999996</v>
       </c>
       <c r="C27">
         <v>41.806339999999999</v>
@@ -4478,7 +4478,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>30.098369999999999</v>
+        <v>23.919130000000003</v>
       </c>
       <c r="C28">
         <v>34.39472</v>
@@ -4501,7 +4501,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>23.10276</v>
+        <v>21.607330000000001</v>
       </c>
       <c r="C29">
         <v>29.158279999999998</v>
@@ -4524,7 +4524,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>20.771380000000001</v>
+        <v>19.958110000000001</v>
       </c>
       <c r="C30">
         <v>24.265139999999999</v>
@@ -4547,7 +4547,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>37.670580000000001</v>
+        <v>33.065460000000002</v>
       </c>
       <c r="C31">
         <v>39.716800000000006</v>
@@ -4570,7 +4570,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>77.025850000000005</v>
+        <v>71.596429999999998</v>
       </c>
       <c r="C32">
         <v>137.2192</v>
@@ -4593,7 +4593,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>168.19660000000002</v>
+        <v>198.84229999999999</v>
       </c>
       <c r="C33">
         <v>351.79079999999999</v>
@@ -4616,7 +4616,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>424.52859999999998</v>
+        <v>233.51589999999999</v>
       </c>
       <c r="C34">
         <v>402.8288</v>
@@ -4639,7 +4639,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>222.44759999999999</v>
+        <v>96.341719999999995</v>
       </c>
       <c r="C35">
         <v>148.87560000000002</v>
@@ -4662,7 +4662,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>66.526320000000013</v>
+        <v>49.2697</v>
       </c>
       <c r="C36">
         <v>64.618809999999996</v>
@@ -4685,7 +4685,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>34.968690000000002</v>
+        <v>29.47878</v>
       </c>
       <c r="C37">
         <v>47.620190000000001</v>
@@ -4746,7 +4746,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>36.322556129999995</v>
+        <v>39.394533629999998</v>
       </c>
       <c r="C2">
         <v>68.716436279999996</v>
@@ -4769,7 +4769,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>32.531920069999998</v>
+        <v>33.881778259999997</v>
       </c>
       <c r="C3">
         <v>43.518480710000006</v>
@@ -4792,7 +4792,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>32.453302029999996</v>
+        <v>27.669721450000001</v>
       </c>
       <c r="C4">
         <v>35.09828589</v>
@@ -4815,7 +4815,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>31.229511070000001</v>
+        <v>27.27724585</v>
       </c>
       <c r="C5">
         <v>34.04163672</v>
@@ -4838,7 +4838,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>27.60567781</v>
+        <v>25.65475696</v>
       </c>
       <c r="C6">
         <v>30.235136539999999</v>
@@ -4861,7 +4861,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>46.618863879999999</v>
+        <v>52.467886480000004</v>
       </c>
       <c r="C7">
         <v>41.592700440000002</v>
@@ -4884,7 +4884,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>130.48041370000001</v>
+        <v>123.1677864</v>
       </c>
       <c r="C8">
         <v>60.059090450000006</v>
@@ -4907,7 +4907,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>430.55565730000001</v>
+        <v>166.23262990000001</v>
       </c>
       <c r="C9">
         <v>249.09494649999999</v>
@@ -4930,7 +4930,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>263.97305949999998</v>
+        <v>162.82172750000001</v>
       </c>
       <c r="C10">
         <v>576.80068549999999</v>
@@ -4953,7 +4953,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>104.41407799999999</v>
+        <v>66.551131959999992</v>
       </c>
       <c r="C11">
         <v>297.2250659</v>
@@ -4976,7 +4976,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>44.116213809999998</v>
+        <v>58.545583860000001</v>
       </c>
       <c r="C12">
         <v>144.12701709999999</v>
@@ -4999,7 +4999,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>28.913753150000002</v>
+        <v>25.914385379999999</v>
       </c>
       <c r="C13">
         <v>52.694858399999994</v>
@@ -5022,7 +5022,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>36.468615589999999</v>
+        <v>36.869770629999998</v>
       </c>
       <c r="C14">
         <v>43.019139889999998</v>
@@ -5045,7 +5045,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>31.649318220000001</v>
+        <v>26.493841980000003</v>
       </c>
       <c r="C15">
         <v>42.015881960000002</v>
@@ -5068,7 +5068,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>24.774592550000001</v>
+        <v>22.3585213</v>
       </c>
       <c r="C16">
         <v>45.296903440000001</v>
@@ -5091,7 +5091,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>26.424043180000002</v>
+        <v>23.030349919999999</v>
       </c>
       <c r="C17">
         <v>39.872492800000003</v>
@@ -5114,7 +5114,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>24.97409459</v>
+        <v>20.91384274</v>
       </c>
       <c r="C18">
         <v>30.78035083</v>
@@ -5137,7 +5137,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>33.48866641</v>
+        <v>31.03302747</v>
       </c>
       <c r="C19">
         <v>42.671297120000006</v>
@@ -5160,7 +5160,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>118.3529451</v>
+        <v>50.721259519999997</v>
       </c>
       <c r="C20">
         <v>106.621708</v>
@@ -5183,7 +5183,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>178.81164920000001</v>
+        <v>113.5885339</v>
       </c>
       <c r="C21">
         <v>769.72709569999995</v>
@@ -5206,7 +5206,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>241.5292144</v>
+        <v>210.88209959999998</v>
       </c>
       <c r="C22">
         <v>662.80359279999993</v>
@@ -5229,7 +5229,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>54.629330770000003</v>
+        <v>80.177667360000001</v>
       </c>
       <c r="C23">
         <v>325.4162202</v>
@@ -5252,7 +5252,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>61.238290169999999</v>
+        <v>48.30885327</v>
       </c>
       <c r="C24">
         <v>157.17131099999997</v>
@@ -5275,7 +5275,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>26.38278781</v>
+        <v>35.13480878</v>
       </c>
       <c r="C25">
         <v>76.50550195000001</v>
@@ -5298,7 +5298,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>33.934077459999997</v>
+        <v>50.739999759999996</v>
       </c>
       <c r="C26">
         <v>72.042445189999995</v>
@@ -5321,7 +5321,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>32.211940409999997</v>
+        <v>40.74616657</v>
       </c>
       <c r="C27">
         <v>48.517599370000006</v>
@@ -5344,7 +5344,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>34.45440498</v>
+        <v>29.260138309999999</v>
       </c>
       <c r="C28">
         <v>42.934383909999994</v>
@@ -5367,7 +5367,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>27.11160799</v>
+        <v>27.96941739</v>
       </c>
       <c r="C29">
         <v>48.678900759999998</v>
@@ -5390,7 +5390,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>24.184437000000003</v>
+        <v>25.635685850000002</v>
       </c>
       <c r="C30">
         <v>41.501980959999997</v>
@@ -5413,7 +5413,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>43.179649380000001</v>
+        <v>41.571222470000002</v>
       </c>
       <c r="C31">
         <v>63.788940189999998</v>
@@ -5436,7 +5436,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>92.028328760000008</v>
+        <v>86.141379270000002</v>
       </c>
       <c r="C32">
         <v>189.85580300000001</v>
@@ -5459,7 +5459,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>204.12465830000002</v>
+        <v>273.29278149999999</v>
       </c>
       <c r="C33">
         <v>462.03587599999997</v>
@@ -5482,7 +5482,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>515.63994189999994</v>
+        <v>307.63734909999999</v>
       </c>
       <c r="C34">
         <v>514.38671190000002</v>
@@ -5505,7 +5505,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>254.64524789999999</v>
+        <v>120.152479</v>
       </c>
       <c r="C35">
         <v>175.12004639999998</v>
@@ -5528,7 +5528,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>74.684812390000005</v>
+        <v>68.633078740000002</v>
       </c>
       <c r="C36">
         <v>77.042593139999994</v>
@@ -5551,7 +5551,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>39.16562175</v>
+        <v>48.996869079999996</v>
       </c>
       <c r="C37">
         <v>59.260924070000002</v>
@@ -5612,7 +5612,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>45.426879999999997</v>
+        <v>20.33756</v>
       </c>
       <c r="C2">
         <v>169.04750000000001</v>
@@ -5635,7 +5635,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>46.549759999999999</v>
+        <v>18.924009999999999</v>
       </c>
       <c r="C3">
         <v>85.647600000000011</v>
@@ -5658,7 +5658,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>17.073979999999999</v>
+        <v>22.01257</v>
       </c>
       <c r="C4">
         <v>59.939</v>
@@ -5681,7 +5681,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>39.499480000000005</v>
+        <v>25.471310000000003</v>
       </c>
       <c r="C5">
         <v>61.521560000000001</v>
@@ -5704,7 +5704,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>37.161389999999997</v>
+        <v>28.280740000000002</v>
       </c>
       <c r="C6">
         <v>52.56156</v>
@@ -5727,7 +5727,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>62.122030000000002</v>
+        <v>104.3515</v>
       </c>
       <c r="C7">
         <v>136.8801</v>
@@ -5750,7 +5750,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>127.0534</v>
+        <v>95.365289999999987</v>
       </c>
       <c r="C8">
         <v>232.77549999999999</v>
@@ -5773,7 +5773,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>212.47489999999999</v>
+        <v>122.5091</v>
       </c>
       <c r="C9">
         <v>452.05059999999997</v>
@@ -5796,7 +5796,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>573.20490000000007</v>
+        <v>239.87779999999998</v>
       </c>
       <c r="C10">
         <v>975.82140000000004</v>
@@ -5819,7 +5819,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>284.25190000000003</v>
+        <v>153.726</v>
       </c>
       <c r="C11">
         <v>512.54129999999998</v>
@@ -5842,7 +5842,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>74.385220000000004</v>
+        <v>68.679179999999988</v>
       </c>
       <c r="C12">
         <v>247.72749999999999</v>
@@ -5865,7 +5865,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>44.572859999999999</v>
+        <v>53.122419999999998</v>
       </c>
       <c r="C13">
         <v>164.14679999999998</v>
@@ -5888,7 +5888,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>44.871190000000006</v>
+        <v>36.973910000000004</v>
       </c>
       <c r="C14">
         <v>140.1962</v>
@@ -5911,7 +5911,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>46.882949999999994</v>
+        <v>47.918039999999998</v>
       </c>
       <c r="C15">
         <v>112.52189999999999</v>
@@ -5934,7 +5934,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>18.9894</v>
+        <v>28.404400000000003</v>
       </c>
       <c r="C16">
         <v>90.910570000000007</v>
@@ -5957,7 +5957,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>26.94857</v>
+        <v>30.70806</v>
       </c>
       <c r="C17">
         <v>84.902289999999994</v>
@@ -5980,7 +5980,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>29.386700000000001</v>
+        <v>35.77704</v>
       </c>
       <c r="C18">
         <v>75.771539999999987</v>
@@ -6003,7 +6003,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>69.15146</v>
+        <v>76.180050000000008</v>
       </c>
       <c r="C19">
         <v>140.35050000000001</v>
@@ -6026,7 +6026,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>95.985590000000002</v>
+        <v>106.428</v>
       </c>
       <c r="C20">
         <v>235.99610000000001</v>
@@ -6049,7 +6049,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>71.561639999999997</v>
+        <v>92.201530000000005</v>
       </c>
       <c r="C21">
         <v>543.29669999999999</v>
@@ -6072,7 +6072,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>386.57259999999997</v>
+        <v>261.35309999999998</v>
       </c>
       <c r="C22">
         <v>530.226</v>
@@ -6095,7 +6095,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>151.19479999999999</v>
+        <v>162.10599999999999</v>
       </c>
       <c r="C23">
         <v>370.27909999999997</v>
@@ -6118,7 +6118,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>54.007649999999998</v>
+        <v>59.494690000000006</v>
       </c>
       <c r="C24">
         <v>203.21079999999998</v>
@@ -6141,7 +6141,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>22.137709999999998</v>
+        <v>48.890449999999994</v>
       </c>
       <c r="C25">
         <v>118.09389999999999</v>
@@ -6164,7 +6164,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>31.957459999999998</v>
+        <v>35.780739999999994</v>
       </c>
       <c r="C26">
         <v>118.96599999999999</v>
@@ -6187,7 +6187,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>31.30781</v>
+        <v>47.075410000000005</v>
       </c>
       <c r="C27">
         <v>85.920659999999998</v>
@@ -6210,7 +6210,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>45.255089999999996</v>
+        <v>22.76275</v>
       </c>
       <c r="C28">
         <v>52.190190000000001</v>
@@ -6233,7 +6233,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>44.032660000000007</v>
+        <v>38.115029999999997</v>
       </c>
       <c r="C29">
         <v>61.143730000000005</v>
@@ -6256,7 +6256,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>36.055030000000002</v>
+        <v>39.982610000000001</v>
       </c>
       <c r="C30">
         <v>51.260640000000002</v>
@@ -6279,7 +6279,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>98.493710000000007</v>
+        <v>67.268679999999989</v>
       </c>
       <c r="C31">
         <v>109.876</v>
@@ -6302,7 +6302,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>159.095</v>
+        <v>95.591649999999987</v>
       </c>
       <c r="C32">
         <v>286.45740000000001</v>
@@ -6325,7 +6325,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>327.1386</v>
+        <v>195.31210000000002</v>
       </c>
       <c r="C33">
         <v>312.86859999999996</v>
@@ -6348,7 +6348,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>667.42869999999994</v>
+        <v>506.25880000000001</v>
       </c>
       <c r="C34">
         <v>209.73729999999998</v>
@@ -6371,7 +6371,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>771.37139999999999</v>
+        <v>142.50779999999997</v>
       </c>
       <c r="C35">
         <v>127.7692</v>
@@ -6394,7 +6394,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>143.54910000000001</v>
+        <v>97.705389999999994</v>
       </c>
       <c r="C36">
         <v>48.783610000000003</v>
@@ -6417,7 +6417,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>58.462559999999996</v>
+        <v>67.803789999999992</v>
       </c>
       <c r="C37">
         <v>35.540120000000002</v>
@@ -6478,7 +6478,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>43.196289999999998</v>
+        <v>22.420480000000001</v>
       </c>
       <c r="C2">
         <v>129.3175</v>
@@ -6501,7 +6501,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>41.21613</v>
+        <v>27.626840000000001</v>
       </c>
       <c r="C3">
         <v>61.481319999999997</v>
@@ -6524,7 +6524,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>29.511770000000002</v>
+        <v>21.969429999999999</v>
       </c>
       <c r="C4">
         <v>46.940440000000002</v>
@@ -6547,7 +6547,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>32.60669</v>
+        <v>22.889669999999999</v>
       </c>
       <c r="C5">
         <v>42.761890000000001</v>
@@ -6570,7 +6570,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>26.535679999999999</v>
+        <v>21.369439999999997</v>
       </c>
       <c r="C6">
         <v>35.075029999999998</v>
@@ -6593,7 +6593,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>45.706510000000002</v>
+        <v>49.170929999999998</v>
       </c>
       <c r="C7">
         <v>63.06006</v>
@@ -6616,7 +6616,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>91.136210000000005</v>
+        <v>67.760249999999999</v>
       </c>
       <c r="C8">
         <v>115.89439999999999</v>
@@ -6639,7 +6639,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>151.50279999999998</v>
+        <v>95.74973</v>
       </c>
       <c r="C9">
         <v>236.249</v>
@@ -6662,7 +6662,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>477.39269999999999</v>
+        <v>214.14400000000001</v>
       </c>
       <c r="C10">
         <v>522.69079999999997</v>
@@ -6685,7 +6685,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>246.6935</v>
+        <v>140.72620000000001</v>
       </c>
       <c r="C11">
         <v>359.62729999999999</v>
@@ -6708,7 +6708,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>72.345020000000005</v>
+        <v>65.066850000000002</v>
       </c>
       <c r="C12">
         <v>160.2843</v>
@@ -6731,7 +6731,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>37.191839999999999</v>
+        <v>40.527670000000001</v>
       </c>
       <c r="C13">
         <v>103.8493</v>
@@ -6754,7 +6754,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>47.728470000000002</v>
+        <v>35.61412</v>
       </c>
       <c r="C14">
         <v>100.85239999999999</v>
@@ -6777,7 +6777,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>41.818959999999997</v>
+        <v>37.797260000000001</v>
       </c>
       <c r="C15">
         <v>70.01764</v>
@@ -6800,7 +6800,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>30.914249999999999</v>
+        <v>29.38804</v>
       </c>
       <c r="C16">
         <v>53.479800000000004</v>
@@ -6823,7 +6823,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>27.799490000000002</v>
+        <v>26.242159999999998</v>
       </c>
       <c r="C17">
         <v>49.335059999999999</v>
@@ -6846,7 +6846,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>23.234830000000002</v>
+        <v>24.344339999999999</v>
       </c>
       <c r="C18">
         <v>39.879429999999999</v>
@@ -6869,7 +6869,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>43.419849999999997</v>
+        <v>46.252989999999997</v>
       </c>
       <c r="C19">
         <v>50.260649999999998</v>
@@ -6892,7 +6892,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>63.075519999999997</v>
+        <v>82.989750000000001</v>
       </c>
       <c r="C20">
         <v>109.2385</v>
@@ -6915,7 +6915,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>39.881889999999999</v>
+        <v>69.752279999999999</v>
       </c>
       <c r="C21">
         <v>243.55610000000001</v>
@@ -6938,7 +6938,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>250.80410000000001</v>
+        <v>222.3032</v>
       </c>
       <c r="C22">
         <v>366.88909999999998</v>
@@ -6961,7 +6961,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>133.88159999999999</v>
+        <v>149.42760000000001</v>
       </c>
       <c r="C23">
         <v>290.44009999999997</v>
@@ -6984,7 +6984,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>49.610480000000003</v>
+        <v>61.891800000000003</v>
       </c>
       <c r="C24">
         <v>138.85929999999999</v>
@@ -7007,7 +7007,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>29.31719</v>
+        <v>43.094379999999994</v>
       </c>
       <c r="C25">
         <v>82.289500000000004</v>
@@ -7030,7 +7030,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>31.468630000000001</v>
+        <v>40.161819999999999</v>
       </c>
       <c r="C26">
         <v>92.795410000000004</v>
@@ -7053,7 +7053,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>33.573569999999997</v>
+        <v>42.30594</v>
       </c>
       <c r="C27">
         <v>63.582650000000001</v>
@@ -7076,7 +7076,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>37.065049999999999</v>
+        <v>28.482970000000002</v>
       </c>
       <c r="C28">
         <v>36.659469999999999</v>
@@ -7099,7 +7099,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>29.10821</v>
+        <v>25.85201</v>
       </c>
       <c r="C29">
         <v>39.5837</v>
@@ -7122,7 +7122,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>25.76014</v>
+        <v>22.516759999999998</v>
       </c>
       <c r="C30">
         <v>32.730879999999999</v>
@@ -7145,7 +7145,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>36.124809999999997</v>
+        <v>41.581009999999999</v>
       </c>
       <c r="C31">
         <v>47.732399999999998</v>
@@ -7168,7 +7168,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>92.39743</v>
+        <v>69.753950000000003</v>
       </c>
       <c r="C32">
         <v>160.1337</v>
@@ -7191,7 +7191,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>161.30760000000001</v>
+        <v>146.82640000000001</v>
       </c>
       <c r="C33">
         <v>231.12309999999999</v>
@@ -7214,7 +7214,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>428.9461</v>
+        <v>357.33640000000003</v>
       </c>
       <c r="C34">
         <v>174.53149999999999</v>
@@ -7237,7 +7237,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>538.71050000000002</v>
+        <v>120.5804</v>
       </c>
       <c r="C35">
         <v>110.0626</v>
@@ -7260,7 +7260,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>117.8977</v>
+        <v>70.49624</v>
       </c>
       <c r="C36">
         <v>57.69323</v>
@@ -7283,7 +7283,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>49.002549999999999</v>
+        <v>56.838370000000005</v>
       </c>
       <c r="C37">
         <v>45.54701</v>
@@ -7344,7 +7344,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>33.264849999999996</v>
+        <v>29.911240000000003</v>
       </c>
       <c r="C2">
         <v>57.626129999999996</v>
@@ -7367,7 +7367,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>28.98507</v>
+        <v>28.338819999999998</v>
       </c>
       <c r="C3">
         <v>38.787129999999998</v>
@@ -7390,7 +7390,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>29.286009999999997</v>
+        <v>22.189720000000001</v>
       </c>
       <c r="C4">
         <v>29.786150000000003</v>
@@ -7413,7 +7413,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>27.627790000000001</v>
+        <v>24.796060000000001</v>
       </c>
       <c r="C5">
         <v>29.228069999999999</v>
@@ -7436,7 +7436,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>24.27638</v>
+        <v>23.329759999999997</v>
       </c>
       <c r="C6">
         <v>26.373840000000001</v>
@@ -7459,7 +7459,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>41.54515</v>
+        <v>46.358839999999994</v>
       </c>
       <c r="C7">
         <v>35.352690000000003</v>
@@ -7482,7 +7482,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>118.7813</v>
+        <v>109.8446</v>
       </c>
       <c r="C8">
         <v>50.902250000000002</v>
@@ -7505,7 +7505,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>377.27440000000001</v>
+        <v>151.24420000000001</v>
       </c>
       <c r="C9">
         <v>203.64060000000001</v>
@@ -7528,7 +7528,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>241.3511</v>
+        <v>152.22749999999999</v>
       </c>
       <c r="C10">
         <v>493.82140000000004</v>
@@ -7551,7 +7551,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>97.09550999999999</v>
+        <v>61.956510000000002</v>
       </c>
       <c r="C11">
         <v>256.48759999999999</v>
@@ -7574,7 +7574,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>41.866639999999997</v>
+        <v>52.784059999999997</v>
       </c>
       <c r="C12">
         <v>123.27500000000001</v>
@@ -7597,7 +7597,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>26.781580000000002</v>
+        <v>20.620480000000001</v>
       </c>
       <c r="C13">
         <v>44.78322</v>
@@ -7620,7 +7620,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>33.801919999999996</v>
+        <v>28.987490000000001</v>
       </c>
       <c r="C14">
         <v>37.060900000000004</v>
@@ -7643,7 +7643,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>28.991619999999998</v>
+        <v>22.594930000000002</v>
       </c>
       <c r="C15">
         <v>34.854889999999997</v>
@@ -7666,7 +7666,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>21.518470000000001</v>
+        <v>18.803830000000001</v>
       </c>
       <c r="C16">
         <v>38.088900000000002</v>
@@ -7689,7 +7689,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>23.789740000000002</v>
+        <v>19.816419999999997</v>
       </c>
       <c r="C17">
         <v>32.390709999999999</v>
@@ -7712,7 +7712,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>22.046250000000001</v>
+        <v>17.826409999999999</v>
       </c>
       <c r="C18">
         <v>25.403419999999997</v>
@@ -7735,7 +7735,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>29.29373</v>
+        <v>27.187889999999999</v>
       </c>
       <c r="C19">
         <v>31.203799999999998</v>
@@ -7758,7 +7758,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>107.2529</v>
+        <v>44.451610000000002</v>
       </c>
       <c r="C20">
         <v>89.73163000000001</v>
@@ -7781,7 +7781,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>159.26560000000001</v>
+        <v>102.6858</v>
       </c>
       <c r="C21">
         <v>657.4303000000001</v>
@@ -7804,7 +7804,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>216.346</v>
+        <v>192.3827</v>
       </c>
       <c r="C22">
         <v>578.86369999999999</v>
@@ -7827,7 +7827,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>50.647750000000002</v>
+        <v>71.992339999999999</v>
       </c>
       <c r="C23">
         <v>281.83409999999998</v>
@@ -7850,7 +7850,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>56.374650000000003</v>
+        <v>41.72531</v>
       </c>
       <c r="C24">
         <v>138.90049999999999</v>
@@ -7873,7 +7873,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>23.42596</v>
+        <v>28.400500000000001</v>
       </c>
       <c r="C25">
         <v>68.058460000000011</v>
@@ -7896,7 +7896,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>30.310549999999999</v>
+        <v>43.372599999999998</v>
       </c>
       <c r="C26">
         <v>62.2288</v>
@@ -7919,7 +7919,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>28.612020000000001</v>
+        <v>37.838980000000006</v>
       </c>
       <c r="C27">
         <v>43.886830000000003</v>
@@ -7942,7 +7942,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>30.418849999999999</v>
+        <v>25.574840000000002</v>
       </c>
       <c r="C28">
         <v>37.042010000000005</v>
@@ -7965,7 +7965,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>23.34075</v>
+        <v>23.57958</v>
       </c>
       <c r="C29">
         <v>35.209669999999996</v>
@@ -7988,7 +7988,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>21.129650000000002</v>
+        <v>22.229140000000001</v>
       </c>
       <c r="C30">
         <v>31.159880000000001</v>
@@ -8011,7 +8011,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>38.304580000000001</v>
+        <v>36.467760000000006</v>
       </c>
       <c r="C31">
         <v>49.345660000000002</v>
@@ -8034,7 +8034,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>84.047240000000002</v>
+        <v>78.578009999999992</v>
       </c>
       <c r="C32">
         <v>162.48479999999998</v>
@@ -8057,7 +8057,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>190.79910000000001</v>
+        <v>231.60050000000001</v>
       </c>
       <c r="C33">
         <v>400.29859999999996</v>
@@ -8080,7 +8080,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>454.5951</v>
+        <v>261.68209999999999</v>
       </c>
       <c r="C34">
         <v>445.2208</v>
@@ -8103,7 +8103,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>231.29</v>
+        <v>103.7231</v>
       </c>
       <c r="C35">
         <v>157.01139999999998</v>
@@ -8126,7 +8126,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>67.72869</v>
+        <v>55.27234</v>
       </c>
       <c r="C36">
         <v>68.470179999999999</v>
@@ -8149,7 +8149,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>35.521650000000001</v>
+        <v>35.529389999999999</v>
       </c>
       <c r="C37">
         <v>51.228819999999999</v>
@@ -8210,7 +8210,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>28.075530000000001</v>
+        <v>17.748669999999997</v>
       </c>
       <c r="C2">
         <v>75.344719999999995</v>
@@ -8233,7 +8233,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>20.556630000000002</v>
+        <v>17.533480000000001</v>
       </c>
       <c r="C3">
         <v>46.063499999999998</v>
@@ -8256,7 +8256,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>19.40325</v>
+        <v>15.71598</v>
       </c>
       <c r="C4">
         <v>43.659769999999995</v>
@@ -8279,7 +8279,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>22.964470000000002</v>
+        <v>17.264040000000001</v>
       </c>
       <c r="C5">
         <v>1.0055529999999999</v>
@@ -8302,7 +8302,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>27.26962</v>
+        <v>27.449660000000002</v>
       </c>
       <c r="C6">
         <v>43.26229</v>
@@ -8325,7 +8325,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>75.354600000000005</v>
+        <v>137.28829999999999</v>
       </c>
       <c r="C7">
         <v>110.98339999999999</v>
@@ -8348,7 +8348,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>124.8117</v>
+        <v>191.40810000000002</v>
       </c>
       <c r="C8">
         <v>179.8477</v>
@@ -8371,7 +8371,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>361.28050000000002</v>
+        <v>169.8776</v>
       </c>
       <c r="C9">
         <v>314.64299999999997</v>
@@ -8394,7 +8394,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>145.63570000000001</v>
+        <v>93.102050000000006</v>
       </c>
       <c r="C10">
         <v>414.76890000000003</v>
@@ -8417,7 +8417,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>25.331319999999998</v>
+        <v>15.737129999999999</v>
       </c>
       <c r="C11">
         <v>168.04429999999999</v>
@@ -8440,7 +8440,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>-10.793700000000001</v>
+        <v>21.246419999999997</v>
       </c>
       <c r="C12">
         <v>60.047730000000001</v>
@@ -8463,7 +8463,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>4.9372189999999998</v>
+        <v>9.9849359999999994</v>
       </c>
       <c r="C13">
         <v>13.002139999999999</v>
@@ -8486,7 +8486,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>15.604950000000001</v>
+        <v>29.356729999999999</v>
       </c>
       <c r="C14">
         <v>64.497839999999997</v>
@@ -8509,7 +8509,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>14.753200000000001</v>
+        <v>9.9630299999999998</v>
       </c>
       <c r="C15">
         <v>25.684750000000001</v>
@@ -8532,7 +8532,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>12.055770000000001</v>
+        <v>6.9595209999999996</v>
       </c>
       <c r="C16">
         <v>30.688310000000001</v>
@@ -8555,7 +8555,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>14.267760000000001</v>
+        <v>8.9373619999999985</v>
       </c>
       <c r="C17">
         <v>29.408150000000003</v>
@@ -8578,7 +8578,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>16.630950000000002</v>
+        <v>10.98348</v>
       </c>
       <c r="C18">
         <v>35.651129999999995</v>
@@ -8601,7 +8601,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>63.868199999999995</v>
+        <v>28.956169999999997</v>
       </c>
       <c r="C19">
         <v>101.2761</v>
@@ -8624,7 +8624,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>221.53299999999999</v>
+        <v>90.381559999999993</v>
       </c>
       <c r="C20">
         <v>154.72929999999999</v>
@@ -8647,7 +8647,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>263.22909999999996</v>
+        <v>198.63129999999998</v>
       </c>
       <c r="C21">
         <v>426.0181</v>
@@ -8670,7 +8670,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>152.1164</v>
+        <v>196.8229</v>
       </c>
       <c r="C22">
         <v>228.25910000000002</v>
@@ -8693,7 +8693,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>15.59897</v>
+        <v>66.634539999999987</v>
       </c>
       <c r="C23">
         <v>56.936970000000002</v>
@@ -8716,7 +8716,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>39.041589999999999</v>
+        <v>35.160690000000002</v>
       </c>
       <c r="C24">
         <v>63.035440000000001</v>
@@ -8739,7 +8739,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>24.48169</v>
+        <v>40.31814</v>
       </c>
       <c r="C25">
         <v>43.810389999999998</v>
@@ -8762,7 +8762,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>24.75994</v>
+        <v>64.725560000000002</v>
       </c>
       <c r="C26">
         <v>87.143320000000003</v>
@@ -8785,7 +8785,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>17.483830000000001</v>
+        <v>42.68385</v>
       </c>
       <c r="C27">
         <v>49.978550000000006</v>
@@ -8808,7 +8808,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>23.759499999999999</v>
+        <v>24.70768</v>
       </c>
       <c r="C28">
         <v>51.539760000000001</v>
@@ -8831,7 +8831,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>16.03877</v>
+        <v>23.775389999999998</v>
       </c>
       <c r="C29">
         <v>33.395650000000003</v>
@@ -8854,7 +8854,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>17.47579</v>
+        <v>29.48254</v>
       </c>
       <c r="C30">
         <v>39.099059999999994</v>
@@ -8877,7 +8877,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>40.785249999999998</v>
+        <v>63.039199999999994</v>
       </c>
       <c r="C31">
         <v>189.46770000000001</v>
@@ -8900,7 +8900,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>114.4302</v>
+        <v>198.83429999999998</v>
       </c>
       <c r="C32">
         <v>391.90949999999998</v>
@@ -8923,7 +8923,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>171.7585</v>
+        <v>259.34410000000003</v>
       </c>
       <c r="C33">
         <v>462.69309999999996</v>
@@ -8946,7 +8946,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>252.03120000000001</v>
+        <v>187.26570000000001</v>
       </c>
       <c r="C34">
         <v>443.85129999999998</v>
@@ -8969,7 +8969,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>38.171289999999999</v>
+        <v>34.649099999999997</v>
       </c>
       <c r="C35">
         <v>117.72839999999999</v>
@@ -8992,7 +8992,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>2.2648580000000003</v>
+        <v>38.17568</v>
       </c>
       <c r="C36">
         <v>42.762740000000001</v>
@@ -9015,7 +9015,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>15.18966</v>
+        <v>83.770649999999989</v>
       </c>
       <c r="C37">
         <v>83.437619999999995</v>
@@ -9076,7 +9076,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>77.578000000000003</v>
+        <v>48.204999999999998</v>
       </c>
       <c r="C2">
         <v>85.269000000000005</v>
@@ -9099,7 +9099,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>47.341000000000001</v>
+        <v>34.927</v>
       </c>
       <c r="C3">
         <v>51.2</v>
@@ -9122,7 +9122,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>37.715000000000003</v>
+        <v>29.489000000000001</v>
       </c>
       <c r="C4">
         <v>49.487000000000002</v>
@@ -9145,7 +9145,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>36.314</v>
+        <v>33.975999999999999</v>
       </c>
       <c r="C5">
         <v>34.761000000000003</v>
@@ -9168,7 +9168,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>33.308</v>
+        <v>37.262999999999998</v>
       </c>
       <c r="C6">
         <v>35.189</v>
@@ -9191,7 +9191,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>51.215000000000003</v>
+        <v>61.067</v>
       </c>
       <c r="C7">
         <v>51.15</v>
@@ -9214,7 +9214,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>146.233</v>
+        <v>134.399</v>
       </c>
       <c r="C8">
         <v>104.712</v>
@@ -9237,7 +9237,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>338.74799999999999</v>
+        <v>111.255</v>
       </c>
       <c r="C9">
         <v>428.37900000000002</v>
@@ -9260,7 +9260,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>164.279</v>
+        <v>67.995000000000005</v>
       </c>
       <c r="C10">
         <v>573.36599999999999</v>
@@ -9283,7 +9283,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>58.875999999999998</v>
+        <v>23.109000000000002</v>
       </c>
       <c r="C11">
         <v>250.25200000000001</v>
@@ -9306,7 +9306,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>24.931999999999999</v>
+        <v>28.164000000000001</v>
       </c>
       <c r="C12">
         <v>86.494</v>
@@ -9329,7 +9329,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>59.713999999999999</v>
+        <v>41.506</v>
       </c>
       <c r="C13">
         <v>49.707000000000001</v>
@@ -9352,7 +9352,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>82.858999999999995</v>
+        <v>57.545000000000002</v>
       </c>
       <c r="C14">
         <v>74.402000000000001</v>
@@ -9375,7 +9375,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>54.338999999999999</v>
+        <v>39.061999999999998</v>
       </c>
       <c r="C15">
         <v>51.75</v>
@@ -9398,7 +9398,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>35.972000000000001</v>
+        <v>37.182000000000002</v>
       </c>
       <c r="C16">
         <v>55.29</v>
@@ -9421,7 +9421,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>32.731999999999999</v>
+        <v>28.965</v>
       </c>
       <c r="C17">
         <v>37.475999999999999</v>
@@ -9444,7 +9444,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>28.943000000000001</v>
+        <v>20.663</v>
       </c>
       <c r="C18">
         <v>39.938000000000002</v>
@@ -9467,7 +9467,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>39.411000000000001</v>
+        <v>29.103999999999999</v>
       </c>
       <c r="C19">
         <v>42.962000000000003</v>
@@ -9490,7 +9490,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>151.24600000000001</v>
+        <v>52.813000000000002</v>
       </c>
       <c r="C20">
         <v>124.867</v>
@@ -9513,7 +9513,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>207.923</v>
+        <v>87.227000000000004</v>
       </c>
       <c r="C21">
         <v>600.93600000000004</v>
@@ -9536,7 +9536,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>151.77000000000001</v>
+        <v>71.593999999999994</v>
       </c>
       <c r="C22">
         <v>437.95299999999997</v>
@@ -9559,7 +9559,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>35.487000000000002</v>
+        <v>25.241</v>
       </c>
       <c r="C23">
         <v>132.39500000000001</v>
@@ -9582,7 +9582,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>72.317999999999998</v>
+        <v>14.561999999999999</v>
       </c>
       <c r="C24">
         <v>77.998000000000005</v>
@@ -9605,7 +9605,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>52.844999999999999</v>
+        <v>50.073999999999998</v>
       </c>
       <c r="C25">
         <v>84.79</v>
@@ -9628,7 +9628,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>87.669289239999998</v>
+        <v>70.822000000000003</v>
       </c>
       <c r="C26">
         <v>103.297</v>
@@ -9651,7 +9651,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>60.285955039999997</v>
+        <v>38.637999999999998</v>
       </c>
       <c r="C27">
         <v>64.864000000000004</v>
@@ -9674,7 +9674,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>54.816706949999997</v>
+        <v>28.521999999999998</v>
       </c>
       <c r="C28">
         <v>58.972999999999999</v>
@@ -9697,7 +9697,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>39.502647119999999</v>
+        <v>23.189</v>
       </c>
       <c r="C29">
         <v>30.925000000000001</v>
@@ -9720,7 +9720,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>33.989246290000004</v>
+        <v>24.265999999999998</v>
       </c>
       <c r="C30">
         <v>31.488</v>
@@ -9743,7 +9743,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>47.730860100000001</v>
+        <v>31.861999999999998</v>
       </c>
       <c r="C31">
         <v>62.232999999999997</v>
@@ -9766,7 +9766,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>132.23944874</v>
+        <v>54.905000000000001</v>
       </c>
       <c r="C32">
         <v>291.58699999999999</v>
@@ -9789,7 +9789,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>296.94932231000001</v>
+        <v>190.47900000000001</v>
       </c>
       <c r="C33">
         <v>494.05599999999998</v>
@@ -9812,7 +9812,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>389.00474378999996</v>
+        <v>142.92699999999999</v>
       </c>
       <c r="C34">
         <v>228.32499999999999</v>
@@ -9835,7 +9835,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>148.29828099999997</v>
+        <v>43.594000000000001</v>
       </c>
       <c r="C35">
         <v>81.888000000000005</v>
@@ -9858,7 +9858,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>17.929669440000001</v>
+        <v>23.756</v>
       </c>
       <c r="C36">
         <v>27.384</v>
@@ -9881,7 +9881,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>52.12231405</v>
+        <v>45.13</v>
       </c>
       <c r="C37">
         <v>70.25</v>
@@ -9942,7 +9942,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>307.43097999999998</v>
+        <v>260.28469000000001</v>
       </c>
       <c r="C2">
         <v>846.84659999999997</v>
@@ -9965,7 +9965,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>379.22376000000003</v>
+        <v>272.4674</v>
       </c>
       <c r="C3">
         <v>667.49953000000005</v>
@@ -9988,7 +9988,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>296.30034999999998</v>
+        <v>246.49001000000001</v>
       </c>
       <c r="C4">
         <v>543.58793000000003</v>
@@ -10011,7 +10011,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>329.35734000000002</v>
+        <v>205.31920000000002</v>
       </c>
       <c r="C5">
         <v>449.51796999999999</v>
@@ -10034,7 +10034,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>323.24390999999997</v>
+        <v>330.68854999999996</v>
       </c>
       <c r="C6">
         <v>469.14665000000002</v>
@@ -10057,7 +10057,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>489.53684000000004</v>
+        <v>747.62995999999998</v>
       </c>
       <c r="C7">
         <v>1001.97183</v>
@@ -10080,7 +10080,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>838.50626</v>
+        <v>965.29324999999994</v>
       </c>
       <c r="C8">
         <v>1130.7236</v>
@@ -10103,7 +10103,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>3133.12817</v>
+        <v>1068.1749499999999</v>
       </c>
       <c r="C9">
         <v>3205.0938500000002</v>
@@ -10126,7 +10126,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>2616.1731099999997</v>
+        <v>1043.7099699999999</v>
       </c>
       <c r="C10">
         <v>6659.4755599999999</v>
@@ -10149,7 +10149,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>1127.9570900000001</v>
+        <v>335.76249999999999</v>
       </c>
       <c r="C11">
         <v>3547.5024199999998</v>
@@ -10172,7 +10172,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>192.81735999999998</v>
+        <v>339.38526999999999</v>
       </c>
       <c r="C12">
         <v>1287.8981999999999</v>
@@ -10195,7 +10195,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>185.90317999999999</v>
+        <v>124.22367999999999</v>
       </c>
       <c r="C13">
         <v>561.35106999999994</v>
@@ -10218,7 +10218,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>265.29784999999998</v>
+        <v>237.74179999999998</v>
       </c>
       <c r="C14">
         <v>716.36901</v>
@@ -10241,7 +10241,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>360.40429999999998</v>
+        <v>288.48759999999999</v>
       </c>
       <c r="C15">
         <v>595.52926000000002</v>
@@ -10264,7 +10264,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>217.14876000000001</v>
+        <v>247.55924999999999</v>
       </c>
       <c r="C16">
         <v>541.21950000000004</v>
@@ -10287,7 +10287,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>309.57371000000001</v>
+        <v>271.04752000000002</v>
       </c>
       <c r="C17">
         <v>397.41045000000003</v>
@@ -10310,7 +10310,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>322.50587000000002</v>
+        <v>204.91283999999999</v>
       </c>
       <c r="C18">
         <v>479.55982</v>
@@ -10333,7 +10333,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>535.82156999999995</v>
+        <v>377.20555000000002</v>
       </c>
       <c r="C19">
         <v>760.60487999999998</v>
@@ -10356,7 +10356,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>979.85526000000004</v>
+        <v>455.58172999999999</v>
       </c>
       <c r="C20">
         <v>1522.8559</v>
@@ -10379,7 +10379,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>1444.31674</v>
+        <v>708.49370999999996</v>
       </c>
       <c r="C21">
         <v>5429.2664100000002</v>
@@ -10402,7 +10402,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>2684.68804</v>
+        <v>1438.6799099999998</v>
       </c>
       <c r="C22">
         <v>5687.9918899999993</v>
@@ -10425,7 +10425,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>546.06851000000006</v>
+        <v>581.30113000000006</v>
       </c>
       <c r="C23">
         <v>2676.0059900000001</v>
@@ -10448,7 +10448,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>516.63591999999994</v>
+        <v>197.25624999999999</v>
       </c>
       <c r="C24">
         <v>1376.8901899999998</v>
@@ -10471,7 +10471,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>243.77939999999998</v>
+        <v>302.60960999999998</v>
       </c>
       <c r="C25">
         <v>661.97355000000005</v>
@@ -10494,7 +10494,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>437.51084000000003</v>
+        <v>454.74218999999999</v>
       </c>
       <c r="C26">
         <v>881.92110000000002</v>
@@ -10517,7 +10517,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>351.53346000000005</v>
+        <v>386.21096</v>
       </c>
       <c r="C27">
         <v>691.69087000000002</v>
@@ -10540,7 +10540,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>394.57535999999999</v>
+        <v>276.30721999999997</v>
       </c>
       <c r="C28">
         <v>540.37846000000002</v>
@@ -10563,7 +10563,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>259.45889</v>
+        <v>504.20076</v>
       </c>
       <c r="C29">
         <v>539.64705000000004</v>
@@ -10586,7 +10586,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>280.42408</v>
+        <v>493.39231000000001</v>
       </c>
       <c r="C30">
         <v>455.70453000000003</v>
@@ -10609,7 +10609,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>581.48798999999997</v>
+        <v>500.71429999999998</v>
       </c>
       <c r="C31">
         <v>1141.30573</v>
@@ -10632,7 +10632,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>1135.77216</v>
+        <v>749.45023000000003</v>
       </c>
       <c r="C32">
         <v>2707.6015400000001</v>
@@ -10655,7 +10655,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>2440.3492700000002</v>
+        <v>1550.6840199999999</v>
       </c>
       <c r="C33">
         <v>4366.7583399999994</v>
@@ -10678,7 +10678,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>5202.63087</v>
+        <v>2358.6873900000001</v>
       </c>
       <c r="C34">
         <v>3799.56016</v>
@@ -10701,7 +10701,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>3767.0521899999999</v>
+        <v>629.63194999999996</v>
       </c>
       <c r="C35">
         <v>1331.4722199999999</v>
@@ -10724,7 +10724,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>664.22307999999998</v>
+        <v>398.57389000000001</v>
       </c>
       <c r="C36">
         <v>553.74089000000004</v>
@@ -10747,7 +10747,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>456.39709999999997</v>
+        <v>498.08321999999998</v>
       </c>
       <c r="C37">
         <v>506.79510999999997</v>

</xml_diff>

<commit_message>
Rule edit: Mead Exclusive Flood Control Space
Thought this change was made in a previous commit, but didnt seem to take.... Edited execution constraint to check if FC slot was greater than 0 (not just Not NaN). This rule was setting Mead outflow during very low scenarios in which flood control rules should not be executing.
</commit_message>
<xml_diff>
--- a/Input Data/DevTesting/DevTesting_InflowsTEST.xlsx
+++ b/Input Data/DevTesting/DevTesting_InflowsTEST.xlsx
@@ -25,7 +25,7 @@
     <sheet name="VCRC2" sheetId="11" r:id="rId11"/>
     <sheet name="YDLC2" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -416,7 +416,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>19.441980000000001</v>
+        <v>15.79041</v>
       </c>
       <c r="C2">
         <v>29.924630000000001</v>
@@ -439,7 +439,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>13.76132</v>
+        <v>12.844959999999999</v>
       </c>
       <c r="C3">
         <v>17.456529999999997</v>
@@ -462,7 +462,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>13.449920000000001</v>
+        <v>11.424790000000002</v>
       </c>
       <c r="C4">
         <v>15.51074</v>
@@ -485,7 +485,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>12.900499999999999</v>
+        <v>11.26017</v>
       </c>
       <c r="C5">
         <v>13.77521</v>
@@ -508,7 +508,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>13.215870000000001</v>
+        <v>11.56165</v>
       </c>
       <c r="C6">
         <v>13.44595</v>
@@ -531,7 +531,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>36.56926</v>
+        <v>21.15372</v>
       </c>
       <c r="C7">
         <v>21.274709999999999</v>
@@ -554,7 +554,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>76.125619999999998</v>
+        <v>49.432070000000003</v>
       </c>
       <c r="C8">
         <v>38.318680000000001</v>
@@ -577,7 +577,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>104.5686</v>
+        <v>209.61320000000001</v>
       </c>
       <c r="C9">
         <v>142.84960000000001</v>
@@ -600,7 +600,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>75.929259999999999</v>
+        <v>103.21980000000001</v>
       </c>
       <c r="C10">
         <v>241.46779999999998</v>
@@ -623,7 +623,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>34.538179999999997</v>
+        <v>45.758679999999998</v>
       </c>
       <c r="C11">
         <v>139.16029999999998</v>
@@ -646,7 +646,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>30.251900000000003</v>
+        <v>14.51702</v>
       </c>
       <c r="C12">
         <v>56.11835</v>
@@ -669,7 +669,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>13.16033</v>
+        <v>12.69421</v>
       </c>
       <c r="C13">
         <v>22.746449999999999</v>
@@ -692,7 +692,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>15.98479</v>
+        <v>12.46017</v>
       </c>
       <c r="C14">
         <v>27.465119999999999</v>
@@ -715,7 +715,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>10.61157</v>
+        <v>10.10182</v>
       </c>
       <c r="C15">
         <v>15.675370000000001</v>
@@ -738,7 +738,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>7.9517359999999995</v>
+        <v>8.8879339999999996</v>
       </c>
       <c r="C16">
         <v>17.018180000000001</v>
@@ -761,7 +761,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>7.5173549999999993</v>
+        <v>9.778512000000001</v>
       </c>
       <c r="C17">
         <v>15.21917</v>
@@ -784,7 +784,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>7.4836360000000006</v>
+        <v>9.1398349999999997</v>
       </c>
       <c r="C18">
         <v>15.18942</v>
@@ -807,7 +807,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>8.2076029999999989</v>
+        <v>12.311399999999999</v>
       </c>
       <c r="C19">
         <v>22.08</v>
@@ -830,7 +830,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>21.365950000000002</v>
+        <v>51.094209999999997</v>
       </c>
       <c r="C20">
         <v>46.151400000000002</v>
@@ -853,7 +853,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>93.10611999999999</v>
+        <v>131.1848</v>
       </c>
       <c r="C21">
         <v>229.4281</v>
@@ -876,7 +876,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>130.05019999999999</v>
+        <v>114.3888</v>
       </c>
       <c r="C22">
         <v>176.8066</v>
@@ -899,7 +899,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>44.526940000000003</v>
+        <v>27.149750000000001</v>
       </c>
       <c r="C23">
         <v>103.69589999999999</v>
@@ -922,7 +922,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>24.902480000000001</v>
+        <v>35.162980000000005</v>
       </c>
       <c r="C24">
         <v>62.717359999999999</v>
@@ -945,7 +945,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>25.378509999999999</v>
+        <v>17.960330000000003</v>
       </c>
       <c r="C25">
         <v>35.688600000000001</v>
@@ -968,7 +968,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>39.286910000000006</v>
+        <v>16.989419999999999</v>
       </c>
       <c r="C26">
         <v>36.099170000000001</v>
@@ -991,7 +991,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>21.189060000000001</v>
+        <v>14.1243</v>
       </c>
       <c r="C27">
         <v>21.459169999999997</v>
@@ -1014,7 +1014,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>22.05152</v>
+        <v>13.76727</v>
       </c>
       <c r="C28">
         <v>16.532229999999998</v>
@@ -1037,7 +1037,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>16.454060000000002</v>
+        <v>11.406940000000001</v>
       </c>
       <c r="C29">
         <v>15.30843</v>
@@ -1060,7 +1060,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>12.43914</v>
+        <v>9.9629750000000001</v>
       </c>
       <c r="C30">
         <v>12.440329999999999</v>
@@ -1083,7 +1083,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>15.50592</v>
+        <v>15.859830000000001</v>
       </c>
       <c r="C31">
         <v>27.498840000000001</v>
@@ -1106,7 +1106,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>48.120040000000003</v>
+        <v>40.68694</v>
       </c>
       <c r="C32">
         <v>108.2043</v>
@@ -1129,7 +1129,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>126.32539999999999</v>
+        <v>90.614879999999999</v>
       </c>
       <c r="C33">
         <v>195.5504</v>
@@ -1152,7 +1152,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>125.53530000000001</v>
+        <v>217.3289</v>
       </c>
       <c r="C34">
         <v>253.01160000000002</v>
@@ -1175,7 +1175,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>44.607870000000005</v>
+        <v>83.498179999999991</v>
       </c>
       <c r="C35">
         <v>99.431399999999996</v>
@@ -1198,7 +1198,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>24.032049999999998</v>
+        <v>25.03537</v>
       </c>
       <c r="C36">
         <v>37.176199999999994</v>
@@ -1221,7 +1221,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>46.412550000000003</v>
+        <v>16.367599999999999</v>
       </c>
       <c r="C37">
         <v>42.928260000000002</v>
@@ -1282,7 +1282,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>4.5902854780700002</v>
+        <v>4.8311157300000005</v>
       </c>
       <c r="C2">
         <v>8.2923371899999996</v>
@@ -1305,7 +1305,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>5.8111237864799996</v>
+        <v>5.2234959600000002</v>
       </c>
       <c r="C3">
         <v>6.2157421489999996</v>
@@ -1328,7 +1328,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>2.1699001854500004</v>
+        <v>4.7704959599999999</v>
       </c>
       <c r="C4">
         <v>5.1372892559999999</v>
@@ -1351,7 +1351,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>2.76610243994</v>
+        <v>4.1261157599999994</v>
       </c>
       <c r="C5">
         <v>4.5278082639999999</v>
@@ -1374,7 +1374,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>3.3411156255500001</v>
+        <v>4.4671569299999998</v>
       </c>
       <c r="C6">
         <v>3.9161057850000001</v>
@@ -1397,7 +1397,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>4.1484537600699998</v>
+        <v>11.15485939</v>
       </c>
       <c r="C7">
         <v>5.0694743799999999</v>
@@ -1420,7 +1420,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>12.5513977934</v>
+        <v>45.991305799999999</v>
       </c>
       <c r="C8">
         <v>4.7846876030000001</v>
@@ -1443,7 +1443,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>25.636687612000003</v>
+        <v>36.95099999</v>
       </c>
       <c r="C9">
         <v>17.916158677999999</v>
@@ -1466,7 +1466,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>12.923275837499999</v>
+        <v>15.646999970000001</v>
       </c>
       <c r="C10">
         <v>54.605494215</v>
@@ -1489,7 +1489,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>8.9502678131899991</v>
+        <v>7.08704964</v>
       </c>
       <c r="C11">
         <v>33.199219835000001</v>
@@ -1512,7 +1512,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>5.2194004279500001</v>
+        <v>6.2172149699999997</v>
       </c>
       <c r="C12">
         <v>15.906981818</v>
@@ -1535,7 +1535,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>4.4504380646000001</v>
+        <v>6.72847931</v>
       </c>
       <c r="C13">
         <v>7.6451504130000005</v>
@@ -1558,7 +1558,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>3.9161435394000002</v>
+        <v>4.7024296999999997</v>
       </c>
       <c r="C14">
         <v>7.6850578509999998</v>
@@ -1581,7 +1581,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>3.1131471405000002</v>
+        <v>3.8798182000000003</v>
       </c>
       <c r="C15">
         <v>6.6010512399999994</v>
@@ -1604,7 +1604,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>3.6258501891999999</v>
+        <v>4.2182479800000001</v>
       </c>
       <c r="C16">
         <v>7.0984462810000002</v>
@@ -1627,7 +1627,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>3.1648001709</v>
+        <v>3.55025624</v>
       </c>
       <c r="C17">
         <v>5.4367338840000006</v>
@@ -1650,7 +1650,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>3.1958501891999997</v>
+        <v>4.3552479799999997</v>
       </c>
       <c r="C18">
         <v>3.631775207</v>
@@ -1673,7 +1673,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>7.4521337433000001</v>
+        <v>10.6979174</v>
       </c>
       <c r="C19">
         <v>3.352264463</v>
@@ -1696,7 +1696,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>15.8195762024</v>
+        <v>21.822223139999998</v>
       </c>
       <c r="C20">
         <v>5.7545057850000001</v>
@@ -1719,7 +1719,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>38.8314094849</v>
+        <v>35.094429720000001</v>
       </c>
       <c r="C21">
         <v>47.944383471000002</v>
@@ -1742,7 +1742,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>12.5039044495</v>
+        <v>9.6564710500000004</v>
       </c>
       <c r="C22">
         <v>71.879087603000002</v>
@@ -1765,7 +1765,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>5.5609594727000005</v>
+        <v>9.5899256000000008</v>
       </c>
       <c r="C23">
         <v>42.633282645000001</v>
@@ -1788,7 +1788,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>4.3801983469999994</v>
+        <v>6.3007272400000005</v>
       </c>
       <c r="C24">
         <v>20.371557024999998</v>
@@ -1811,7 +1811,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>6.3203186188</v>
+        <v>6.7167438499999994</v>
       </c>
       <c r="C25">
         <v>11.676952066</v>
@@ -1834,7 +1834,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>5.0160610961999996</v>
+        <v>4.7056032100000005</v>
       </c>
       <c r="C26">
         <v>10.936978512</v>
@@ -1857,7 +1857,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>3.8878501891999999</v>
+        <v>5.4317767899999998</v>
       </c>
       <c r="C27">
         <v>7.32</v>
@@ -1880,7 +1880,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>3.9968501891999999</v>
+        <v>4.6540743300000003</v>
       </c>
       <c r="C28">
         <v>6.1669289259999998</v>
@@ -1903,7 +1903,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>3.2408001709000001</v>
+        <v>3.9633635599999999</v>
       </c>
       <c r="C29">
         <v>5.4657322309999996</v>
@@ -1926,7 +1926,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>3.8808501891999998</v>
+        <v>4.6378759399999998</v>
       </c>
       <c r="C30">
         <v>4.7108826449999999</v>
@@ -1949,7 +1949,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>7.3539051970999996</v>
+        <v>7.4825371699999996</v>
       </c>
       <c r="C31">
         <v>6.0535933880000004</v>
@@ -1972,7 +1972,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>25.400750488300002</v>
+        <v>21.78670249</v>
       </c>
       <c r="C32">
         <v>10.271464463000001</v>
@@ -1995,7 +1995,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>41.525772460900001</v>
+        <v>64.997586779999992</v>
       </c>
       <c r="C33">
         <v>40.584198346999997</v>
@@ -2018,7 +2018,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>16.1900247803</v>
+        <v>36.56282642</v>
       </c>
       <c r="C34">
         <v>58.168085949999998</v>
@@ -2041,7 +2041,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>7.7384530944999996</v>
+        <v>11.36762813</v>
       </c>
       <c r="C35">
         <v>23.878968595</v>
@@ -2064,7 +2064,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>5.9147315062999999</v>
+        <v>7.1627272599999996</v>
       </c>
       <c r="C36">
         <v>10.269421488000001</v>
@@ -2087,7 +2087,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>3.9043111115000002</v>
+        <v>7.2987851799999994</v>
       </c>
       <c r="C37">
         <v>9.2335735540000012</v>
@@ -2148,7 +2148,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>11.8096</v>
+        <v>9.3044419999999999</v>
       </c>
       <c r="C2">
         <v>19.320040000000002</v>
@@ -2171,7 +2171,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>6.0536440000000002</v>
+        <v>5.281784</v>
       </c>
       <c r="C3">
         <v>10.24516</v>
@@ -2194,7 +2194,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>5.8738339999999996</v>
+        <v>4.825469</v>
       </c>
       <c r="C4">
         <v>8.6558600000000006</v>
@@ -2217,7 +2217,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>5.290241</v>
+        <v>5.4648789999999998</v>
       </c>
       <c r="C5">
         <v>0.37124020000000002</v>
@@ -2240,7 +2240,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>5.292859</v>
+        <v>5.2060529999999998</v>
       </c>
       <c r="C6">
         <v>5.1253289999999998</v>
@@ -2263,7 +2263,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>13.29707</v>
+        <v>8.5143039999999992</v>
       </c>
       <c r="C7">
         <v>8.0487269999999995</v>
@@ -2286,7 +2286,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>41.68826</v>
+        <v>21.721540000000001</v>
       </c>
       <c r="C8">
         <v>11.393450000000001</v>
@@ -2309,7 +2309,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>58.142389999999999</v>
+        <v>98.217590000000001</v>
       </c>
       <c r="C9">
         <v>58.473639999999996</v>
@@ -2332,7 +2332,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>34.141260000000003</v>
+        <v>43.64761</v>
       </c>
       <c r="C10">
         <v>112.2482</v>
@@ -2355,7 +2355,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>14.47199</v>
+        <v>19.205770000000001</v>
       </c>
       <c r="C11">
         <v>47.462800000000001</v>
@@ -2378,7 +2378,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>13.93252</v>
+        <v>7.8293670000000004</v>
       </c>
       <c r="C12">
         <v>23.439990000000002</v>
@@ -2401,7 +2401,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>6.2529489999999992</v>
+        <v>7.6047780000000005</v>
       </c>
       <c r="C13">
         <v>11.152419999999999</v>
@@ -2424,7 +2424,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>8.9992859999999997</v>
+        <v>8.1999610000000001</v>
       </c>
       <c r="C14">
         <v>18.693860000000001</v>
@@ -2447,7 +2447,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>3.9251499999999999</v>
+        <v>4.3675119999999996</v>
       </c>
       <c r="C15">
         <v>7.3858509999999997</v>
@@ -2470,7 +2470,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>2.6607270000000001</v>
+        <v>3.656628</v>
       </c>
       <c r="C16">
         <v>7.3714120000000003</v>
@@ -2493,7 +2493,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>2.772456</v>
+        <v>3.972585</v>
       </c>
       <c r="C17">
         <v>6.1968399999999999</v>
@@ -2516,7 +2516,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>2.4570250000000002</v>
+        <v>3.214861</v>
       </c>
       <c r="C18">
         <v>5.32925</v>
@@ -2539,7 +2539,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>4.1965290000000008</v>
+        <v>3.434898</v>
       </c>
       <c r="C19">
         <v>7.4334150000000001</v>
@@ -2562,7 +2562,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>15.09423</v>
+        <v>26.953779999999998</v>
       </c>
       <c r="C20">
         <v>18.190549999999998</v>
@@ -2585,7 +2585,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>53.299800000000005</v>
+        <v>69.031059999999997</v>
       </c>
       <c r="C21">
         <v>100.81010000000001</v>
@@ -2608,7 +2608,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>73.172169999999994</v>
+        <v>45.965249999999997</v>
       </c>
       <c r="C22">
         <v>71.207369999999997</v>
@@ -2631,7 +2631,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>23.922999999999998</v>
+        <v>11.759360000000001</v>
       </c>
       <c r="C23">
         <v>35.676180000000002</v>
@@ -2654,7 +2654,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>13.41836</v>
+        <v>18.859029999999997</v>
       </c>
       <c r="C24">
         <v>24.032250000000001</v>
@@ -2677,7 +2677,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>17.082129999999999</v>
+        <v>10.256930000000001</v>
       </c>
       <c r="C25">
         <v>19.543779999999998</v>
@@ -2700,7 +2700,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>21.42878</v>
+        <v>11.73377</v>
       </c>
       <c r="C26">
         <v>23.183759999999999</v>
@@ -2723,7 +2723,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>12.464549999999999</v>
+        <v>6.5544650000000004</v>
       </c>
       <c r="C27">
         <v>11.256540000000001</v>
@@ -2746,7 +2746,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>7.168927</v>
+        <v>6.1817020000000005</v>
       </c>
       <c r="C28">
         <v>9.0916960000000007</v>
@@ -2769,7 +2769,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>5.6124170000000007</v>
+        <v>4.8122990000000003</v>
       </c>
       <c r="C29">
         <v>6.0569649999999999</v>
@@ -2792,7 +2792,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>3.9631619999999996</v>
+        <v>4.1712449999999999</v>
       </c>
       <c r="C30">
         <v>5.3950610000000001</v>
@@ -2815,7 +2815,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>6.0090050000000002</v>
+        <v>7.3053590000000002</v>
       </c>
       <c r="C31">
         <v>8.6311929999999997</v>
@@ -2838,7 +2838,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>22.758610000000001</v>
+        <v>21.617039999999999</v>
       </c>
       <c r="C32">
         <v>40.939120000000003</v>
@@ -2861,7 +2861,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>65.197479999999999</v>
+        <v>44.17848</v>
       </c>
       <c r="C33">
         <v>96.956450000000004</v>
@@ -2884,7 +2884,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>50.733220000000003</v>
+        <v>78.654049999999998</v>
       </c>
       <c r="C34">
         <v>127.67960000000001</v>
@@ -2907,7 +2907,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>14.986120000000001</v>
+        <v>23.105610000000002</v>
       </c>
       <c r="C35">
         <v>44.021080000000005</v>
@@ -2930,7 +2930,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>10.19256</v>
+        <v>9.3066380000000013</v>
       </c>
       <c r="C36">
         <v>17.965790000000002</v>
@@ -2953,7 +2953,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>31.6144</v>
+        <v>7.5785809999999998</v>
       </c>
       <c r="C37">
         <v>25.509799999999998</v>
@@ -3014,7 +3014,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>17.2234767594</v>
+        <v>21.98479</v>
       </c>
       <c r="C2">
         <v>56.132227000000007</v>
@@ -3037,7 +3037,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>17.963411431800001</v>
+        <v>26.602310000000003</v>
       </c>
       <c r="C3">
         <v>45.659489999999998</v>
@@ -3060,7 +3060,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>22.847759661000005</v>
+        <v>20.951400000000003</v>
       </c>
       <c r="C4">
         <v>31.687921000000003</v>
@@ -3083,7 +3083,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>15.4679653765</v>
+        <v>26.901820000000001</v>
       </c>
       <c r="C5">
         <v>28.363636000000003</v>
@@ -3106,7 +3106,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>13.5012335226</v>
+        <v>35.928599999999996</v>
       </c>
       <c r="C6">
         <v>37.527279999999998</v>
@@ -3129,7 +3129,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>81.137289331899993</v>
+        <v>76.345789999999994</v>
       </c>
       <c r="C7">
         <v>113.553713</v>
@@ -3152,7 +3152,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>198.439085318</v>
+        <v>259.79500000000002</v>
       </c>
       <c r="C8">
         <v>157.41221999999999</v>
@@ -3175,7 +3175,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>275.11685217600001</v>
+        <v>714.64459999999997</v>
       </c>
       <c r="C9">
         <v>584.80663000000004</v>
@@ -3198,7 +3198,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>181.04769779900002</v>
+        <v>517.05119999999999</v>
       </c>
       <c r="C10">
         <v>916.16519999999991</v>
@@ -3221,7 +3221,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>24.453508829100002</v>
+        <v>112.43899999999999</v>
       </c>
       <c r="C11">
         <v>362.142</v>
@@ -3244,7 +3244,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>13.537740430400001</v>
+        <v>20.45355</v>
       </c>
       <c r="C12">
         <v>85.918019000000001</v>
@@ -3267,7 +3267,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>6.7797935554900004</v>
+        <v>13.908100000000001</v>
       </c>
       <c r="C13">
         <v>26.419836</v>
@@ -3290,7 +3290,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>8.1857855999999991</v>
+        <v>30.779499999999999</v>
       </c>
       <c r="C14">
         <v>54.017840999999997</v>
@@ -3313,7 +3313,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>11.26215</v>
+        <v>28.163310000000003</v>
       </c>
       <c r="C15">
         <v>45.000989999999994</v>
@@ -3336,7 +3336,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>14.5388419</v>
+        <v>17.67868</v>
       </c>
       <c r="C16">
         <v>40.938848</v>
@@ -3359,7 +3359,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>14.915702700000001</v>
+        <v>15.675370000000001</v>
       </c>
       <c r="C17">
         <v>40.214873999999995</v>
@@ -3382,7 +3382,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>18.690249200000004</v>
+        <v>14.34446</v>
       </c>
       <c r="C18">
         <v>35.900840000000002</v>
@@ -3405,7 +3405,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>78.291584999999998</v>
+        <v>31.973549999999999</v>
       </c>
       <c r="C19">
         <v>55.735551000000001</v>
@@ -3428,7 +3428,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>158.10248999999999</v>
+        <v>198.47399999999999</v>
       </c>
       <c r="C20">
         <v>284.82645000000002</v>
@@ -3451,7 +3451,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>191.84133000000003</v>
+        <v>473.8116</v>
       </c>
       <c r="C21">
         <v>1127.1271400000001</v>
@@ -3474,7 +3474,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>299.64297000000005</v>
+        <v>612.25790000000006</v>
       </c>
       <c r="C22">
         <v>959.00819999999999</v>
@@ -3497,7 +3497,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>43.709752000000002</v>
+        <v>80.219499999999996</v>
       </c>
       <c r="C23">
         <v>318.68433999999996</v>
@@ -3520,7 +3520,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>7.7057847000000006</v>
+        <v>25.72364</v>
       </c>
       <c r="C24">
         <v>94.476685000000018</v>
@@ -3543,7 +3543,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>7.5272730000000001</v>
+        <v>13.80298</v>
       </c>
       <c r="C25">
         <v>55.207920000000001</v>
@@ -3566,7 +3566,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>20.052892499999999</v>
+        <v>26.753060000000001</v>
       </c>
       <c r="C26">
         <v>66.23602600000001</v>
@@ -3589,7 +3589,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>21.506778000000001</v>
+        <v>33.334209999999999</v>
       </c>
       <c r="C27">
         <v>63.250920000000001</v>
@@ -3612,7 +3612,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>14.852230199999999</v>
+        <v>28.65917</v>
       </c>
       <c r="C28">
         <v>51.153719999999993</v>
@@ -3635,7 +3635,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>14.899833799999998</v>
+        <v>29.95438</v>
       </c>
       <c r="C29">
         <v>39.966936000000004</v>
@@ -3658,7 +3658,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>15.104132400000001</v>
+        <v>27.459169999999997</v>
       </c>
       <c r="C30">
         <v>38.142160000000004</v>
@@ -3681,7 +3681,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>52.595716000000003</v>
+        <v>97.541160000000005</v>
       </c>
       <c r="C31">
         <v>121.64629400000001</v>
@@ -3704,7 +3704,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>120.31737000000001</v>
+        <v>326.26120000000003</v>
       </c>
       <c r="C32">
         <v>488.58840000000004</v>
@@ -3727,7 +3727,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>365.13722000000001</v>
+        <v>831.8678000000001</v>
       </c>
       <c r="C33">
         <v>810.6447300000001</v>
@@ -3750,7 +3750,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>341.7321</v>
+        <v>1168.6610000000001</v>
       </c>
       <c r="C34">
         <v>446.57850000000002</v>
@@ -3773,7 +3773,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>52.573892000000001</v>
+        <v>535.14049999999997</v>
       </c>
       <c r="C35">
         <v>103.52924299999999</v>
@@ -3796,7 +3796,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>25.7434726</v>
+        <v>67.438020000000009</v>
       </c>
       <c r="C36">
         <v>40.764287000000003</v>
@@ -3819,7 +3819,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>19.317024</v>
+        <v>34.901160000000004</v>
       </c>
       <c r="C37">
         <v>21.352065</v>
@@ -3880,7 +3880,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>25.65063</v>
+        <v>33.035129999999995</v>
       </c>
       <c r="C2">
         <v>52.643529999999998</v>
@@ -3903,7 +3903,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>25.848500000000001</v>
+        <v>27.419119999999999</v>
       </c>
       <c r="C3">
         <v>36.661449999999995</v>
@@ -3926,7 +3926,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>19.727689999999999</v>
+        <v>27.544640000000001</v>
       </c>
       <c r="C4">
         <v>27.399540000000002</v>
@@ -3949,7 +3949,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>23.681330000000003</v>
+        <v>26.41872</v>
       </c>
       <c r="C5">
         <v>27.065459999999998</v>
@@ -3972,7 +3972,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>21.779769999999999</v>
+        <v>23.512830000000001</v>
       </c>
       <c r="C6">
         <v>23.79964</v>
@@ -3995,7 +3995,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>42.286139999999996</v>
+        <v>39.590180000000004</v>
       </c>
       <c r="C7">
         <v>31.192679999999999</v>
@@ -4018,7 +4018,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>97.546199999999999</v>
+        <v>104.3032</v>
       </c>
       <c r="C8">
         <v>42.44979</v>
@@ -4041,7 +4041,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>139.4675</v>
+        <v>343.60040000000004</v>
       </c>
       <c r="C9">
         <v>167.9264</v>
@@ -4064,7 +4064,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>145.73420000000002</v>
+        <v>229.21860000000001</v>
       </c>
       <c r="C10">
         <v>442.96320000000003</v>
@@ -4087,7 +4087,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>59.89226</v>
+        <v>95.147869999999998</v>
       </c>
       <c r="C11">
         <v>238.18529999999998</v>
@@ -4110,7 +4110,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>50.195550000000004</v>
+        <v>41.65493</v>
       </c>
       <c r="C12">
         <v>113.9067</v>
@@ -4133,7 +4133,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>18.242060000000002</v>
+        <v>26.129630000000002</v>
       </c>
       <c r="C13">
         <v>41.228720000000003</v>
@@ -4156,7 +4156,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>25.446180000000002</v>
+        <v>32.706380000000003</v>
       </c>
       <c r="C14">
         <v>34.384010000000004</v>
@@ -4179,7 +4179,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>20.843250000000001</v>
+        <v>27.054479999999998</v>
       </c>
       <c r="C15">
         <v>31.637630000000001</v>
@@ -4202,7 +4202,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>17.206790000000002</v>
+        <v>20.68282</v>
       </c>
       <c r="C16">
         <v>34.850529999999999</v>
@@ -4225,7 +4225,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>18.372479999999999</v>
+        <v>22.10623</v>
       </c>
       <c r="C17">
         <v>29.029330000000002</v>
@@ -4248,7 +4248,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>15.768120000000001</v>
+        <v>21.535550000000001</v>
       </c>
       <c r="C18">
         <v>21.8188</v>
@@ -4271,7 +4271,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>24.624470000000002</v>
+        <v>28.69293</v>
       </c>
       <c r="C19">
         <v>23.558810000000001</v>
@@ -4294,7 +4294,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>38.664230000000003</v>
+        <v>96.121080000000006</v>
       </c>
       <c r="C20">
         <v>74.140799999999999</v>
@@ -4317,7 +4317,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>94.119309999999999</v>
+        <v>142.97889999999998</v>
       </c>
       <c r="C21">
         <v>569.19709999999998</v>
@@ -4340,7 +4340,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>181.04429999999999</v>
+        <v>204.64929999999998</v>
       </c>
       <c r="C22">
         <v>527.41669999999999</v>
@@ -4363,7 +4363,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>68.314869999999999</v>
+        <v>49.841059999999999</v>
       </c>
       <c r="C23">
         <v>262.25380000000001</v>
@@ -4386,7 +4386,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>38.767489999999995</v>
+        <v>55.565730000000002</v>
       </c>
       <c r="C24">
         <v>130.6918</v>
@@ -4409,7 +4409,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>25.374939999999999</v>
+        <v>23.139009999999999</v>
       </c>
       <c r="C25">
         <v>64.263419999999996</v>
@@ -4432,7 +4432,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>40.062609999999999</v>
+        <v>29.27262</v>
       </c>
       <c r="C26">
         <v>57.819780000000002</v>
@@ -4455,7 +4455,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>36.532849999999996</v>
+        <v>27.175540000000002</v>
       </c>
       <c r="C27">
         <v>41.806339999999999</v>
@@ -4478,7 +4478,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>23.919130000000003</v>
+        <v>30.098369999999999</v>
       </c>
       <c r="C28">
         <v>34.39472</v>
@@ -4501,7 +4501,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>21.607330000000001</v>
+        <v>23.10276</v>
       </c>
       <c r="C29">
         <v>29.158279999999998</v>
@@ -4524,7 +4524,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>19.958110000000001</v>
+        <v>20.771380000000001</v>
       </c>
       <c r="C30">
         <v>24.265139999999999</v>
@@ -4547,7 +4547,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>33.065460000000002</v>
+        <v>37.670580000000001</v>
       </c>
       <c r="C31">
         <v>39.716800000000006</v>
@@ -4570,7 +4570,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>71.596429999999998</v>
+        <v>77.025850000000005</v>
       </c>
       <c r="C32">
         <v>137.2192</v>
@@ -4593,7 +4593,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>198.84229999999999</v>
+        <v>168.19660000000002</v>
       </c>
       <c r="C33">
         <v>351.79079999999999</v>
@@ -4616,7 +4616,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>233.51589999999999</v>
+        <v>424.52859999999998</v>
       </c>
       <c r="C34">
         <v>402.8288</v>
@@ -4639,7 +4639,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>96.341719999999995</v>
+        <v>222.44759999999999</v>
       </c>
       <c r="C35">
         <v>148.87560000000002</v>
@@ -4662,7 +4662,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>49.2697</v>
+        <v>66.526320000000013</v>
       </c>
       <c r="C36">
         <v>64.618809999999996</v>
@@ -4685,7 +4685,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>29.47878</v>
+        <v>34.968690000000002</v>
       </c>
       <c r="C37">
         <v>47.620190000000001</v>
@@ -4746,7 +4746,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>39.394533629999998</v>
+        <v>36.322556129999995</v>
       </c>
       <c r="C2">
         <v>68.716436279999996</v>
@@ -4769,7 +4769,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>33.881778259999997</v>
+        <v>32.531920069999998</v>
       </c>
       <c r="C3">
         <v>43.518480710000006</v>
@@ -4792,7 +4792,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>27.669721450000001</v>
+        <v>32.453302029999996</v>
       </c>
       <c r="C4">
         <v>35.09828589</v>
@@ -4815,7 +4815,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>27.27724585</v>
+        <v>31.229511070000001</v>
       </c>
       <c r="C5">
         <v>34.04163672</v>
@@ -4838,7 +4838,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>25.65475696</v>
+        <v>27.60567781</v>
       </c>
       <c r="C6">
         <v>30.235136539999999</v>
@@ -4861,7 +4861,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>52.467886480000004</v>
+        <v>46.618863879999999</v>
       </c>
       <c r="C7">
         <v>41.592700440000002</v>
@@ -4884,7 +4884,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>123.1677864</v>
+        <v>130.48041370000001</v>
       </c>
       <c r="C8">
         <v>60.059090450000006</v>
@@ -4907,7 +4907,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>166.23262990000001</v>
+        <v>430.55565730000001</v>
       </c>
       <c r="C9">
         <v>249.09494649999999</v>
@@ -4930,7 +4930,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>162.82172750000001</v>
+        <v>263.97305949999998</v>
       </c>
       <c r="C10">
         <v>576.80068549999999</v>
@@ -4953,7 +4953,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>66.551131959999992</v>
+        <v>104.41407799999999</v>
       </c>
       <c r="C11">
         <v>297.2250659</v>
@@ -4976,7 +4976,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>58.545583860000001</v>
+        <v>44.116213809999998</v>
       </c>
       <c r="C12">
         <v>144.12701709999999</v>
@@ -4999,7 +4999,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>25.914385379999999</v>
+        <v>28.913753150000002</v>
       </c>
       <c r="C13">
         <v>52.694858399999994</v>
@@ -5022,7 +5022,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>36.869770629999998</v>
+        <v>36.468615589999999</v>
       </c>
       <c r="C14">
         <v>43.019139889999998</v>
@@ -5045,7 +5045,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>26.493841980000003</v>
+        <v>31.649318220000001</v>
       </c>
       <c r="C15">
         <v>42.015881960000002</v>
@@ -5068,7 +5068,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>22.3585213</v>
+        <v>24.774592550000001</v>
       </c>
       <c r="C16">
         <v>45.296903440000001</v>
@@ -5091,7 +5091,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>23.030349919999999</v>
+        <v>26.424043180000002</v>
       </c>
       <c r="C17">
         <v>39.872492800000003</v>
@@ -5114,7 +5114,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>20.91384274</v>
+        <v>24.97409459</v>
       </c>
       <c r="C18">
         <v>30.78035083</v>
@@ -5137,7 +5137,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>31.03302747</v>
+        <v>33.48866641</v>
       </c>
       <c r="C19">
         <v>42.671297120000006</v>
@@ -5160,7 +5160,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>50.721259519999997</v>
+        <v>118.3529451</v>
       </c>
       <c r="C20">
         <v>106.621708</v>
@@ -5183,7 +5183,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>113.5885339</v>
+        <v>178.81164920000001</v>
       </c>
       <c r="C21">
         <v>769.72709569999995</v>
@@ -5206,7 +5206,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>210.88209959999998</v>
+        <v>241.5292144</v>
       </c>
       <c r="C22">
         <v>662.80359279999993</v>
@@ -5229,7 +5229,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>80.177667360000001</v>
+        <v>54.629330770000003</v>
       </c>
       <c r="C23">
         <v>325.4162202</v>
@@ -5252,7 +5252,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>48.30885327</v>
+        <v>61.238290169999999</v>
       </c>
       <c r="C24">
         <v>157.17131099999997</v>
@@ -5275,7 +5275,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>35.13480878</v>
+        <v>26.38278781</v>
       </c>
       <c r="C25">
         <v>76.50550195000001</v>
@@ -5298,7 +5298,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>50.739999759999996</v>
+        <v>33.934077459999997</v>
       </c>
       <c r="C26">
         <v>72.042445189999995</v>
@@ -5321,7 +5321,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>40.74616657</v>
+        <v>32.211940409999997</v>
       </c>
       <c r="C27">
         <v>48.517599370000006</v>
@@ -5344,7 +5344,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>29.260138309999999</v>
+        <v>34.45440498</v>
       </c>
       <c r="C28">
         <v>42.934383909999994</v>
@@ -5367,7 +5367,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>27.96941739</v>
+        <v>27.11160799</v>
       </c>
       <c r="C29">
         <v>48.678900759999998</v>
@@ -5390,7 +5390,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>25.635685850000002</v>
+        <v>24.184437000000003</v>
       </c>
       <c r="C30">
         <v>41.501980959999997</v>
@@ -5413,7 +5413,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>41.571222470000002</v>
+        <v>43.179649380000001</v>
       </c>
       <c r="C31">
         <v>63.788940189999998</v>
@@ -5436,7 +5436,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>86.141379270000002</v>
+        <v>92.028328760000008</v>
       </c>
       <c r="C32">
         <v>189.85580300000001</v>
@@ -5459,7 +5459,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>273.29278149999999</v>
+        <v>204.12465830000002</v>
       </c>
       <c r="C33">
         <v>462.03587599999997</v>
@@ -5482,7 +5482,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>307.63734909999999</v>
+        <v>515.63994189999994</v>
       </c>
       <c r="C34">
         <v>514.38671190000002</v>
@@ -5505,7 +5505,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>120.152479</v>
+        <v>254.64524789999999</v>
       </c>
       <c r="C35">
         <v>175.12004639999998</v>
@@ -5528,7 +5528,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>68.633078740000002</v>
+        <v>74.684812390000005</v>
       </c>
       <c r="C36">
         <v>77.042593139999994</v>
@@ -5551,7 +5551,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>48.996869079999996</v>
+        <v>39.16562175</v>
       </c>
       <c r="C37">
         <v>59.260924070000002</v>
@@ -5612,7 +5612,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>20.33756</v>
+        <v>45.426879999999997</v>
       </c>
       <c r="C2">
         <v>169.04750000000001</v>
@@ -5635,7 +5635,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>18.924009999999999</v>
+        <v>46.549759999999999</v>
       </c>
       <c r="C3">
         <v>85.647600000000011</v>
@@ -5658,7 +5658,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>22.01257</v>
+        <v>17.073979999999999</v>
       </c>
       <c r="C4">
         <v>59.939</v>
@@ -5681,7 +5681,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>25.471310000000003</v>
+        <v>39.499480000000005</v>
       </c>
       <c r="C5">
         <v>61.521560000000001</v>
@@ -5704,7 +5704,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>28.280740000000002</v>
+        <v>37.161389999999997</v>
       </c>
       <c r="C6">
         <v>52.56156</v>
@@ -5727,7 +5727,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>104.3515</v>
+        <v>62.122030000000002</v>
       </c>
       <c r="C7">
         <v>136.8801</v>
@@ -5750,7 +5750,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>95.365289999999987</v>
+        <v>127.0534</v>
       </c>
       <c r="C8">
         <v>232.77549999999999</v>
@@ -5773,7 +5773,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>122.5091</v>
+        <v>212.47489999999999</v>
       </c>
       <c r="C9">
         <v>452.05059999999997</v>
@@ -5796,7 +5796,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>239.87779999999998</v>
+        <v>573.20490000000007</v>
       </c>
       <c r="C10">
         <v>975.82140000000004</v>
@@ -5819,7 +5819,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>153.726</v>
+        <v>284.25190000000003</v>
       </c>
       <c r="C11">
         <v>512.54129999999998</v>
@@ -5842,7 +5842,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>68.679179999999988</v>
+        <v>74.385220000000004</v>
       </c>
       <c r="C12">
         <v>247.72749999999999</v>
@@ -5865,7 +5865,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>53.122419999999998</v>
+        <v>44.572859999999999</v>
       </c>
       <c r="C13">
         <v>164.14679999999998</v>
@@ -5888,7 +5888,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>36.973910000000004</v>
+        <v>44.871190000000006</v>
       </c>
       <c r="C14">
         <v>140.1962</v>
@@ -5911,7 +5911,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>47.918039999999998</v>
+        <v>46.882949999999994</v>
       </c>
       <c r="C15">
         <v>112.52189999999999</v>
@@ -5934,7 +5934,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>28.404400000000003</v>
+        <v>18.9894</v>
       </c>
       <c r="C16">
         <v>90.910570000000007</v>
@@ -5957,7 +5957,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>30.70806</v>
+        <v>26.94857</v>
       </c>
       <c r="C17">
         <v>84.902289999999994</v>
@@ -5980,7 +5980,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>35.77704</v>
+        <v>29.386700000000001</v>
       </c>
       <c r="C18">
         <v>75.771539999999987</v>
@@ -6003,7 +6003,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>76.180050000000008</v>
+        <v>69.15146</v>
       </c>
       <c r="C19">
         <v>140.35050000000001</v>
@@ -6026,7 +6026,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>106.428</v>
+        <v>95.985590000000002</v>
       </c>
       <c r="C20">
         <v>235.99610000000001</v>
@@ -6049,7 +6049,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>92.201530000000005</v>
+        <v>71.561639999999997</v>
       </c>
       <c r="C21">
         <v>543.29669999999999</v>
@@ -6072,7 +6072,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>261.35309999999998</v>
+        <v>386.57259999999997</v>
       </c>
       <c r="C22">
         <v>530.226</v>
@@ -6095,7 +6095,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>162.10599999999999</v>
+        <v>151.19479999999999</v>
       </c>
       <c r="C23">
         <v>370.27909999999997</v>
@@ -6118,7 +6118,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>59.494690000000006</v>
+        <v>54.007649999999998</v>
       </c>
       <c r="C24">
         <v>203.21079999999998</v>
@@ -6141,7 +6141,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>48.890449999999994</v>
+        <v>22.137709999999998</v>
       </c>
       <c r="C25">
         <v>118.09389999999999</v>
@@ -6164,7 +6164,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>35.780739999999994</v>
+        <v>31.957459999999998</v>
       </c>
       <c r="C26">
         <v>118.96599999999999</v>
@@ -6187,7 +6187,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>47.075410000000005</v>
+        <v>31.30781</v>
       </c>
       <c r="C27">
         <v>85.920659999999998</v>
@@ -6210,7 +6210,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>22.76275</v>
+        <v>45.255089999999996</v>
       </c>
       <c r="C28">
         <v>52.190190000000001</v>
@@ -6233,7 +6233,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>38.115029999999997</v>
+        <v>44.032660000000007</v>
       </c>
       <c r="C29">
         <v>61.143730000000005</v>
@@ -6256,7 +6256,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>39.982610000000001</v>
+        <v>36.055030000000002</v>
       </c>
       <c r="C30">
         <v>51.260640000000002</v>
@@ -6279,7 +6279,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>67.268679999999989</v>
+        <v>98.493710000000007</v>
       </c>
       <c r="C31">
         <v>109.876</v>
@@ -6302,7 +6302,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>95.591649999999987</v>
+        <v>159.095</v>
       </c>
       <c r="C32">
         <v>286.45740000000001</v>
@@ -6325,7 +6325,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>195.31210000000002</v>
+        <v>327.1386</v>
       </c>
       <c r="C33">
         <v>312.86859999999996</v>
@@ -6348,7 +6348,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>506.25880000000001</v>
+        <v>667.42869999999994</v>
       </c>
       <c r="C34">
         <v>209.73729999999998</v>
@@ -6371,7 +6371,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>142.50779999999997</v>
+        <v>771.37139999999999</v>
       </c>
       <c r="C35">
         <v>127.7692</v>
@@ -6394,7 +6394,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>97.705389999999994</v>
+        <v>143.54910000000001</v>
       </c>
       <c r="C36">
         <v>48.783610000000003</v>
@@ -6417,7 +6417,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>67.803789999999992</v>
+        <v>58.462559999999996</v>
       </c>
       <c r="C37">
         <v>35.540120000000002</v>
@@ -6478,7 +6478,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>22.420480000000001</v>
+        <v>43.196289999999998</v>
       </c>
       <c r="C2">
         <v>129.3175</v>
@@ -6501,7 +6501,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>27.626840000000001</v>
+        <v>41.21613</v>
       </c>
       <c r="C3">
         <v>61.481319999999997</v>
@@ -6524,7 +6524,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>21.969429999999999</v>
+        <v>29.511770000000002</v>
       </c>
       <c r="C4">
         <v>46.940440000000002</v>
@@ -6547,7 +6547,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>22.889669999999999</v>
+        <v>32.60669</v>
       </c>
       <c r="C5">
         <v>42.761890000000001</v>
@@ -6570,7 +6570,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>21.369439999999997</v>
+        <v>26.535679999999999</v>
       </c>
       <c r="C6">
         <v>35.075029999999998</v>
@@ -6593,7 +6593,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>49.170929999999998</v>
+        <v>45.706510000000002</v>
       </c>
       <c r="C7">
         <v>63.06006</v>
@@ -6616,7 +6616,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>67.760249999999999</v>
+        <v>91.136210000000005</v>
       </c>
       <c r="C8">
         <v>115.89439999999999</v>
@@ -6639,7 +6639,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>95.74973</v>
+        <v>151.50279999999998</v>
       </c>
       <c r="C9">
         <v>236.249</v>
@@ -6662,7 +6662,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>214.14400000000001</v>
+        <v>477.39269999999999</v>
       </c>
       <c r="C10">
         <v>522.69079999999997</v>
@@ -6685,7 +6685,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>140.72620000000001</v>
+        <v>246.6935</v>
       </c>
       <c r="C11">
         <v>359.62729999999999</v>
@@ -6708,7 +6708,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>65.066850000000002</v>
+        <v>72.345020000000005</v>
       </c>
       <c r="C12">
         <v>160.2843</v>
@@ -6731,7 +6731,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>40.527670000000001</v>
+        <v>37.191839999999999</v>
       </c>
       <c r="C13">
         <v>103.8493</v>
@@ -6754,7 +6754,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>35.61412</v>
+        <v>47.728470000000002</v>
       </c>
       <c r="C14">
         <v>100.85239999999999</v>
@@ -6777,7 +6777,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>37.797260000000001</v>
+        <v>41.818959999999997</v>
       </c>
       <c r="C15">
         <v>70.01764</v>
@@ -6800,7 +6800,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>29.38804</v>
+        <v>30.914249999999999</v>
       </c>
       <c r="C16">
         <v>53.479800000000004</v>
@@ -6823,7 +6823,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>26.242159999999998</v>
+        <v>27.799490000000002</v>
       </c>
       <c r="C17">
         <v>49.335059999999999</v>
@@ -6846,7 +6846,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>24.344339999999999</v>
+        <v>23.234830000000002</v>
       </c>
       <c r="C18">
         <v>39.879429999999999</v>
@@ -6869,7 +6869,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>46.252989999999997</v>
+        <v>43.419849999999997</v>
       </c>
       <c r="C19">
         <v>50.260649999999998</v>
@@ -6892,7 +6892,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>82.989750000000001</v>
+        <v>63.075519999999997</v>
       </c>
       <c r="C20">
         <v>109.2385</v>
@@ -6915,7 +6915,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>69.752279999999999</v>
+        <v>39.881889999999999</v>
       </c>
       <c r="C21">
         <v>243.55610000000001</v>
@@ -6938,7 +6938,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>222.3032</v>
+        <v>250.80410000000001</v>
       </c>
       <c r="C22">
         <v>366.88909999999998</v>
@@ -6961,7 +6961,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>149.42760000000001</v>
+        <v>133.88159999999999</v>
       </c>
       <c r="C23">
         <v>290.44009999999997</v>
@@ -6984,7 +6984,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>61.891800000000003</v>
+        <v>49.610480000000003</v>
       </c>
       <c r="C24">
         <v>138.85929999999999</v>
@@ -7007,7 +7007,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>43.094379999999994</v>
+        <v>29.31719</v>
       </c>
       <c r="C25">
         <v>82.289500000000004</v>
@@ -7030,7 +7030,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>40.161819999999999</v>
+        <v>31.468630000000001</v>
       </c>
       <c r="C26">
         <v>92.795410000000004</v>
@@ -7053,7 +7053,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>42.30594</v>
+        <v>33.573569999999997</v>
       </c>
       <c r="C27">
         <v>63.582650000000001</v>
@@ -7076,7 +7076,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>28.482970000000002</v>
+        <v>37.065049999999999</v>
       </c>
       <c r="C28">
         <v>36.659469999999999</v>
@@ -7099,7 +7099,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>25.85201</v>
+        <v>29.10821</v>
       </c>
       <c r="C29">
         <v>39.5837</v>
@@ -7122,7 +7122,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>22.516759999999998</v>
+        <v>25.76014</v>
       </c>
       <c r="C30">
         <v>32.730879999999999</v>
@@ -7145,7 +7145,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>41.581009999999999</v>
+        <v>36.124809999999997</v>
       </c>
       <c r="C31">
         <v>47.732399999999998</v>
@@ -7168,7 +7168,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>69.753950000000003</v>
+        <v>92.39743</v>
       </c>
       <c r="C32">
         <v>160.1337</v>
@@ -7191,7 +7191,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>146.82640000000001</v>
+        <v>161.30760000000001</v>
       </c>
       <c r="C33">
         <v>231.12309999999999</v>
@@ -7214,7 +7214,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>357.33640000000003</v>
+        <v>428.9461</v>
       </c>
       <c r="C34">
         <v>174.53149999999999</v>
@@ -7237,7 +7237,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>120.5804</v>
+        <v>538.71050000000002</v>
       </c>
       <c r="C35">
         <v>110.0626</v>
@@ -7260,7 +7260,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>70.49624</v>
+        <v>117.8977</v>
       </c>
       <c r="C36">
         <v>57.69323</v>
@@ -7283,7 +7283,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>56.838370000000005</v>
+        <v>49.002549999999999</v>
       </c>
       <c r="C37">
         <v>45.54701</v>
@@ -7344,7 +7344,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>29.911240000000003</v>
+        <v>33.264849999999996</v>
       </c>
       <c r="C2">
         <v>57.626129999999996</v>
@@ -7367,7 +7367,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>28.338819999999998</v>
+        <v>28.98507</v>
       </c>
       <c r="C3">
         <v>38.787129999999998</v>
@@ -7390,7 +7390,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>22.189720000000001</v>
+        <v>29.286009999999997</v>
       </c>
       <c r="C4">
         <v>29.786150000000003</v>
@@ -7413,7 +7413,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>24.796060000000001</v>
+        <v>27.627790000000001</v>
       </c>
       <c r="C5">
         <v>29.228069999999999</v>
@@ -7436,7 +7436,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>23.329759999999997</v>
+        <v>24.27638</v>
       </c>
       <c r="C6">
         <v>26.373840000000001</v>
@@ -7459,7 +7459,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>46.358839999999994</v>
+        <v>41.54515</v>
       </c>
       <c r="C7">
         <v>35.352690000000003</v>
@@ -7482,7 +7482,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>109.8446</v>
+        <v>118.7813</v>
       </c>
       <c r="C8">
         <v>50.902250000000002</v>
@@ -7505,7 +7505,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>151.24420000000001</v>
+        <v>377.27440000000001</v>
       </c>
       <c r="C9">
         <v>203.64060000000001</v>
@@ -7528,7 +7528,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>152.22749999999999</v>
+        <v>241.3511</v>
       </c>
       <c r="C10">
         <v>493.82140000000004</v>
@@ -7551,7 +7551,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>61.956510000000002</v>
+        <v>97.09550999999999</v>
       </c>
       <c r="C11">
         <v>256.48759999999999</v>
@@ -7574,7 +7574,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>52.784059999999997</v>
+        <v>41.866639999999997</v>
       </c>
       <c r="C12">
         <v>123.27500000000001</v>
@@ -7597,7 +7597,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>20.620480000000001</v>
+        <v>26.781580000000002</v>
       </c>
       <c r="C13">
         <v>44.78322</v>
@@ -7620,7 +7620,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>28.987490000000001</v>
+        <v>33.801919999999996</v>
       </c>
       <c r="C14">
         <v>37.060900000000004</v>
@@ -7643,7 +7643,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>22.594930000000002</v>
+        <v>28.991619999999998</v>
       </c>
       <c r="C15">
         <v>34.854889999999997</v>
@@ -7666,7 +7666,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>18.803830000000001</v>
+        <v>21.518470000000001</v>
       </c>
       <c r="C16">
         <v>38.088900000000002</v>
@@ -7689,7 +7689,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>19.816419999999997</v>
+        <v>23.789740000000002</v>
       </c>
       <c r="C17">
         <v>32.390709999999999</v>
@@ -7712,7 +7712,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>17.826409999999999</v>
+        <v>22.046250000000001</v>
       </c>
       <c r="C18">
         <v>25.403419999999997</v>
@@ -7735,7 +7735,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>27.187889999999999</v>
+        <v>29.29373</v>
       </c>
       <c r="C19">
         <v>31.203799999999998</v>
@@ -7758,7 +7758,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>44.451610000000002</v>
+        <v>107.2529</v>
       </c>
       <c r="C20">
         <v>89.73163000000001</v>
@@ -7781,7 +7781,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>102.6858</v>
+        <v>159.26560000000001</v>
       </c>
       <c r="C21">
         <v>657.4303000000001</v>
@@ -7804,7 +7804,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>192.3827</v>
+        <v>216.346</v>
       </c>
       <c r="C22">
         <v>578.86369999999999</v>
@@ -7827,7 +7827,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>71.992339999999999</v>
+        <v>50.647750000000002</v>
       </c>
       <c r="C23">
         <v>281.83409999999998</v>
@@ -7850,7 +7850,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>41.72531</v>
+        <v>56.374650000000003</v>
       </c>
       <c r="C24">
         <v>138.90049999999999</v>
@@ -7873,7 +7873,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>28.400500000000001</v>
+        <v>23.42596</v>
       </c>
       <c r="C25">
         <v>68.058460000000011</v>
@@ -7896,7 +7896,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>43.372599999999998</v>
+        <v>30.310549999999999</v>
       </c>
       <c r="C26">
         <v>62.2288</v>
@@ -7919,7 +7919,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>37.838980000000006</v>
+        <v>28.612020000000001</v>
       </c>
       <c r="C27">
         <v>43.886830000000003</v>
@@ -7942,7 +7942,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>25.574840000000002</v>
+        <v>30.418849999999999</v>
       </c>
       <c r="C28">
         <v>37.042010000000005</v>
@@ -7965,7 +7965,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>23.57958</v>
+        <v>23.34075</v>
       </c>
       <c r="C29">
         <v>35.209669999999996</v>
@@ -7988,7 +7988,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>22.229140000000001</v>
+        <v>21.129650000000002</v>
       </c>
       <c r="C30">
         <v>31.159880000000001</v>
@@ -8011,7 +8011,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>36.467760000000006</v>
+        <v>38.304580000000001</v>
       </c>
       <c r="C31">
         <v>49.345660000000002</v>
@@ -8034,7 +8034,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>78.578009999999992</v>
+        <v>84.047240000000002</v>
       </c>
       <c r="C32">
         <v>162.48479999999998</v>
@@ -8057,7 +8057,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>231.60050000000001</v>
+        <v>190.79910000000001</v>
       </c>
       <c r="C33">
         <v>400.29859999999996</v>
@@ -8080,7 +8080,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>261.68209999999999</v>
+        <v>454.5951</v>
       </c>
       <c r="C34">
         <v>445.2208</v>
@@ -8103,7 +8103,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>103.7231</v>
+        <v>231.29</v>
       </c>
       <c r="C35">
         <v>157.01139999999998</v>
@@ -8126,7 +8126,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>55.27234</v>
+        <v>67.72869</v>
       </c>
       <c r="C36">
         <v>68.470179999999999</v>
@@ -8149,7 +8149,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>35.529389999999999</v>
+        <v>35.521650000000001</v>
       </c>
       <c r="C37">
         <v>51.228819999999999</v>
@@ -8210,7 +8210,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>17.748669999999997</v>
+        <v>28.075530000000001</v>
       </c>
       <c r="C2">
         <v>75.344719999999995</v>
@@ -8233,7 +8233,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>17.533480000000001</v>
+        <v>20.556630000000002</v>
       </c>
       <c r="C3">
         <v>46.063499999999998</v>
@@ -8256,7 +8256,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>15.71598</v>
+        <v>19.40325</v>
       </c>
       <c r="C4">
         <v>43.659769999999995</v>
@@ -8279,7 +8279,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>17.264040000000001</v>
+        <v>22.964470000000002</v>
       </c>
       <c r="C5">
         <v>1.0055529999999999</v>
@@ -8302,7 +8302,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>27.449660000000002</v>
+        <v>27.26962</v>
       </c>
       <c r="C6">
         <v>43.26229</v>
@@ -8325,7 +8325,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>137.28829999999999</v>
+        <v>75.354600000000005</v>
       </c>
       <c r="C7">
         <v>110.98339999999999</v>
@@ -8348,7 +8348,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>191.40810000000002</v>
+        <v>124.8117</v>
       </c>
       <c r="C8">
         <v>179.8477</v>
@@ -8371,7 +8371,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>169.8776</v>
+        <v>361.28050000000002</v>
       </c>
       <c r="C9">
         <v>314.64299999999997</v>
@@ -8394,7 +8394,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>93.102050000000006</v>
+        <v>145.63570000000001</v>
       </c>
       <c r="C10">
         <v>414.76890000000003</v>
@@ -8417,7 +8417,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>15.737129999999999</v>
+        <v>25.331319999999998</v>
       </c>
       <c r="C11">
         <v>168.04429999999999</v>
@@ -8440,7 +8440,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>21.246419999999997</v>
+        <v>-10.793700000000001</v>
       </c>
       <c r="C12">
         <v>60.047730000000001</v>
@@ -8463,7 +8463,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>9.9849359999999994</v>
+        <v>4.9372189999999998</v>
       </c>
       <c r="C13">
         <v>13.002139999999999</v>
@@ -8486,7 +8486,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>29.356729999999999</v>
+        <v>15.604950000000001</v>
       </c>
       <c r="C14">
         <v>64.497839999999997</v>
@@ -8509,7 +8509,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>9.9630299999999998</v>
+        <v>14.753200000000001</v>
       </c>
       <c r="C15">
         <v>25.684750000000001</v>
@@ -8532,7 +8532,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>6.9595209999999996</v>
+        <v>12.055770000000001</v>
       </c>
       <c r="C16">
         <v>30.688310000000001</v>
@@ -8555,7 +8555,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>8.9373619999999985</v>
+        <v>14.267760000000001</v>
       </c>
       <c r="C17">
         <v>29.408150000000003</v>
@@ -8578,7 +8578,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>10.98348</v>
+        <v>16.630950000000002</v>
       </c>
       <c r="C18">
         <v>35.651129999999995</v>
@@ -8601,7 +8601,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>28.956169999999997</v>
+        <v>63.868199999999995</v>
       </c>
       <c r="C19">
         <v>101.2761</v>
@@ -8624,7 +8624,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>90.381559999999993</v>
+        <v>221.53299999999999</v>
       </c>
       <c r="C20">
         <v>154.72929999999999</v>
@@ -8647,7 +8647,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>198.63129999999998</v>
+        <v>263.22909999999996</v>
       </c>
       <c r="C21">
         <v>426.0181</v>
@@ -8670,7 +8670,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>196.8229</v>
+        <v>152.1164</v>
       </c>
       <c r="C22">
         <v>228.25910000000002</v>
@@ -8693,7 +8693,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>66.634539999999987</v>
+        <v>15.59897</v>
       </c>
       <c r="C23">
         <v>56.936970000000002</v>
@@ -8716,7 +8716,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>35.160690000000002</v>
+        <v>39.041589999999999</v>
       </c>
       <c r="C24">
         <v>63.035440000000001</v>
@@ -8739,7 +8739,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>40.31814</v>
+        <v>24.48169</v>
       </c>
       <c r="C25">
         <v>43.810389999999998</v>
@@ -8762,7 +8762,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>64.725560000000002</v>
+        <v>24.75994</v>
       </c>
       <c r="C26">
         <v>87.143320000000003</v>
@@ -8785,7 +8785,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>42.68385</v>
+        <v>17.483830000000001</v>
       </c>
       <c r="C27">
         <v>49.978550000000006</v>
@@ -8808,7 +8808,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>24.70768</v>
+        <v>23.759499999999999</v>
       </c>
       <c r="C28">
         <v>51.539760000000001</v>
@@ -8831,7 +8831,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>23.775389999999998</v>
+        <v>16.03877</v>
       </c>
       <c r="C29">
         <v>33.395650000000003</v>
@@ -8854,7 +8854,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>29.48254</v>
+        <v>17.47579</v>
       </c>
       <c r="C30">
         <v>39.099059999999994</v>
@@ -8877,7 +8877,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>63.039199999999994</v>
+        <v>40.785249999999998</v>
       </c>
       <c r="C31">
         <v>189.46770000000001</v>
@@ -8900,7 +8900,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>198.83429999999998</v>
+        <v>114.4302</v>
       </c>
       <c r="C32">
         <v>391.90949999999998</v>
@@ -8923,7 +8923,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>259.34410000000003</v>
+        <v>171.7585</v>
       </c>
       <c r="C33">
         <v>462.69309999999996</v>
@@ -8946,7 +8946,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>187.26570000000001</v>
+        <v>252.03120000000001</v>
       </c>
       <c r="C34">
         <v>443.85129999999998</v>
@@ -8969,7 +8969,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>34.649099999999997</v>
+        <v>38.171289999999999</v>
       </c>
       <c r="C35">
         <v>117.72839999999999</v>
@@ -8992,7 +8992,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>38.17568</v>
+        <v>2.2648580000000003</v>
       </c>
       <c r="C36">
         <v>42.762740000000001</v>
@@ -9015,7 +9015,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>83.770649999999989</v>
+        <v>15.18966</v>
       </c>
       <c r="C37">
         <v>83.437619999999995</v>
@@ -9076,7 +9076,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>48.204999999999998</v>
+        <v>77.578000000000003</v>
       </c>
       <c r="C2">
         <v>85.269000000000005</v>
@@ -9099,7 +9099,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>34.927</v>
+        <v>47.341000000000001</v>
       </c>
       <c r="C3">
         <v>51.2</v>
@@ -9122,7 +9122,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>29.489000000000001</v>
+        <v>37.715000000000003</v>
       </c>
       <c r="C4">
         <v>49.487000000000002</v>
@@ -9145,7 +9145,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>33.975999999999999</v>
+        <v>36.314</v>
       </c>
       <c r="C5">
         <v>34.761000000000003</v>
@@ -9168,7 +9168,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>37.262999999999998</v>
+        <v>33.308</v>
       </c>
       <c r="C6">
         <v>35.189</v>
@@ -9191,7 +9191,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>61.067</v>
+        <v>51.215000000000003</v>
       </c>
       <c r="C7">
         <v>51.15</v>
@@ -9214,7 +9214,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>134.399</v>
+        <v>146.233</v>
       </c>
       <c r="C8">
         <v>104.712</v>
@@ -9237,7 +9237,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>111.255</v>
+        <v>338.74799999999999</v>
       </c>
       <c r="C9">
         <v>428.37900000000002</v>
@@ -9260,7 +9260,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>67.995000000000005</v>
+        <v>164.279</v>
       </c>
       <c r="C10">
         <v>573.36599999999999</v>
@@ -9283,7 +9283,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>23.109000000000002</v>
+        <v>58.875999999999998</v>
       </c>
       <c r="C11">
         <v>250.25200000000001</v>
@@ -9306,7 +9306,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>28.164000000000001</v>
+        <v>24.931999999999999</v>
       </c>
       <c r="C12">
         <v>86.494</v>
@@ -9329,7 +9329,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>41.506</v>
+        <v>59.713999999999999</v>
       </c>
       <c r="C13">
         <v>49.707000000000001</v>
@@ -9352,7 +9352,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>57.545000000000002</v>
+        <v>82.858999999999995</v>
       </c>
       <c r="C14">
         <v>74.402000000000001</v>
@@ -9375,7 +9375,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>39.061999999999998</v>
+        <v>54.338999999999999</v>
       </c>
       <c r="C15">
         <v>51.75</v>
@@ -9398,7 +9398,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>37.182000000000002</v>
+        <v>35.972000000000001</v>
       </c>
       <c r="C16">
         <v>55.29</v>
@@ -9421,7 +9421,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>28.965</v>
+        <v>32.731999999999999</v>
       </c>
       <c r="C17">
         <v>37.475999999999999</v>
@@ -9444,7 +9444,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>20.663</v>
+        <v>28.943000000000001</v>
       </c>
       <c r="C18">
         <v>39.938000000000002</v>
@@ -9467,7 +9467,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>29.103999999999999</v>
+        <v>39.411000000000001</v>
       </c>
       <c r="C19">
         <v>42.962000000000003</v>
@@ -9490,7 +9490,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>52.813000000000002</v>
+        <v>151.24600000000001</v>
       </c>
       <c r="C20">
         <v>124.867</v>
@@ -9513,7 +9513,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>87.227000000000004</v>
+        <v>207.923</v>
       </c>
       <c r="C21">
         <v>600.93600000000004</v>
@@ -9536,7 +9536,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>71.593999999999994</v>
+        <v>151.77000000000001</v>
       </c>
       <c r="C22">
         <v>437.95299999999997</v>
@@ -9559,7 +9559,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>25.241</v>
+        <v>35.487000000000002</v>
       </c>
       <c r="C23">
         <v>132.39500000000001</v>
@@ -9582,7 +9582,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>14.561999999999999</v>
+        <v>72.317999999999998</v>
       </c>
       <c r="C24">
         <v>77.998000000000005</v>
@@ -9605,7 +9605,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>50.073999999999998</v>
+        <v>52.844999999999999</v>
       </c>
       <c r="C25">
         <v>84.79</v>
@@ -9628,7 +9628,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>70.822000000000003</v>
+        <v>87.669289239999998</v>
       </c>
       <c r="C26">
         <v>103.297</v>
@@ -9651,7 +9651,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>38.637999999999998</v>
+        <v>60.285955039999997</v>
       </c>
       <c r="C27">
         <v>64.864000000000004</v>
@@ -9674,7 +9674,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>28.521999999999998</v>
+        <v>54.816706949999997</v>
       </c>
       <c r="C28">
         <v>58.972999999999999</v>
@@ -9697,7 +9697,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>23.189</v>
+        <v>39.502647119999999</v>
       </c>
       <c r="C29">
         <v>30.925000000000001</v>
@@ -9720,7 +9720,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>24.265999999999998</v>
+        <v>33.989246290000004</v>
       </c>
       <c r="C30">
         <v>31.488</v>
@@ -9743,7 +9743,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>31.861999999999998</v>
+        <v>47.730860100000001</v>
       </c>
       <c r="C31">
         <v>62.232999999999997</v>
@@ -9766,7 +9766,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>54.905000000000001</v>
+        <v>132.23944874</v>
       </c>
       <c r="C32">
         <v>291.58699999999999</v>
@@ -9789,7 +9789,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>190.47900000000001</v>
+        <v>296.94932231000001</v>
       </c>
       <c r="C33">
         <v>494.05599999999998</v>
@@ -9812,7 +9812,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>142.92699999999999</v>
+        <v>389.00474378999996</v>
       </c>
       <c r="C34">
         <v>228.32499999999999</v>
@@ -9835,7 +9835,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>43.594000000000001</v>
+        <v>148.29828099999997</v>
       </c>
       <c r="C35">
         <v>81.888000000000005</v>
@@ -9858,7 +9858,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>23.756</v>
+        <v>17.929669440000001</v>
       </c>
       <c r="C36">
         <v>27.384</v>
@@ -9881,7 +9881,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>45.13</v>
+        <v>52.12231405</v>
       </c>
       <c r="C37">
         <v>70.25</v>
@@ -9942,7 +9942,7 @@
         <v>43739</v>
       </c>
       <c r="B2">
-        <v>260.28469000000001</v>
+        <v>307.43097999999998</v>
       </c>
       <c r="C2">
         <v>846.84659999999997</v>
@@ -9965,7 +9965,7 @@
         <v>43770</v>
       </c>
       <c r="B3">
-        <v>272.4674</v>
+        <v>379.22376000000003</v>
       </c>
       <c r="C3">
         <v>667.49953000000005</v>
@@ -9988,7 +9988,7 @@
         <v>43800</v>
       </c>
       <c r="B4">
-        <v>246.49001000000001</v>
+        <v>296.30034999999998</v>
       </c>
       <c r="C4">
         <v>543.58793000000003</v>
@@ -10011,7 +10011,7 @@
         <v>43831</v>
       </c>
       <c r="B5">
-        <v>205.31920000000002</v>
+        <v>329.35734000000002</v>
       </c>
       <c r="C5">
         <v>449.51796999999999</v>
@@ -10034,7 +10034,7 @@
         <v>43862</v>
       </c>
       <c r="B6">
-        <v>330.68854999999996</v>
+        <v>323.24390999999997</v>
       </c>
       <c r="C6">
         <v>469.14665000000002</v>
@@ -10057,7 +10057,7 @@
         <v>43891</v>
       </c>
       <c r="B7">
-        <v>747.62995999999998</v>
+        <v>489.53684000000004</v>
       </c>
       <c r="C7">
         <v>1001.97183</v>
@@ -10080,7 +10080,7 @@
         <v>43922</v>
       </c>
       <c r="B8">
-        <v>965.29324999999994</v>
+        <v>838.50626</v>
       </c>
       <c r="C8">
         <v>1130.7236</v>
@@ -10103,7 +10103,7 @@
         <v>43952</v>
       </c>
       <c r="B9">
-        <v>1068.1749499999999</v>
+        <v>3133.12817</v>
       </c>
       <c r="C9">
         <v>3205.0938500000002</v>
@@ -10126,7 +10126,7 @@
         <v>43983</v>
       </c>
       <c r="B10">
-        <v>1043.7099699999999</v>
+        <v>2616.1731099999997</v>
       </c>
       <c r="C10">
         <v>6659.4755599999999</v>
@@ -10149,7 +10149,7 @@
         <v>44013</v>
       </c>
       <c r="B11">
-        <v>335.76249999999999</v>
+        <v>1127.9570900000001</v>
       </c>
       <c r="C11">
         <v>3547.5024199999998</v>
@@ -10172,7 +10172,7 @@
         <v>44044</v>
       </c>
       <c r="B12">
-        <v>339.38526999999999</v>
+        <v>192.81735999999998</v>
       </c>
       <c r="C12">
         <v>1287.8981999999999</v>
@@ -10195,7 +10195,7 @@
         <v>44075</v>
       </c>
       <c r="B13">
-        <v>124.22367999999999</v>
+        <v>185.90317999999999</v>
       </c>
       <c r="C13">
         <v>561.35106999999994</v>
@@ -10218,7 +10218,7 @@
         <v>44105</v>
       </c>
       <c r="B14">
-        <v>237.74179999999998</v>
+        <v>265.29784999999998</v>
       </c>
       <c r="C14">
         <v>716.36901</v>
@@ -10241,7 +10241,7 @@
         <v>44136</v>
       </c>
       <c r="B15">
-        <v>288.48759999999999</v>
+        <v>360.40429999999998</v>
       </c>
       <c r="C15">
         <v>595.52926000000002</v>
@@ -10264,7 +10264,7 @@
         <v>44166</v>
       </c>
       <c r="B16">
-        <v>247.55924999999999</v>
+        <v>217.14876000000001</v>
       </c>
       <c r="C16">
         <v>541.21950000000004</v>
@@ -10287,7 +10287,7 @@
         <v>44197</v>
       </c>
       <c r="B17">
-        <v>271.04752000000002</v>
+        <v>309.57371000000001</v>
       </c>
       <c r="C17">
         <v>397.41045000000003</v>
@@ -10310,7 +10310,7 @@
         <v>44228</v>
       </c>
       <c r="B18">
-        <v>204.91283999999999</v>
+        <v>322.50587000000002</v>
       </c>
       <c r="C18">
         <v>479.55982</v>
@@ -10333,7 +10333,7 @@
         <v>44256</v>
       </c>
       <c r="B19">
-        <v>377.20555000000002</v>
+        <v>535.82156999999995</v>
       </c>
       <c r="C19">
         <v>760.60487999999998</v>
@@ -10356,7 +10356,7 @@
         <v>44287</v>
       </c>
       <c r="B20">
-        <v>455.58172999999999</v>
+        <v>979.85526000000004</v>
       </c>
       <c r="C20">
         <v>1522.8559</v>
@@ -10379,7 +10379,7 @@
         <v>44317</v>
       </c>
       <c r="B21">
-        <v>708.49370999999996</v>
+        <v>1444.31674</v>
       </c>
       <c r="C21">
         <v>5429.2664100000002</v>
@@ -10402,7 +10402,7 @@
         <v>44348</v>
       </c>
       <c r="B22">
-        <v>1438.6799099999998</v>
+        <v>2684.68804</v>
       </c>
       <c r="C22">
         <v>5687.9918899999993</v>
@@ -10425,7 +10425,7 @@
         <v>44378</v>
       </c>
       <c r="B23">
-        <v>581.30113000000006</v>
+        <v>546.06851000000006</v>
       </c>
       <c r="C23">
         <v>2676.0059900000001</v>
@@ -10448,7 +10448,7 @@
         <v>44409</v>
       </c>
       <c r="B24">
-        <v>197.25624999999999</v>
+        <v>516.63591999999994</v>
       </c>
       <c r="C24">
         <v>1376.8901899999998</v>
@@ -10471,7 +10471,7 @@
         <v>44440</v>
       </c>
       <c r="B25">
-        <v>302.60960999999998</v>
+        <v>243.77939999999998</v>
       </c>
       <c r="C25">
         <v>661.97355000000005</v>
@@ -10494,7 +10494,7 @@
         <v>44470</v>
       </c>
       <c r="B26">
-        <v>454.74218999999999</v>
+        <v>437.51084000000003</v>
       </c>
       <c r="C26">
         <v>881.92110000000002</v>
@@ -10517,7 +10517,7 @@
         <v>44501</v>
       </c>
       <c r="B27">
-        <v>386.21096</v>
+        <v>351.53346000000005</v>
       </c>
       <c r="C27">
         <v>691.69087000000002</v>
@@ -10540,7 +10540,7 @@
         <v>44531</v>
       </c>
       <c r="B28">
-        <v>276.30721999999997</v>
+        <v>394.57535999999999</v>
       </c>
       <c r="C28">
         <v>540.37846000000002</v>
@@ -10563,7 +10563,7 @@
         <v>44562</v>
       </c>
       <c r="B29">
-        <v>504.20076</v>
+        <v>259.45889</v>
       </c>
       <c r="C29">
         <v>539.64705000000004</v>
@@ -10586,7 +10586,7 @@
         <v>44593</v>
       </c>
       <c r="B30">
-        <v>493.39231000000001</v>
+        <v>280.42408</v>
       </c>
       <c r="C30">
         <v>455.70453000000003</v>
@@ -10609,7 +10609,7 @@
         <v>44621</v>
       </c>
       <c r="B31">
-        <v>500.71429999999998</v>
+        <v>581.48798999999997</v>
       </c>
       <c r="C31">
         <v>1141.30573</v>
@@ -10632,7 +10632,7 @@
         <v>44652</v>
       </c>
       <c r="B32">
-        <v>749.45023000000003</v>
+        <v>1135.77216</v>
       </c>
       <c r="C32">
         <v>2707.6015400000001</v>
@@ -10655,7 +10655,7 @@
         <v>44682</v>
       </c>
       <c r="B33">
-        <v>1550.6840199999999</v>
+        <v>2440.3492700000002</v>
       </c>
       <c r="C33">
         <v>4366.7583399999994</v>
@@ -10678,7 +10678,7 @@
         <v>44713</v>
       </c>
       <c r="B34">
-        <v>2358.6873900000001</v>
+        <v>5202.63087</v>
       </c>
       <c r="C34">
         <v>3799.56016</v>
@@ -10701,7 +10701,7 @@
         <v>44743</v>
       </c>
       <c r="B35">
-        <v>629.63194999999996</v>
+        <v>3767.0521899999999</v>
       </c>
       <c r="C35">
         <v>1331.4722199999999</v>
@@ -10724,7 +10724,7 @@
         <v>44774</v>
       </c>
       <c r="B36">
-        <v>398.57389000000001</v>
+        <v>664.22307999999998</v>
       </c>
       <c r="C36">
         <v>553.74089000000004</v>
@@ -10747,7 +10747,7 @@
         <v>44805</v>
       </c>
       <c r="B37">
-        <v>498.08321999999998</v>
+        <v>456.39709999999997</v>
       </c>
       <c r="C37">
         <v>506.79510999999997</v>

</xml_diff>